<commit_message>
Reconfigured some of the tables and added initial data
</commit_message>
<xml_diff>
--- a/Table Creator.xlsx
+++ b/Table Creator.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\Visual Studio 2015\Projects\DungeonsAndDragons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew\Dropbox\Programming Projects\C#\DungeonsAndDragons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Worker" sheetId="8" r:id="rId1"/>
     <sheet name="Enum Tables" sheetId="12" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="116">
   <si>
     <t>Fields</t>
   </si>
@@ -141,12 +141,6 @@
     <t>PK</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>varchar(255)</t>
-  </si>
-  <si>
     <t>AS</t>
   </si>
   <si>
@@ -306,12 +300,6 @@
     <t>FROM</t>
   </si>
   <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>InvoiceSettings</t>
-  </si>
-  <si>
     <t>Create SP</t>
   </si>
   <si>
@@ -357,91 +345,40 @@
     <t>CommunicationType</t>
   </si>
   <si>
-    <t>PlayerCharacters</t>
-  </si>
-  <si>
     <t>dbo</t>
   </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>SkillSetId</t>
-  </si>
-  <si>
-    <t>SenseSetId</t>
-  </si>
-  <si>
-    <t>DefenseSetId</t>
-  </si>
-  <si>
-    <t>InitiativeId</t>
-  </si>
-  <si>
-    <t>AbilitySetId</t>
-  </si>
-  <si>
-    <t>MovementSetId</t>
-  </si>
-  <si>
-    <t>BaseActionPoints</t>
-  </si>
-  <si>
-    <t>AdditionalActionPoints</t>
-  </si>
-  <si>
-    <t>AdditionalHitPoints</t>
-  </si>
-  <si>
-    <t>BaseHitPoints</t>
-  </si>
-  <si>
-    <t>RaceId</t>
-  </si>
-  <si>
     <t>varchar(50)</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>ClassId</t>
-  </si>
-  <si>
-    <t>ParagonPathId</t>
-  </si>
-  <si>
-    <t>EpicDestinyId</t>
-  </si>
-  <si>
-    <t>ExperiencePoints</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>SizeId</t>
-  </si>
-  <si>
-    <t>GenderId</t>
-  </si>
-  <si>
-    <t>AlignmentId</t>
-  </si>
-  <si>
     <t>DeityId</t>
+  </si>
+  <si>
+    <t>CompassionLevels</t>
+  </si>
+  <si>
+    <t>Deities</t>
+  </si>
+  <si>
+    <t>AuthorityLevelId</t>
+  </si>
+  <si>
+    <t>CompassionLevelId</t>
+  </si>
+  <si>
+    <t>FlavourText</t>
+  </si>
+  <si>
+    <t>varchar(MAX)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -689,23 +626,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -741,23 +661,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -913,7 +816,7 @@
   <dimension ref="A1:AR102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,33 +861,33 @@
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L1" s="21"/>
       <c r="M1" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N1" s="20"/>
       <c r="O1" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P1" s="17"/>
       <c r="Q1" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R1" s="10"/>
       <c r="S1" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T1" s="11"/>
       <c r="U1" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Y1" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AA1" s="7"/>
       <c r="AB1" s="7"/>
@@ -1010,47 +913,50 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="J2" s="3" t="str">
         <f>A2&amp;" ["&amp;B2&amp;"].["&amp;C2&amp;"]"</f>
-        <v>CREATE TABLE [dbo].[PlayerCharacters]</v>
+        <v>CREATE TABLE [dbo].[Deities]</v>
       </c>
       <c r="L2" s="22" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Create]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_PlayerCharacters_Create]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_Deities_Create]</v>
       </c>
       <c r="N2" s="23" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Update]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_PlayerCharacters_Update]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_Deities_Update]</v>
       </c>
       <c r="P2" s="18" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Get]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_PlayerCharacters_Get]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_Deities_Get]</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V2" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Z2" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1075,27 +981,27 @@
       </c>
       <c r="L3" s="22" t="str">
         <f>IF(NOT(ISBLANK(B4)),"@"&amp;B4&amp;" "&amp;UPPER(C4)&amp;" = NULL OUTPUT,","")</f>
-        <v>@PlayerCharacterId INT = NULL OUTPUT,</v>
+        <v>@DeityId INT = NULL OUTPUT,</v>
       </c>
       <c r="N3" s="23" t="str">
         <f>IF(NOT(ISBLANK(B4)),"@"&amp;B4&amp;" "&amp;UPPER(C4)&amp;",","")</f>
-        <v>@PlayerCharacterId INT,</v>
+        <v>@DeityId INT,</v>
       </c>
       <c r="P3" s="18" t="str">
         <f>"@"&amp;C2&amp;"Id"&amp;" INT"</f>
-        <v>@PlayerCharactersId INT</v>
+        <v>@DeitiesId INT</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V3" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Z3" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
@@ -1103,8 +1009,8 @@
         <v>0</v>
       </c>
       <c r="B4" s="14" t="str">
-        <f>LEFT(C2,LEN(C2)-1)&amp;"Id"</f>
-        <v>PlayerCharacterId</v>
+        <f>IF(NOT(ISBLANK(B3)),B3,LEFT(C2,LEN(C2)-1)&amp;"Id")</f>
+        <v>DeityId</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>6</v>
@@ -1119,34 +1025,34 @@
       <c r="H4" s="14"/>
       <c r="J4" s="3" t="str">
         <f>"    "&amp;B4&amp;" "&amp;UPPER(C4)&amp;IF(E4," NOT NULL","")&amp;IF(D4," IDENTITY(1,1)","")&amp;IF(NOT(ISBLANK(F4))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_PK PRIMARY KEY","")&amp;IF(LEN(G4)&gt;0," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_FK FOREIGN KEY REFERENCES "&amp;G4,"")&amp;IF(NOT(ISBLANK(H4))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_DF DEFAULT("&amp;H4&amp;")","")&amp;IF(NOT(ISBLANK(B5)),",","")</f>
-        <v xml:space="preserve">    PlayerCharacterId INT IDENTITY(1,1) CONSTRAINT PlayerCharacters_PlayerCharacterId_PK PRIMARY KEY,</v>
+        <v xml:space="preserve">    DeityId INT IDENTITY(1,1) CONSTRAINT Deities_DeityId_PK PRIMARY KEY,</v>
       </c>
       <c r="L4" s="22" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@Name VARCHAR(50),</v>
+        <v>@AuthorityLevelId INT,</v>
       </c>
       <c r="N4" s="23" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@Name VARCHAR(50),</v>
+        <v>@AuthorityLevelId INT,</v>
       </c>
       <c r="P4" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V4" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="X4" s="12" t="str">
         <f>"namespace Dots.Domain."&amp;B2&amp;"s"</f>
         <v>namespace Dots.Domain.dbos</v>
       </c>
       <c r="Z4" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
@@ -1154,77 +1060,73 @@
         <v>112</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>124</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" t="str">
         <f>IF(UPPER(RIGHT(B5,2))="ID",B$2&amp;"."&amp;LEFT(B5,LEN(B5)-2)&amp;"("&amp;B5&amp;")","")</f>
-        <v/>
+        <v>dbo.AuthorityLevel(AuthorityLevelId)</v>
       </c>
       <c r="H5" s="19"/>
       <c r="J5" s="3" t="str">
         <f t="shared" ref="J5:J32" si="0">"    "&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(E5," NOT NULL","")&amp;IF(D5," IDENTITY(1,1)","")&amp;IF(NOT(ISBLANK(F5))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_PK PRIMARY KEY","")&amp;IF(LEN(G5)&gt;0," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_FK FOREIGN KEY REFERENCES "&amp;G5,"")&amp;IF(NOT(ISBLANK(H5))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_DF DEFAULT("&amp;H5&amp;")","")&amp;IF(NOT(ISBLANK(B6)),",","")</f>
-        <v xml:space="preserve">    Name VARCHAR(50) NOT NULL,</v>
+        <v xml:space="preserve">    AuthorityLevelId INT CONSTRAINT Deities_AuthorityLevelId_FK FOREIGN KEY REFERENCES dbo.AuthorityLevel(AuthorityLevelId),</v>
       </c>
       <c r="L5" s="22" t="str">
         <f t="shared" ref="L5:L19" si="1">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;" "&amp;UPPER(C6)&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>@Level INT,</v>
+        <v>@CompassionLevelId INT,</v>
       </c>
       <c r="N5" s="23" t="str">
         <f t="shared" ref="N5:N19" si="2">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;" "&amp;UPPER(C6)&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>@Level INT,</v>
+        <v>@CompassionLevelId INT,</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="V5" s="16" t="s">
         <v>12</v>
       </c>
       <c r="X5" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Z5" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" t="str">
         <f t="shared" ref="G6" si="3">IF(UPPER(RIGHT(B6,2))="ID",B$2&amp;"."&amp;LEFT(B6,LEN(B6)-2)&amp;"("&amp;B6&amp;")","")</f>
-        <v/>
+        <v>dbo.CompassionLevel(CompassionLevelId)</v>
       </c>
       <c r="H6" s="19"/>
       <c r="J6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    Level INT NOT NULL,</v>
+        <v xml:space="preserve">    CompassionLevelId INT CONSTRAINT Deities_CompassionLevelId_FK FOREIGN KEY REFERENCES dbo.CompassionLevel(CompassionLevelId),</v>
       </c>
       <c r="L6" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@ClassId INT,</v>
+        <v>@FlavourText VARCHAR(MAX)</v>
       </c>
       <c r="N6" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@ClassId INT,</v>
+        <v>@FlavourText VARCHAR(MAX)</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>12</v>
@@ -1238,44 +1140,42 @@
       </c>
       <c r="X6" s="12" t="str">
         <f>"    public interface I"&amp;C2&amp;"Repository"</f>
-        <v>    public interface IPlayerCharactersRepository</v>
+        <v>    public interface IDeitiesRepository</v>
       </c>
       <c r="Z6" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" t="str">
         <f t="shared" ref="G7:G20" si="4">IF(UPPER(RIGHT(B7,2))="ID",B$2&amp;"."&amp;LEFT(B7,LEN(B7)-2)&amp;"("&amp;B7&amp;")","")</f>
-        <v>dbo.Class(ClassId)</v>
+        <v/>
       </c>
       <c r="H7" s="2"/>
       <c r="J7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    ClassId INT NOT NULL CONSTRAINT PlayerCharacters_ClassId_FK FOREIGN KEY REFERENCES dbo.Class(ClassId),</v>
+        <v xml:space="preserve">    FlavourText VARCHAR(MAX)</v>
       </c>
       <c r="L7" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@ParagonPathId INT,</v>
+        <v/>
       </c>
       <c r="N7" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@ParagonPathId INT,</v>
+        <v/>
       </c>
       <c r="P7" s="18" t="str">
         <f>IF(NOT(ISBLANK(B4)),"    ["&amp;B4&amp;"]"&amp;IF(LEN(P8)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">    [PlayerCharacterId],</v>
+        <v xml:space="preserve">    [DeityId],</v>
       </c>
       <c r="R7" s="5" t="str">
         <f>"namespace Dots.Domain."&amp;B2</f>
@@ -1286,59 +1186,55 @@
         <v>namespace Dots.Domain.dbos</v>
       </c>
       <c r="V7" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="X7" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Z7" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" t="str">
         <f t="shared" si="4"/>
-        <v>dbo.ParagonPath(ParagonPathId)</v>
+        <v/>
       </c>
       <c r="H8" s="2"/>
       <c r="J8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    ParagonPathId INT CONSTRAINT PlayerCharacters_ParagonPathId_FK FOREIGN KEY REFERENCES dbo.ParagonPath(ParagonPathId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L8" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@EpicDestinyId INT,</v>
+        <v/>
       </c>
       <c r="N8" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@EpicDestinyId INT,</v>
+        <v/>
       </c>
       <c r="P8" s="18" t="str">
         <f t="shared" ref="P8:P22" si="5">IF(NOT(ISBLANK(B5)),"    ["&amp;B5&amp;"]"&amp;IF(LEN(P9)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">    [Name],</v>
+        <v xml:space="preserve">    [AuthorityLevelId],</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="V8" s="16" t="str">
         <f>"    public static class "&amp;C2&amp;"Helper"</f>
-        <v>    public static class PlayerCharactersHelper</v>
+        <v>    public static class DeitiesHelper</v>
       </c>
       <c r="X8" s="12" t="str">
         <f>"        "&amp;C2&amp;" Get(int "&amp;LOWER(C2)&amp;"Id);"</f>
-        <v>        PlayerCharacters Get(int playercharactersId);</v>
+        <v>        Deities Get(int deitiesId);</v>
       </c>
       <c r="Z8" s="13" t="str">
         <f>"namespace Dots.Domain.Repositories."&amp;B2&amp;"s"</f>
@@ -1346,65 +1242,55 @@
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" t="str">
         <f t="shared" si="4"/>
-        <v>dbo.EpicDestiny(EpicDestinyId)</v>
+        <v/>
       </c>
       <c r="H9" s="2"/>
       <c r="J9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    EpicDestinyId INT CONSTRAINT PlayerCharacters_EpicDestinyId_FK FOREIGN KEY REFERENCES dbo.EpicDestiny(EpicDestinyId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L9" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@ExperiencePoints INT,</v>
+        <v/>
       </c>
       <c r="N9" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@ExperiencePoints INT,</v>
+        <v/>
       </c>
       <c r="P9" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [Level],</v>
+        <v xml:space="preserve">    [CompassionLevelId],</v>
       </c>
       <c r="R9" s="5" t="str">
         <f>"    public interface I"&amp;C2&amp;" : IEntity"</f>
-        <v>    public interface IPlayerCharacters : IEntity</v>
+        <v>    public interface IDeities : IEntity</v>
       </c>
       <c r="T9" s="6" t="str">
         <f>"    public class "&amp;C2&amp;" : IEntity"</f>
-        <v>    public class PlayerCharacters : IEntity</v>
+        <v>    public class Deities : IEntity</v>
       </c>
       <c r="V9" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="X9" s="12" t="s">
         <v>12</v>
       </c>
       <c r="Z9" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" t="str">
         <f t="shared" si="4"/>
@@ -1413,152 +1299,136 @@
       <c r="H10" s="19"/>
       <c r="J10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    ExperiencePoints INT NOT NULL,</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L10" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@RaceId INT,</v>
+        <v/>
       </c>
       <c r="N10" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@RaceId INT,</v>
+        <v/>
       </c>
       <c r="P10" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [ClassId],</v>
+        <v xml:space="preserve">    [FlavourText]</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="V10" s="16" t="str">
         <f>"        public static "&amp;C2&amp;" ParseReader(IDataReader reader)"</f>
-        <v>        public static PlayerCharacters ParseReader(IDataReader reader)</v>
+        <v>        public static Deities ParseReader(IDataReader reader)</v>
       </c>
       <c r="X10" s="12" t="str">
         <f>"        DataResult&lt;"&amp;C2&amp;"&gt; Save("&amp;C2&amp;" "&amp;LOWER(C2)&amp;");"</f>
-        <v>        DataResult&lt;PlayerCharacters&gt; Save(PlayerCharacters playercharacters);</v>
+        <v>        DataResult&lt;Deities&gt; Save(Deities deities);</v>
       </c>
       <c r="Z10" s="13" t="str">
         <f>"    public class Sql"&amp;C2&amp;"Repository : Repository&lt;"&amp;C2&amp;"&gt;, I"&amp;C2&amp;"Repository"</f>
-        <v>    public class SqlPlayerCharactersRepository : Repository&lt;PlayerCharacters&gt;, IPlayerCharactersRepository</v>
+        <v>    public class SqlDeitiesRepository : Repository&lt;Deities&gt;, IDeitiesRepository</v>
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" t="str">
         <f t="shared" si="4"/>
-        <v>dbo.Race(RaceId)</v>
+        <v/>
       </c>
       <c r="H11" s="19"/>
       <c r="J11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    RaceId INT NOT NULL CONSTRAINT PlayerCharacters_RaceId_FK FOREIGN KEY REFERENCES dbo.Race(RaceId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L11" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@SizeId INT,</v>
+        <v/>
       </c>
       <c r="N11" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@SizeId INT,</v>
+        <v/>
       </c>
       <c r="P11" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [ParagonPathId],</v>
+        <v/>
       </c>
       <c r="T11" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="X11" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="X11" s="12" t="s">
-        <v>56</v>
-      </c>
       <c r="Z11" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" t="str">
         <f t="shared" si="4"/>
-        <v>dbo.Size(SizeId)</v>
+        <v/>
       </c>
       <c r="H12" s="19"/>
       <c r="J12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    SizeId INT NOT NULL CONSTRAINT PlayerCharacters_SizeId_FK FOREIGN KEY REFERENCES dbo.Size(SizeId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L12" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@Age INT,</v>
+        <v/>
       </c>
       <c r="N12" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@Age INT,</v>
+        <v/>
       </c>
       <c r="P12" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [EpicDestinyId],</v>
+        <v/>
       </c>
       <c r="Q12" t="str">
         <f t="shared" ref="Q12:Q27" si="6">IF(NOT(ISBLANK(C5)),C5,"")</f>
-        <v>varchar(50)</v>
+        <v>int</v>
       </c>
       <c r="R12" s="5" t="str">
         <f t="shared" ref="R12:R27" si="7">IF(NOT(ISBLANK(C5)),"        "&amp;IF(ISBLANK(S12),C5,S12)&amp;" "&amp;B5&amp;" { get; set; }","")</f>
-        <v xml:space="preserve">        string Name { get; set; }</v>
+        <v xml:space="preserve">        string AuthorityLevelId { get; set; }</v>
       </c>
       <c r="S12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="T12" s="6" t="str">
         <f t="shared" ref="T12:T27" si="8">IF(LEN(R12)&gt;0,"        public "&amp;TRIM(R12),"")</f>
-        <v xml:space="preserve">        public string Name { get; set; }</v>
+        <v xml:space="preserve">        public string AuthorityLevelId { get; set; }</v>
       </c>
       <c r="V12" s="16" t="str">
         <f>"            return new "&amp;C2&amp;"("</f>
-        <v>            return new PlayerCharacters(</v>
+        <v>            return new Deities(</v>
       </c>
       <c r="X12" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Z12" s="13" t="str">
         <f>"        public Sql"&amp;C2&amp;"Repository(IUnitOfWork unitOfWork)"</f>
-        <v>        public SqlPlayerCharactersRepository(IUnitOfWork unitOfWork)</v>
+        <v>        public SqlDeitiesRepository(IUnitOfWork unitOfWork)</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1569,19 +1439,19 @@
       <c r="H13" s="2"/>
       <c r="J13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    Age INT,</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L13" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@GenderId ,</v>
+        <v/>
       </c>
       <c r="N13" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@GenderId ,</v>
+        <v/>
       </c>
       <c r="P13" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [ExperiencePoints],</v>
+        <v/>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="6"/>
@@ -1589,82 +1459,76 @@
       </c>
       <c r="R13" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        string Level { get; set; }</v>
+        <v xml:space="preserve">        string CompassionLevelId { get; set; }</v>
       </c>
       <c r="S13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="T13" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public string Level { get; set; }</v>
+        <v xml:space="preserve">        public string CompassionLevelId { get; set; }</v>
       </c>
       <c r="V13" s="16" t="str">
         <f>"                reader.Get&lt;int&gt;("&amp;C2&amp;"Col.Id),"</f>
-        <v xml:space="preserve">                reader.Get&lt;int&gt;(PlayerCharactersCol.Id),</v>
+        <v xml:space="preserve">                reader.Get&lt;int&gt;(DeitiesCol.Id),</v>
       </c>
       <c r="Z13" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" t="str">
         <f t="shared" si="4"/>
-        <v>dbo.Gender(GenderId)</v>
+        <v/>
       </c>
       <c r="H14" s="2"/>
       <c r="J14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    GenderId  CONSTRAINT PlayerCharacters_GenderId_FK FOREIGN KEY REFERENCES dbo.Gender(GenderId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L14" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@Height VARCHAR(50),</v>
+        <v/>
       </c>
       <c r="N14" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@Height VARCHAR(50),</v>
+        <v/>
       </c>
       <c r="P14" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [RaceId],</v>
+        <v/>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v>varchar(MAX)</v>
       </c>
       <c r="R14" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        int ClassId { get; set; }</v>
+        <v xml:space="preserve">        int FlavourText { get; set; }</v>
       </c>
       <c r="S14" t="s">
         <v>6</v>
       </c>
       <c r="T14" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public int ClassId { get; set; }</v>
+        <v xml:space="preserve">        public int FlavourText { get; set; }</v>
       </c>
       <c r="V14" s="16" t="str">
         <f t="shared" ref="V14:V29" si="9">IF(LEN(S12)&gt;0,"                reader.Get&lt;"&amp;S12&amp;"&gt;("&amp;C$2&amp;"Col."&amp;B5&amp;")"&amp;IF(LEN(V15)&gt;0,",",""),"")</f>
-        <v>                reader.Get&lt;string&gt;(PlayerCharactersCol.Name),</v>
+        <v>                reader.Get&lt;string&gt;(DeitiesCol.AuthorityLevelId),</v>
       </c>
       <c r="Z14" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1675,50 +1539,46 @@
       <c r="H15" s="2"/>
       <c r="J15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    Height VARCHAR(50),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L15" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@Weight VARCHAR(50),</v>
+        <v/>
       </c>
       <c r="N15" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@Weight VARCHAR(50),</v>
+        <v/>
       </c>
       <c r="P15" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [SizeId],</v>
+        <v/>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v/>
       </c>
       <c r="R15" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        CurrencyType ParagonPathId { get; set; }</v>
+        <v/>
       </c>
       <c r="S15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="T15" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public CurrencyType ParagonPathId { get; set; }</v>
+        <v/>
       </c>
       <c r="V15" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;string&gt;(PlayerCharactersCol.Level),</v>
+        <v>                reader.Get&lt;string&gt;(DeitiesCol.CompassionLevelId),</v>
       </c>
       <c r="Z15" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1729,289 +1589,261 @@
       <c r="H16" s="2"/>
       <c r="J16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    Weight VARCHAR(50),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L16" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@AlignmentId INT,</v>
+        <v/>
       </c>
       <c r="N16" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@AlignmentId INT,</v>
+        <v/>
       </c>
       <c r="P16" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [Age],</v>
+        <v/>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v/>
       </c>
       <c r="R16" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        bool EpicDestinyId { get; set; }</v>
+        <v/>
       </c>
       <c r="S16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="T16" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public bool EpicDestinyId { get; set; }</v>
+        <v/>
       </c>
       <c r="V16" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;int&gt;(PlayerCharactersCol.ClassId),</v>
+        <v>                reader.Get&lt;int&gt;(DeitiesCol.FlavourText),</v>
       </c>
     </row>
     <row r="17" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" t="str">
         <f t="shared" si="4"/>
-        <v>dbo.Alignment(AlignmentId)</v>
+        <v/>
       </c>
       <c r="H17" s="2"/>
       <c r="J17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    AlignmentId INT NOT NULL CONSTRAINT PlayerCharacters_AlignmentId_FK FOREIGN KEY REFERENCES dbo.Alignment(AlignmentId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L17" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@DeityId INT,</v>
+        <v/>
       </c>
       <c r="N17" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@DeityId INT,</v>
+        <v/>
       </c>
       <c r="P17" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [GenderId],</v>
+        <v/>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v/>
       </c>
       <c r="R17" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        string ExperiencePoints { get; set; }</v>
+        <v/>
       </c>
       <c r="S17" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="T17" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public string ExperiencePoints { get; set; }</v>
+        <v/>
       </c>
       <c r="V17" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;CurrencyType&gt;(PlayerCharactersCol.ParagonPathId),</v>
+        <v>                reader.Get&lt;CurrencyType&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z17" s="13" t="str">
         <f>"        protected override "&amp;C2&amp;" Map(IDataReader reader)"</f>
-        <v xml:space="preserve">        protected override PlayerCharacters Map(IDataReader reader)</v>
+        <v xml:space="preserve">        protected override Deities Map(IDataReader reader)</v>
       </c>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" t="str">
         <f t="shared" si="4"/>
-        <v>dbo.Deity(DeityId)</v>
+        <v/>
       </c>
       <c r="H18" s="2"/>
       <c r="J18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    DeityId INT CONSTRAINT PlayerCharacters_DeityId_FK FOREIGN KEY REFERENCES dbo.Deity(DeityId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L18" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@InitiativeId INT,</v>
+        <v/>
       </c>
       <c r="N18" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@InitiativeId INT,</v>
+        <v/>
       </c>
       <c r="P18" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [Height],</v>
+        <v/>
       </c>
       <c r="Q18" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v/>
       </c>
       <c r="R18" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        string RaceId { get; set; }</v>
+        <v/>
       </c>
       <c r="S18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="T18" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public string RaceId { get; set; }</v>
+        <v/>
       </c>
       <c r="V18" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;bool&gt;(PlayerCharactersCol.EpicDestinyId),</v>
+        <v>                reader.Get&lt;bool&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z18" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" t="str">
         <f t="shared" si="4"/>
-        <v>dbo.Initiative(InitiativeId)</v>
+        <v/>
       </c>
       <c r="H19" s="2"/>
       <c r="J19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    InitiativeId INT NOT NULL CONSTRAINT PlayerCharacters_InitiativeId_FK FOREIGN KEY REFERENCES dbo.Initiative(InitiativeId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L19" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@AbilitySetId INT,</v>
+        <v/>
       </c>
       <c r="N19" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@AbilitySetId INT,</v>
+        <v/>
       </c>
       <c r="P19" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [Weight],</v>
+        <v/>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v/>
       </c>
       <c r="R19" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        string SizeId { get; set; }</v>
+        <v/>
       </c>
       <c r="S19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="T19" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public string SizeId { get; set; }</v>
+        <v/>
       </c>
       <c r="V19" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;string&gt;(PlayerCharactersCol.ExperiencePoints),</v>
+        <v>                reader.Get&lt;string&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z19" s="13" t="str">
         <f>"           return "&amp;C2&amp;"Helper.ParseReader(reader);"</f>
-        <v>           return PlayerCharactersHelper.ParseReader(reader);</v>
+        <v>           return DeitiesHelper.ParseReader(reader);</v>
       </c>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" t="str">
         <f t="shared" si="4"/>
-        <v>dbo.AbilitySet(AbilitySetId)</v>
+        <v/>
       </c>
       <c r="H20" s="2"/>
       <c r="J20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    AbilitySetId INT NOT NULL CONSTRAINT PlayerCharacters_AbilitySetId_FK FOREIGN KEY REFERENCES dbo.AbilitySet(AbilitySetId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N20" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P20" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [AlignmentId],</v>
+        <v/>
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v/>
       </c>
       <c r="R20" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        InvoiceLayoutType Age { get; set; }</v>
+        <v/>
       </c>
       <c r="S20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="T20" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public InvoiceLayoutType Age { get; set; }</v>
+        <v/>
       </c>
       <c r="V20" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;string&gt;(PlayerCharactersCol.RaceId),</v>
+        <v>                reader.Get&lt;string&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z20" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" t="str">
         <f t="shared" ref="G21:G24" si="10">IF(UPPER(RIGHT(B21,2))="ID",B$2&amp;"."&amp;LEFT(B21,LEN(B21)-2)&amp;"("&amp;B21&amp;")","")</f>
-        <v>dbo.DefenseSet(DefenseSetId)</v>
+        <v/>
       </c>
       <c r="H21" s="2"/>
       <c r="J21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    DefenseSetId INT NOT NULL CONSTRAINT PlayerCharacters_DefenseSetId_FK FOREIGN KEY REFERENCES dbo.DefenseSet(DefenseSetId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="N21" s="23" t="s">
         <v>11</v>
       </c>
       <c r="P21" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [DeityId],</v>
+        <v/>
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="6"/>
@@ -2030,123 +1862,105 @@
       </c>
       <c r="V21" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;string&gt;(PlayerCharactersCol.SizeId),</v>
+        <v>                reader.Get&lt;string&gt;(DeitiesCol.),</v>
       </c>
     </row>
     <row r="22" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" t="str">
         <f t="shared" si="10"/>
-        <v>dbo.MovementSet(MovementSetId)</v>
+        <v/>
       </c>
       <c r="H22" s="2"/>
       <c r="J22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    MovementSetId INT NOT NULL CONSTRAINT PlayerCharacters_MovementSetId_FK FOREIGN KEY REFERENCES dbo.MovementSet(MovementSetId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P22" s="18" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    [InitiativeId]</v>
+        <v/>
       </c>
       <c r="Q22" t="str">
         <f t="shared" si="6"/>
-        <v>varchar(50)</v>
+        <v/>
       </c>
       <c r="R22" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        TimeFrequency Height { get; set; }</v>
+        <v/>
       </c>
       <c r="S22" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="T22" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public TimeFrequency Height { get; set; }</v>
+        <v/>
       </c>
       <c r="V22" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;InvoiceLayoutType&gt;(PlayerCharactersCol.Age),</v>
+        <v>                reader.Get&lt;InvoiceLayoutType&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z22" s="13" t="str">
         <f>"        public "&amp;C2&amp;" Get(int "&amp;LOWER(C2)&amp;"Id)"</f>
-        <v>        public PlayerCharacters Get(int playercharactersId)</v>
+        <v>        public Deities Get(int deitiesId)</v>
       </c>
     </row>
     <row r="23" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" t="str">
         <f t="shared" si="10"/>
-        <v>dbo.SenseSet(SenseSetId)</v>
+        <v/>
       </c>
       <c r="H23" s="2"/>
       <c r="J23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    SenseSetId INT NOT NULL CONSTRAINT PlayerCharacters_SenseSetId_FK FOREIGN KEY REFERENCES dbo.SenseSet(SenseSetId),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N23" s="23" t="str">
         <f>"UPDATE "&amp;B2&amp;"."&amp;C2</f>
-        <v>UPDATE dbo.PlayerCharacters</v>
+        <v>UPDATE dbo.Deities</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="6"/>
-        <v>varchar(50)</v>
+        <v/>
       </c>
       <c r="R23" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        TimeFrequency Weight { get; set; }</v>
+        <v/>
       </c>
       <c r="S23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="T23" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public TimeFrequency Weight { get; set; }</v>
+        <v/>
       </c>
       <c r="V23" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;int&gt;(PlayerCharactersCol.GenderId),</v>
+        <v>                reader.Get&lt;int&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z23" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" t="str">
         <f t="shared" si="10"/>
@@ -2155,49 +1969,45 @@
       <c r="H24" s="2"/>
       <c r="J24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    BaseHitPoints INT NOT NULL,</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L24" s="22" t="str">
         <f>"FROM "&amp;B2&amp;"."&amp;C2</f>
-        <v>FROM dbo.PlayerCharacters</v>
+        <v>FROM dbo.Deities</v>
       </c>
       <c r="N24" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P24" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v/>
       </c>
       <c r="R24" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        bool AlignmentId { get; set; }</v>
+        <v/>
       </c>
       <c r="S24" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="T24" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public bool AlignmentId { get; set; }</v>
+        <v/>
       </c>
       <c r="V24" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;TimeFrequency&gt;(PlayerCharactersCol.Height),</v>
+        <v>                reader.Get&lt;TimeFrequency&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z24" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Get""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_PlayerCharacters_Get"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Deities_Get"))</v>
       </c>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2208,53 +2018,47 @@
       <c r="H25" s="2"/>
       <c r="J25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    AdditionalHitPoints INT,</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N25" s="23" t="str">
         <f t="shared" ref="N25:N40" si="12">IF(NOT(ISBLANK(B5)),"["&amp;B5&amp;"] = @"&amp;B5&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>[Name] = @Name,</v>
+        <v>[AuthorityLevelId] = @AuthorityLevelId,</v>
       </c>
       <c r="P25" s="18" t="str">
         <f>"    "&amp;B2&amp;"."&amp;C2</f>
-        <v xml:space="preserve">    dbo.PlayerCharacters</v>
+        <v xml:space="preserve">    dbo.Deities</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v/>
       </c>
       <c r="R25" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        CommunicationType DeityId { get; set; }</v>
+        <v/>
       </c>
       <c r="S25" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="T25" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public CommunicationType DeityId { get; set; }</v>
+        <v/>
       </c>
       <c r="V25" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;TimeFrequency&gt;(PlayerCharactersCol.Weight),</v>
+        <v>                reader.Get&lt;TimeFrequency&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z25" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" t="str">
         <f t="shared" si="11"/>
@@ -2263,46 +2067,42 @@
       <c r="H26" s="2"/>
       <c r="J26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    BaseActionPoints INT NOT NULL,</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L26" s="22" t="str">
         <f>IF(NOT(ISBLANK(B4)),"["&amp;B4&amp;"] = ISNULL(@"&amp;B4&amp;", 0)","")</f>
-        <v>[PlayerCharacterId] = ISNULL(@PlayerCharacterId, 0)</v>
+        <v>[DeityId] = ISNULL(@DeityId, 0)</v>
       </c>
       <c r="N26" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[Level] = @Level,</v>
+        <v>[CompassionLevelId] = @CompassionLevelId,</v>
       </c>
       <c r="P26" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v/>
       </c>
       <c r="R26" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        int InitiativeId { get; set; }</v>
+        <v/>
       </c>
       <c r="T26" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public int InitiativeId { get; set; }</v>
+        <v/>
       </c>
       <c r="V26" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;bool&gt;(PlayerCharactersCol.AlignmentId),</v>
+        <v>                reader.Get&lt;bool&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z26" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -2313,70 +2113,64 @@
       <c r="H27" s="2"/>
       <c r="J27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    AdditionalActionPoints INT,</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N27" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[ClassId] = @ClassId,</v>
+        <v>[FlavourText] = @FlavourText</v>
       </c>
       <c r="P27" s="18" t="str">
         <f>"    "&amp;B4&amp;" = @"&amp;B4</f>
-        <v xml:space="preserve">    PlayerCharacterId = @PlayerCharacterId</v>
+        <v xml:space="preserve">    DeityId = @DeityId</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
+        <v/>
       </c>
       <c r="R27" s="5" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        int AbilitySetId { get; set; }</v>
+        <v/>
       </c>
       <c r="T27" s="6" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">        public int AbilitySetId { get; set; }</v>
+        <v/>
       </c>
       <c r="V27" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>                reader.Get&lt;CommunicationType&gt;(PlayerCharactersCol.DeityId)</v>
+        <v>                reader.Get&lt;CommunicationType&gt;(DeitiesCol.)</v>
       </c>
       <c r="Z27" s="13" t="str">
         <f>"                    .AddWithValue(""@"&amp;C2&amp;"Id"", "&amp;LOWER(C2)&amp;"Id, SqlDbType.Int);"</f>
-        <v>                    .AddWithValue("@PlayerCharactersId", playercharactersId, SqlDbType.Int);</v>
+        <v>                    .AddWithValue("@DeitiesId", deitiesId, SqlDbType.Int);</v>
       </c>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" t="str">
         <f t="shared" si="11"/>
-        <v>dbo.SkillSet(SkillSetId)</v>
+        <v/>
       </c>
       <c r="H28" s="2"/>
       <c r="J28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    SkillSetId INT NOT NULL CONSTRAINT PlayerCharacters_SkillSetId_FK FOREIGN KEY REFERENCES dbo.SkillSet(SkillSetId)</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L28" s="22" t="s">
         <v>11</v>
       </c>
       <c r="N28" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[ParagonPathId] = @ParagonPathId,</v>
+        <v/>
       </c>
       <c r="R28" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="V28" s="16" t="str">
         <f t="shared" si="9"/>
@@ -2400,25 +2194,25 @@
       </c>
       <c r="L29" s="22" t="str">
         <f>"INSERT INTO "&amp;B2&amp;"."&amp;C2&amp;" ("</f>
-        <v>INSERT INTO dbo.PlayerCharacters (</v>
+        <v>INSERT INTO dbo.Deities (</v>
       </c>
       <c r="N29" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[EpicDestinyId] = @EpicDestinyId,</v>
+        <v/>
       </c>
       <c r="R29" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="T29" s="6" t="str">
         <f>"        public "&amp;C2&amp;"("</f>
-        <v>        public PlayerCharacters(</v>
+        <v>        public Deities(</v>
       </c>
       <c r="V29" s="16" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="Z29" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="2:26" x14ac:dyDescent="0.25">
@@ -2438,18 +2232,18 @@
       </c>
       <c r="L30" s="22" t="str">
         <f>IF(NOT(ISBLANK(B5)),"["&amp;B5&amp;"]"&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>[Name],</v>
+        <v>[AuthorityLevelId],</v>
       </c>
       <c r="N30" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[ExperiencePoints] = @ExperiencePoints,</v>
+        <v/>
       </c>
       <c r="T30" s="6" t="str">
         <f>IF(NOT(ISBLANK(B4)),"            int"&amp;" "&amp;LOWER(LEFT(B4,1))&amp;MID(B4,2,LEN(B4)-1)&amp;IF(LEN(T31)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            int playerCharacterId,</v>
+        <v xml:space="preserve">            int deityId,</v>
       </c>
       <c r="Z30" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="2:26" x14ac:dyDescent="0.25">
@@ -2469,21 +2263,21 @@
       </c>
       <c r="L31" s="22" t="str">
         <f t="shared" ref="L31:L45" si="14">IF(NOT(ISBLANK(B6)),"["&amp;B6&amp;"]"&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>[Level],</v>
+        <v>[CompassionLevelId],</v>
       </c>
       <c r="N31" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[RaceId] = @RaceId,</v>
+        <v/>
       </c>
       <c r="T31" s="6" t="str">
         <f t="shared" ref="T31:T46" si="15">IF(NOT(ISBLANK(B5)),"            "&amp;S12&amp;" "&amp;LOWER(LEFT(B5,1))&amp;MID(B5,2,LEN(B5)-1)&amp;IF(LEN(T32)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            string name,</v>
+        <v xml:space="preserve">            string authorityLevelId,</v>
       </c>
       <c r="V31" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Z31" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="2:26" x14ac:dyDescent="0.25">
@@ -2503,18 +2297,18 @@
       </c>
       <c r="L32" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[ClassId],</v>
+        <v>[FlavourText]</v>
       </c>
       <c r="N32" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[SizeId] = @SizeId,</v>
+        <v/>
       </c>
       <c r="T32" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            string level,</v>
+        <v xml:space="preserve">            string compassionLevelId,</v>
       </c>
       <c r="V32" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
@@ -2527,98 +2321,98 @@
       </c>
       <c r="L33" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[ParagonPathId],</v>
+        <v/>
       </c>
       <c r="N33" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[Age] = @Age,</v>
+        <v/>
       </c>
       <c r="T33" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            int classId,</v>
+        <v xml:space="preserve">            int flavourText</v>
       </c>
       <c r="V33" s="16" t="s">
         <v>12</v>
       </c>
       <c r="Z33" s="13" t="str">
         <f>"        public DataResult&lt;"&amp;C2&amp;"&gt; Save("&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;PlayerCharacters&gt; Save(PlayerCharacters value)</v>
+        <v xml:space="preserve">        public DataResult&lt;Deities&gt; Save(Deities value)</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L34" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[EpicDestinyId],</v>
+        <v/>
       </c>
       <c r="N34" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[GenderId] = @GenderId,</v>
+        <v/>
       </c>
       <c r="T34" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            CurrencyType paragonPathId,</v>
+        <v/>
       </c>
       <c r="V34" s="16" t="str">
         <f>"        public static IEnumerable&lt;"&amp;C2&amp;"&gt; ParseMultipleReader(IDataReader reader)"</f>
-        <v>        public static IEnumerable&lt;PlayerCharacters&gt; ParseMultipleReader(IDataReader reader)</v>
+        <v>        public static IEnumerable&lt;Deities&gt; ParseMultipleReader(IDataReader reader)</v>
       </c>
       <c r="Z34" s="13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L35" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[ExperiencePoints],</v>
+        <v/>
       </c>
       <c r="N35" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[Height] = @Height,</v>
+        <v/>
       </c>
       <c r="T35" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            bool epicDestinyId,</v>
+        <v/>
       </c>
       <c r="V35" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Z35" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L36" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[RaceId],</v>
+        <v/>
       </c>
       <c r="N36" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[Weight] = @Weight,</v>
+        <v/>
       </c>
       <c r="T36" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            string experiencePoints,</v>
+        <v/>
       </c>
       <c r="V36" s="16" t="str">
         <f>"            var "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;"s = new List&lt;"&amp;C2&amp;"&gt;();"</f>
-        <v>            var playerCharacterss = new List&lt;PlayerCharacters&gt;();</v>
+        <v>            var deitiess = new List&lt;Deities&gt;();</v>
       </c>
       <c r="Z36" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L37" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[SizeId],</v>
+        <v/>
       </c>
       <c r="N37" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[AlignmentId] = @AlignmentId,</v>
+        <v/>
       </c>
       <c r="T37" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            string raceId,</v>
+        <v/>
       </c>
       <c r="V37" s="16" t="s">
         <v>12</v>
@@ -2627,90 +2421,90 @@
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L38" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[Age],</v>
+        <v/>
       </c>
       <c r="N38" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[DeityId] = @DeityId,</v>
+        <v/>
       </c>
       <c r="T38" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            string sizeId,</v>
+        <v/>
       </c>
       <c r="V38" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z38" s="13" t="str">
         <f>"        public DataResult&lt;"&amp;C2&amp;"&gt; Create("&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;PlayerCharacters&gt; Create(PlayerCharacters value)</v>
+        <v xml:space="preserve">        public DataResult&lt;Deities&gt; Create(Deities value)</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L39" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[GenderId],</v>
+        <v/>
       </c>
       <c r="N39" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[InitiativeId] = @InitiativeId,</v>
+        <v/>
       </c>
       <c r="T39" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            InvoiceLayoutType age,</v>
+        <v/>
       </c>
       <c r="V39" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Z39" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L40" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[Height],</v>
+        <v/>
       </c>
       <c r="N40" s="23" t="str">
         <f t="shared" si="12"/>
-        <v>[AbilitySetId] = @AbilitySetId,</v>
+        <v/>
       </c>
       <c r="T40" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            int genderId,</v>
+        <v/>
       </c>
       <c r="V40" s="16" t="str">
         <f>"                "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;".Add(ParseReader(reader));"</f>
-        <v>                playerCharacters.Add(ParseReader(reader));</v>
+        <v>                deities.Add(ParseReader(reader));</v>
       </c>
       <c r="Z40" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Create""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_PlayerCharacters_Create"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Deities_Create"))</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L41" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[Weight],</v>
+        <v/>
       </c>
       <c r="N41" s="23" t="str">
         <f>IF(NOT(ISBLANK(B4)),"WHERE ["&amp;B4&amp;"] = ISNULL(@"&amp;B4&amp;", 0)","")</f>
-        <v>WHERE [PlayerCharacterId] = ISNULL(@PlayerCharacterId, 0)</v>
+        <v>WHERE [DeityId] = ISNULL(@DeityId, 0)</v>
       </c>
       <c r="T41" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            TimeFrequency height,</v>
+        <v/>
       </c>
       <c r="V41" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Z41" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L42" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[AlignmentId],</v>
+        <v/>
       </c>
       <c r="N42" s="23" t="str">
         <f>IF(NOT(ISBLANK(D16)),"["&amp;D16&amp;"]"&amp;IF(NOT(ISBLANK(D17)),",",""),"")</f>
@@ -2718,37 +2512,37 @@
       </c>
       <c r="T42" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            TimeFrequency weight,</v>
+        <v/>
       </c>
       <c r="V42" s="16" t="s">
         <v>12</v>
       </c>
       <c r="Z42" s="13" t="str">
         <f>"                var idParameter = command.AddOutput(""@"&amp;C2&amp;"Id"", SqlDbType.Int);"</f>
-        <v>                var idParameter = command.AddOutput("@PlayerCharactersId", SqlDbType.Int);</v>
+        <v>                var idParameter = command.AddOutput("@DeitiesId", SqlDbType.Int);</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L43" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[DeityId],</v>
+        <v/>
       </c>
       <c r="N43" s="23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="T43" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            bool alignmentId,</v>
+        <v/>
       </c>
       <c r="V43" s="16" t="str">
         <f>"            return "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;";"</f>
-        <v>            return playerCharacters;</v>
+        <v>            return deities;</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L44" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[InitiativeId],</v>
+        <v/>
       </c>
       <c r="N44" s="23" t="str">
         <f>IF(NOT(ISBLANK(D18)),"["&amp;D18&amp;"]"&amp;IF(NOT(ISBLANK(D19)),",",""),"")</f>
@@ -2756,407 +2550,407 @@
       </c>
       <c r="T44" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            CommunicationType deityId,</v>
+        <v/>
       </c>
       <c r="V44" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z44" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L45" s="22" t="str">
         <f t="shared" si="14"/>
-        <v>[AbilitySetId],</v>
+        <v/>
       </c>
       <c r="N45" s="23" t="s">
         <v>14</v>
       </c>
       <c r="T45" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">             initiativeId,</v>
+        <v/>
       </c>
       <c r="V45" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="Z45" s="13" t="e">
+      <c r="Z45" s="13" t="str">
         <f t="shared" ref="Z45" si="16">IF(NOT(ISBLANK(B4)),"                    .AddWithValue(""@"&amp;B4&amp;""", value.Id,  SqlDbType.Int"&amp;")"&amp;IF(LEN(Z46)&gt;0,"",";"),"")</f>
-        <v>#VALUE!</v>
+        <v>                    .AddWithValue("@DeityId", value.Id,  SqlDbType.Int)</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L46" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="T46" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">             abilitySetId,</v>
+        <v/>
       </c>
       <c r="V46" s="16" t="str">
         <f>"        private enum "&amp;C2&amp;"Col"</f>
-        <v>        private enum PlayerCharactersCol</v>
-      </c>
-      <c r="Z46" s="13" t="e">
+        <v>        private enum DeitiesCol</v>
+      </c>
+      <c r="Z46" s="13" t="str">
         <f>IF(NOT(ISBLANK(B5)),"                    .AddWithValue(""@"&amp;B5&amp;""", value."&amp;B5&amp;", SqlDbType."&amp;IF(NOT(OR(ISBLANK(Q12),Q12="int")),UPPER(LEFT(Q12,1))&amp;MID(Q12,2,LEN(Q12)-1),"Int")&amp;")"&amp;IF(LEFT(Z47,24)="                    .Add","",";"),"")</f>
-        <v>#VALUE!</v>
+        <v>                    .AddWithValue("@AuthorityLevelId", value.AuthorityLevelId, SqlDbType.Int)</v>
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L47" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T47" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V47" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z47" s="13" t="e">
+        <v>52</v>
+      </c>
+      <c r="Z47" s="13" t="str">
         <f t="shared" ref="Z47:Z62" si="17">IF(NOT(ISBLANK(B6)),"                    .AddWithValue(""@"&amp;B6&amp;""", value."&amp;B6&amp;", SqlDbType."&amp;IF(NOT(OR(ISBLANK(Q13),Q13="int")),UPPER(LEFT(Q13,1))&amp;MID(Q13,2,LEN(Q13)-1),"Int")&amp;")"&amp;IF(LEFT(Z48,24)="                    .Add","",";"),"")</f>
-        <v>#VALUE!</v>
+        <v>                    .AddWithValue("@CompassionLevelId", value.CompassionLevelId, SqlDbType.Int)</v>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L48" s="22" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@Name,</v>
+        <v>@AuthorityLevelId,</v>
       </c>
       <c r="T48" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V48" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z48" s="13" t="e">
+        <v>86</v>
+      </c>
+      <c r="Z48" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>                    .AddWithValue("@FlavourText", value.FlavourText, SqlDbType.Varchar(MAX));</v>
       </c>
     </row>
     <row r="49" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L49" s="22" t="str">
         <f t="shared" ref="L49:L63" si="18">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>@Level,</v>
+        <v>@CompassionLevelId,</v>
       </c>
       <c r="T49" s="6" t="str">
         <f>IF(NOT(ISBLANK(B4)),"            Id = "&amp;LOWER(LEFT(B4,1))&amp;MID(B4,2,LEN(B4)-1)&amp;";","")</f>
-        <v xml:space="preserve">            Id = playerCharacterId;</v>
+        <v xml:space="preserve">            Id = deityId;</v>
       </c>
       <c r="V49" s="16" t="str">
         <f t="shared" ref="V49:V64" si="19">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;IF(LEN(V15)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            Name,</v>
-      </c>
-      <c r="Z49" s="13" t="e">
+        <v xml:space="preserve">            AuthorityLevelId,</v>
+      </c>
+      <c r="Z49" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="50" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L50" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@ClassId,</v>
+        <v>@FlavourText</v>
       </c>
       <c r="T50" s="6" t="str">
         <f t="shared" ref="T50:T65" si="20">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;" = "&amp;LOWER(LEFT(B5,1))&amp;MID(B5,2,LEN(B5)-1)&amp;";","")</f>
-        <v xml:space="preserve">            Name = name;</v>
+        <v xml:space="preserve">            AuthorityLevelId = authorityLevelId;</v>
       </c>
       <c r="V50" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            Level,</v>
-      </c>
-      <c r="Z50" s="13" t="e">
+        <v xml:space="preserve">            CompassionLevelId,</v>
+      </c>
+      <c r="Z50" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="51" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L51" s="22" t="str">
         <f>IF(NOT(ISBLANK(B8)),"@"&amp;B8&amp;IF(NOT(ISBLANK(B9)),",",""),"")</f>
-        <v>@ParagonPathId,</v>
+        <v/>
       </c>
       <c r="T51" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            Level = level;</v>
+        <v xml:space="preserve">            CompassionLevelId = compassionLevelId;</v>
       </c>
       <c r="V51" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            ClassId,</v>
-      </c>
-      <c r="Z51" s="13" t="e">
+        <v xml:space="preserve">            FlavourText,</v>
+      </c>
+      <c r="Z51" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="52" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L52" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@EpicDestinyId,</v>
+        <v/>
       </c>
       <c r="T52" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            ClassId = classId;</v>
+        <v xml:space="preserve">            FlavourText = flavourText;</v>
       </c>
       <c r="V52" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            ParagonPathId,</v>
-      </c>
-      <c r="Z52" s="13" t="e">
+        <v/>
+      </c>
+      <c r="Z52" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="53" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L53" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@ExperiencePoints,</v>
+        <v/>
       </c>
       <c r="T53" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            ParagonPathId = paragonPathId;</v>
+        <v/>
       </c>
       <c r="V53" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            EpicDestinyId,</v>
-      </c>
-      <c r="Z53" s="13" t="e">
+        <v/>
+      </c>
+      <c r="Z53" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="54" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L54" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@RaceId,</v>
+        <v/>
       </c>
       <c r="T54" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            EpicDestinyId = epicDestinyId;</v>
+        <v/>
       </c>
       <c r="V54" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            ExperiencePoints,</v>
-      </c>
-      <c r="Z54" s="13" t="e">
+        <v/>
+      </c>
+      <c r="Z54" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="55" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L55" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@SizeId,</v>
+        <v/>
       </c>
       <c r="T55" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            ExperiencePoints = experiencePoints;</v>
+        <v/>
       </c>
       <c r="V55" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            RaceId,</v>
-      </c>
-      <c r="Z55" s="13" t="e">
+        <v/>
+      </c>
+      <c r="Z55" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="56" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L56" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@Age,</v>
+        <v/>
       </c>
       <c r="T56" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            RaceId = raceId;</v>
+        <v/>
       </c>
       <c r="V56" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            SizeId,</v>
+        <v/>
       </c>
       <c r="Z56" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>                    .AddWithValue("@Height", value.Height, SqlDbType.Varchar(50))</v>
+        <v/>
       </c>
     </row>
     <row r="57" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L57" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@GenderId,</v>
+        <v/>
       </c>
       <c r="T57" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            SizeId = sizeId;</v>
+        <v/>
       </c>
       <c r="V57" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            Age,</v>
+        <v/>
       </c>
       <c r="Z57" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>                    .AddWithValue("@Weight", value.Weight, SqlDbType.Varchar(50))</v>
+        <v/>
       </c>
     </row>
     <row r="58" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L58" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@Height,</v>
+        <v/>
       </c>
       <c r="T58" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            Age = age;</v>
+        <v/>
       </c>
       <c r="V58" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            GenderId,</v>
+        <v/>
       </c>
       <c r="Z58" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>                    .AddWithValue("@AlignmentId", value.AlignmentId, SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="59" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L59" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@Weight,</v>
+        <v/>
       </c>
       <c r="T59" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            GenderId = genderId;</v>
+        <v/>
       </c>
       <c r="V59" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            Height,</v>
+        <v/>
       </c>
       <c r="Z59" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>                    .AddWithValue("@DeityId", value.DeityId, SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="60" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L60" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@AlignmentId,</v>
+        <v/>
       </c>
       <c r="T60" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            Height = height;</v>
+        <v/>
       </c>
       <c r="V60" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            Weight,</v>
+        <v/>
       </c>
       <c r="Z60" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>                    .AddWithValue("@InitiativeId", value.InitiativeId, SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="61" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L61" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@DeityId,</v>
+        <v/>
       </c>
       <c r="T61" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            Weight = weight;</v>
+        <v/>
       </c>
       <c r="V61" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            AlignmentId,</v>
+        <v/>
       </c>
       <c r="Z61" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>                    .AddWithValue("@AbilitySetId", value.AbilitySetId, SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="62" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L62" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@InitiativeId,</v>
+        <v/>
       </c>
       <c r="T62" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            AlignmentId = alignmentId;</v>
+        <v/>
       </c>
       <c r="V62" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            DeityId</v>
+        <v/>
       </c>
       <c r="Z62" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>                    .AddWithValue("@DefenseSetId", value.DefenseSetId, SqlDbType.Int);</v>
+        <v/>
       </c>
     </row>
     <row r="63" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L63" s="22" t="str">
         <f t="shared" si="18"/>
-        <v>@AbilitySetId,</v>
+        <v/>
       </c>
       <c r="T63" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            DeityId = deityId;</v>
+        <v/>
       </c>
       <c r="V63" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            InitiativeId</v>
+        <v/>
       </c>
       <c r="Z63" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L64" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="T64" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            InitiativeId = initiativeId;</v>
+        <v/>
       </c>
       <c r="V64" s="16" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">            AbilitySetId</v>
+        <v/>
       </c>
     </row>
     <row r="65" spans="12:26" x14ac:dyDescent="0.25">
       <c r="T65" s="6" t="str">
         <f t="shared" si="20"/>
-        <v xml:space="preserve">            AbilitySetId = abilitySetId;</v>
+        <v/>
       </c>
       <c r="V65" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z65" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L66" s="22" t="str">
         <f>"SELECT @"&amp;B4&amp;" = SCOPE_IDENTITY()"</f>
-        <v>SELECT @PlayerCharacterId = SCOPE_IDENTITY()</v>
+        <v>SELECT @DeityId = SCOPE_IDENTITY()</v>
       </c>
       <c r="V66" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="12:26" x14ac:dyDescent="0.25">
       <c r="T67" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="V67" s="16" t="s">
         <v>55</v>
-      </c>
-      <c r="V67" s="16" t="s">
-        <v>57</v>
       </c>
       <c r="Z67" s="13" t="str">
         <f>"                return new DataResult&lt;"&amp;C2&amp;"&gt;(value, result);"</f>
-        <v>                return new DataResult&lt;PlayerCharacters&gt;(value, result);</v>
+        <v>                return new DataResult&lt;Deities&gt;(value, result);</v>
       </c>
     </row>
     <row r="68" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L68" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="T68" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Z68" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="12:26" x14ac:dyDescent="0.25">
@@ -3164,188 +2958,188 @@
         <v>14</v>
       </c>
       <c r="T69" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Z69" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z71" s="13" t="str">
         <f>"        public DataResult&lt;"&amp;C2&amp;"&gt; Update("&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;PlayerCharacters&gt; Update(PlayerCharacters value)</v>
+        <v xml:space="preserve">        public DataResult&lt;Deities&gt; Update(Deities value)</v>
       </c>
     </row>
     <row r="72" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z72" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z73" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Update""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_PlayerCharacters_Update"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Deities_Update"))</v>
       </c>
     </row>
     <row r="74" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z74" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z75" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="Z76" s="13" t="e">
+      <c r="Z76" s="13" t="str">
         <f t="shared" ref="Z76" si="21">IF(NOT(ISBLANK(B4)),"                    .AddWithValue(""@"&amp;B4&amp;""", value.Id,  SqlDbType.Int"&amp;")"&amp;IF(LEN(Z77)&gt;0,"",";"),"")</f>
-        <v>#VALUE!</v>
+        <v>                    .AddWithValue("@DeityId", value.Id,  SqlDbType.Int)</v>
       </c>
     </row>
     <row r="77" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="Z77" s="13" t="e">
+      <c r="Z77" s="13" t="str">
         <f>IF(NOT(ISBLANK(B5)),"                    .AddWithValue(""@"&amp;B5&amp;""", value."&amp;B5&amp;", SqlDbType."&amp;IF(NOT(OR(ISBLANK(Q12),Q12="int")),UPPER(LEFT(Q12,1))&amp;MID(Q12,2,LEN(Q12)-1),"Int")&amp;")"&amp;IF(LEFT(Z47,24)="                    .Add","",";"),"")</f>
-        <v>#VALUE!</v>
+        <v>                    .AddWithValue("@AuthorityLevelId", value.AuthorityLevelId, SqlDbType.Int)</v>
       </c>
     </row>
     <row r="78" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="Z78" s="13" t="e">
+      <c r="Z78" s="13" t="str">
         <f t="shared" ref="Z78:Z90" si="22">IF(NOT(ISBLANK(B6)),"                    .AddWithValue(""@"&amp;B6&amp;""", value."&amp;B6&amp;", SqlDbType."&amp;IF(NOT(OR(ISBLANK(Q13),Q13="int")),UPPER(LEFT(Q13,1))&amp;MID(Q13,2,LEN(Q13)-1),"Int")&amp;")"&amp;IF(LEFT(Z48,24)="                    .Add","",";"),"")</f>
-        <v>#VALUE!</v>
+        <v>                    .AddWithValue("@CompassionLevelId", value.CompassionLevelId, SqlDbType.Int)</v>
       </c>
     </row>
     <row r="79" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="Z79" s="13" t="e">
+      <c r="Z79" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
+        <v>                    .AddWithValue("@FlavourText", value.FlavourText, SqlDbType.Varchar(MAX));</v>
       </c>
     </row>
     <row r="80" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="Z80" s="13" t="e">
+      <c r="Z80" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="81" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z81" s="13" t="e">
+      <c r="Z81" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="82" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z82" s="13" t="e">
+      <c r="Z82" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="83" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z83" s="13" t="e">
+      <c r="Z83" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="84" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z84" s="13" t="e">
+      <c r="Z84" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="85" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z85" s="13" t="e">
+      <c r="Z85" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="86" spans="26:26" x14ac:dyDescent="0.25">
-      <c r="Z86" s="13" t="e">
+      <c r="Z86" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
     </row>
     <row r="87" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z87" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>                    .AddWithValue("@Height", value.Height, SqlDbType.Varchar(50))</v>
+        <v/>
       </c>
     </row>
     <row r="88" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z88" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>                    .AddWithValue("@Weight", value.Weight, SqlDbType.Varchar(50))</v>
+        <v/>
       </c>
     </row>
     <row r="89" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z89" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>                    .AddWithValue("@AlignmentId", value.AlignmentId, SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="90" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z90" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>                    .AddWithValue("@DeityId", value.DeityId, SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="91" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z91" s="13" t="str">
         <f t="shared" ref="Z91:Z95" si="23">IF(NOT(ISBLANK(B19)),"                    .AddWithValue(""@"&amp;B19&amp;""", value.Id,  SqlDbType.Int"&amp;")"&amp;IF(LEN(Z92)&gt;0,"",";"),"")</f>
-        <v>                    .AddWithValue("@InitiativeId", value.Id,  SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="92" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z92" s="13" t="str">
         <f t="shared" si="23"/>
-        <v>                    .AddWithValue("@AbilitySetId", value.Id,  SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="93" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z93" s="13" t="str">
         <f t="shared" si="23"/>
-        <v>                    .AddWithValue("@DefenseSetId", value.Id,  SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="94" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z94" s="13" t="str">
         <f t="shared" si="23"/>
-        <v>                    .AddWithValue("@MovementSetId", value.Id,  SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="95" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z95" s="13" t="str">
         <f t="shared" si="23"/>
-        <v>                    .AddWithValue("@SenseSetId", value.Id,  SqlDbType.Int)</v>
+        <v/>
       </c>
     </row>
     <row r="96" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z96" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z98" s="13" t="str">
         <f>"                return new DataResult&lt;"&amp;C2&amp;"&gt;(value, result);"</f>
-        <v>                return new DataResult&lt;PlayerCharacters&gt;(value, result);</v>
+        <v>                return new DataResult&lt;Deities&gt;(value, result);</v>
       </c>
     </row>
     <row r="99" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z99" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="100" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z100" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="101" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z101" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z102" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3358,9 +3152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP94"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3402,29 +3194,29 @@
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L1" s="9"/>
       <c r="M1" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N1" s="17"/>
       <c r="O1" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P1" s="10"/>
       <c r="Q1" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R1" s="11"/>
       <c r="S1" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Y1" s="7"/>
       <c r="Z1" s="7"/>
@@ -3450,37 +3242,37 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="J2" s="3" t="str">
         <f>A2&amp;" ["&amp;B2&amp;"].["&amp;C2&amp;"]"</f>
-        <v>CREATE TABLE [Client].[InvoiceSettings]</v>
+        <v>CREATE TABLE [dbo].[CompassionLevels]</v>
       </c>
       <c r="L2" s="4" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_CreateUpdate]"</f>
-        <v>CREATE PROCEDURE [Client].[USP_InvoiceSettings_CreateUpdate]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_CompassionLevels_CreateUpdate]</v>
       </c>
       <c r="N2" s="18" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Get]"</f>
-        <v>CREATE PROCEDURE [Client].[USP_InvoiceSettings_Get]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_CompassionLevels_Get]</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="X2" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
@@ -3511,23 +3303,23 @@
       </c>
       <c r="L3" s="4" t="str">
         <f>IF(NOT(ISBLANK(B4)),"@"&amp;B4&amp;" "&amp;UPPER(C4)&amp;" = NULL OUTPUT,","")</f>
-        <v>@InvoiceSettingsId INT = NULL OUTPUT,</v>
+        <v>@CompassionLevelId INT = NULL OUTPUT,</v>
       </c>
       <c r="N3" s="18" t="str">
         <f>"@"&amp;C2&amp;"Id"&amp;" INT"</f>
-        <v>@InvoiceSettingsId INT</v>
+        <v>@CompassionLevelsId INT</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T3" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="X3" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
@@ -3535,8 +3327,8 @@
         <v>0</v>
       </c>
       <c r="B4" s="14" t="str">
-        <f>C2&amp;"Id"</f>
-        <v>InvoiceSettingsId</v>
+        <f>LEFT(C2,LEN(C2)-1)&amp;"Id"</f>
+        <v>CompassionLevelId</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>6</v>
@@ -3551,38 +3343,38 @@
       <c r="H4" s="14"/>
       <c r="J4" s="3" t="str">
         <f>"    "&amp;B4&amp;" "&amp;UPPER(C4)&amp;IF(E4," NOT NULL","")&amp;IF(D4," IDENTITY(1,1)","")&amp;IF(NOT(ISBLANK(F4))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_PK PRIMARY KEY","")&amp;IF(LEN(G4)&gt;0," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_FK FOREIGN KEY REFERENCES "&amp;G4,"")&amp;IF(NOT(ISBLANK(H4))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_DF DEFAULT("&amp;H4&amp;")","")&amp;IF(NOT(ISBLANK(B5)),",","")</f>
-        <v xml:space="preserve">    InvoiceSettingsId INT IDENTITY(1,1) CONSTRAINT InvoiceSettings_InvoiceSettingsId_PK PRIMARY KEY,</v>
+        <v xml:space="preserve">    CompassionLevelId INT IDENTITY(1,1) CONSTRAINT CompassionLevels_CompassionLevelId_PK PRIMARY KEY,</v>
       </c>
       <c r="L4" s="4" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@Description VARCHAR(255)</v>
+        <v>@Name VARCHAR(50)</v>
       </c>
       <c r="N4" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T4" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V4" s="12" t="str">
         <f>"namespace Dots.Domain.Repositories."&amp;B2</f>
-        <v>namespace Dots.Domain.Repositories.Client</v>
+        <v>namespace Dots.Domain.Repositories.dbo</v>
       </c>
       <c r="X4" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="b">
@@ -3596,26 +3388,26 @@
       <c r="H5" s="2"/>
       <c r="J5" s="3" t="str">
         <f t="shared" ref="J5:J20" si="0">"    "&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(E5," NOT NULL","")&amp;IF(D5," IDENTITY(1,1)","")&amp;IF(NOT(ISBLANK(F5))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_PK PRIMARY KEY","")&amp;IF(LEN(G5)&gt;0," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_FK FOREIGN KEY REFERENCES "&amp;G5,"")&amp;IF(NOT(ISBLANK(H5))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_DF DEFAULT("&amp;H5&amp;")","")&amp;IF(NOT(ISBLANK(B6)),",","")</f>
-        <v xml:space="preserve">    Description VARCHAR(255) NOT NULL</v>
+        <v xml:space="preserve">    Name VARCHAR(50) NOT NULL</v>
       </c>
       <c r="L5" s="4" t="str">
         <f t="shared" ref="L5:L19" si="1">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;" "&amp;UPPER(C6)&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
         <v/>
       </c>
       <c r="P5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="T5" s="16" t="s">
         <v>12</v>
       </c>
       <c r="V5" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
@@ -3638,7 +3430,7 @@
         <v/>
       </c>
       <c r="N6" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>12</v>
@@ -3647,14 +3439,14 @@
         <v>12</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V6" s="12" t="str">
         <f>"    public interface I"&amp;C2&amp;"Repository"</f>
-        <v>    public interface IInvoiceSettingsRepository</v>
+        <v>    public interface ICompassionLevelsRepository</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.25">
@@ -3678,21 +3470,21 @@
       </c>
       <c r="N7" s="18" t="str">
         <f>IF(NOT(ISBLANK(B4)),"    ["&amp;B4&amp;"]"&amp;IF(LEN(N8)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">    [InvoiceSettingsId],</v>
+        <v xml:space="preserve">    [CompassionLevelId],</v>
       </c>
       <c r="P7" s="5" t="str">
         <f>"namespace Dots.Domain."&amp;B2</f>
-        <v>namespace Dots.Domain.Client</v>
+        <v>namespace Dots.Domain.dbo</v>
       </c>
       <c r="R7" s="6" t="str">
         <f>"namespace Dots.Domain."&amp;B2</f>
-        <v>namespace Dots.Domain.Client</v>
+        <v>namespace Dots.Domain.dbo</v>
       </c>
       <c r="T7" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="V7" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="X7" s="13" t="s">
         <v>12</v>
@@ -3719,25 +3511,25 @@
       </c>
       <c r="N8" s="18" t="str">
         <f t="shared" ref="N8:N22" si="3">IF(NOT(ISBLANK(B5)),"    ["&amp;B5&amp;"]"&amp;IF(LEN(N9)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">    [Description]</v>
+        <v xml:space="preserve">    [Name]</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="T8" s="16" t="str">
         <f>"    public static class "&amp;C2&amp;"Helper"</f>
-        <v>    public static class InvoiceSettingsHelper</v>
+        <v>    public static class CompassionLevelsHelper</v>
       </c>
       <c r="V8" s="12" t="str">
         <f>"        I"&amp;C2&amp;" Get(int "&amp;LOWER(C2)&amp;"Id);"</f>
-        <v>        IInvoiceSettings Get(int invoicesettingsId);</v>
+        <v>        ICompassionLevels Get(int compassionlevelsId);</v>
       </c>
       <c r="X8" s="13" t="str">
         <f>"namespace Dots.Domain.Repositories."&amp;B2</f>
-        <v>namespace Dots.Domain.Repositories.Client</v>
+        <v>namespace Dots.Domain.Repositories.dbo</v>
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.25">
@@ -3765,20 +3557,20 @@
       </c>
       <c r="P9" s="5" t="str">
         <f>"    public interface I"&amp;C2&amp;" : IEntity"</f>
-        <v>    public interface IInvoiceSettings : IEntity</v>
+        <v>    public interface ICompassionLevels : IEntity</v>
       </c>
       <c r="R9" s="6" t="str">
         <f>"    public class "&amp;C2&amp;" : I"&amp;C2</f>
-        <v>    public class InvoiceSettings : IInvoiceSettings</v>
+        <v>    public class CompassionLevels : ICompassionLevels</v>
       </c>
       <c r="T9" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="V9" s="12" t="s">
         <v>12</v>
       </c>
       <c r="X9" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
@@ -3805,22 +3597,22 @@
         <v/>
       </c>
       <c r="P10" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="T10" s="16" t="str">
         <f>"        public static I"&amp;C2&amp;" ParseReader(IDataReader reader)"</f>
-        <v>        public static IInvoiceSettings ParseReader(IDataReader reader)</v>
+        <v>        public static ICompassionLevels ParseReader(IDataReader reader)</v>
       </c>
       <c r="V10" s="12" t="str">
         <f>"        DataResult&lt;I"&amp;C2&amp;"&gt; Save(I"&amp;C2&amp;" "&amp;LOWER(C2)&amp;");"</f>
-        <v>        DataResult&lt;IInvoiceSettings&gt; Save(IInvoiceSettings invoicesettings);</v>
+        <v>        DataResult&lt;ICompassionLevels&gt; Save(ICompassionLevels compassionlevels);</v>
       </c>
       <c r="X10" s="13" t="str">
         <f>"    public class Sql"&amp;C2&amp;"Repository : Repository&lt;I"&amp;C2&amp;"&gt;, I"&amp;C2&amp;"Repository"</f>
-        <v>    public class SqlInvoiceSettingsRepository : Repository&lt;IInvoiceSettings&gt;, IInvoiceSettingsRepository</v>
+        <v>    public class SqlCompassionLevelsRepository : Repository&lt;ICompassionLevels&gt;, ICompassionLevelsRepository</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
@@ -3847,16 +3639,16 @@
         <v/>
       </c>
       <c r="R11" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="T11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="V11" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="V11" s="12" t="s">
-        <v>56</v>
-      </c>
       <c r="X11" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
@@ -3884,26 +3676,26 @@
       </c>
       <c r="O12" t="str">
         <f t="shared" ref="O12:O27" si="4">IF(NOT(ISBLANK(C5)),C5,"")</f>
-        <v>varchar(255)</v>
+        <v>varchar(50)</v>
       </c>
       <c r="P12" s="5" t="str">
         <f t="shared" ref="P12:P27" si="5">IF(NOT(ISBLANK(C5)),"        "&amp;IF(ISBLANK(Q12),C5,Q12)&amp;" "&amp;B5&amp;" { get; set; }","")</f>
-        <v xml:space="preserve">        varchar(255) Description { get; set; }</v>
+        <v xml:space="preserve">        varchar(50) Name { get; set; }</v>
       </c>
       <c r="R12" s="6" t="str">
         <f t="shared" ref="R12:R27" si="6">IF(LEN(P12)&gt;0,"        public "&amp;TRIM(P12),"")</f>
-        <v xml:space="preserve">        public varchar(255) Description { get; set; }</v>
+        <v xml:space="preserve">        public varchar(50) Name { get; set; }</v>
       </c>
       <c r="T12" s="16" t="str">
         <f>"            return new "&amp;C2&amp;"("</f>
-        <v>            return new InvoiceSettings(</v>
+        <v>            return new CompassionLevels(</v>
       </c>
       <c r="V12" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X12" s="13" t="str">
         <f>"        public Sql"&amp;C2&amp;"Repository(IUnitOfWork unitOfWork)"</f>
-        <v>        public SqlInvoiceSettingsRepository(IUnitOfWork unitOfWork)</v>
+        <v>        public SqlCompassionLevelsRepository(IUnitOfWork unitOfWork)</v>
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
@@ -3943,10 +3735,10 @@
       </c>
       <c r="T13" s="16" t="str">
         <f>"                reader.Get&lt;int&gt;("&amp;C2&amp;"Col.Id),"</f>
-        <v xml:space="preserve">                reader.Get&lt;int&gt;(InvoiceSettingsCol.Id),</v>
+        <v xml:space="preserve">                reader.Get&lt;int&gt;(CompassionLevelsCol.Id),</v>
       </c>
       <c r="X13" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
@@ -3989,7 +3781,7 @@
         <v/>
       </c>
       <c r="X14" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.25">
@@ -4032,7 +3824,7 @@
         <v/>
       </c>
       <c r="X15" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
@@ -4116,7 +3908,7 @@
       </c>
       <c r="X17" s="13" t="str">
         <f>"        protected override I"&amp;C2&amp;" Map(IDataReader reader)"</f>
-        <v xml:space="preserve">        protected override IInvoiceSettings Map(IDataReader reader)</v>
+        <v xml:space="preserve">        protected override ICompassionLevels Map(IDataReader reader)</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
@@ -4159,7 +3951,7 @@
         <v/>
       </c>
       <c r="X18" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
@@ -4203,7 +3995,7 @@
       </c>
       <c r="X19" s="13" t="str">
         <f>"           return "&amp;C2&amp;"Helper.ParseReader(reader);"</f>
-        <v>           return InvoiceSettingsHelper.ParseReader(reader);</v>
+        <v>           return CompassionLevelsHelper.ParseReader(reader);</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
@@ -4222,7 +4014,7 @@
         <v xml:space="preserve">     </v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N20" s="18" t="str">
         <f t="shared" si="3"/>
@@ -4245,7 +4037,7 @@
         <v/>
       </c>
       <c r="X20" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
@@ -4279,7 +4071,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L22" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N22" s="18" t="str">
         <f t="shared" si="3"/>
@@ -4303,7 +4095,7 @@
       </c>
       <c r="X22" s="13" t="str">
         <f>"        public I"&amp;C2&amp;" Get(int "&amp;LOWER(C2)&amp;"Id)"</f>
-        <v>        public IInvoiceSettings Get(int invoicesettingsId)</v>
+        <v>        public ICompassionLevels Get(int compassionlevelsId)</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
@@ -4316,7 +4108,7 @@
       </c>
       <c r="L23" s="4" t="str">
         <f>"SELECT "&amp;B4</f>
-        <v>SELECT InvoiceSettingsId</v>
+        <v>SELECT CompassionLevelId</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="4"/>
@@ -4335,16 +4127,16 @@
         <v/>
       </c>
       <c r="X23" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L24" s="4" t="str">
         <f>"FROM "&amp;B2&amp;"."&amp;C2</f>
-        <v>FROM Client.InvoiceSettings</v>
+        <v>FROM dbo.CompassionLevels</v>
       </c>
       <c r="N24" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="4"/>
@@ -4364,7 +4156,7 @@
       </c>
       <c r="X24" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Get""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("Client.USP_InvoiceSettings_Get"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_CompassionLevels_Get"))</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
@@ -4373,22 +4165,22 @@
       </c>
       <c r="B25" t="str">
         <f>B2</f>
-        <v>Client</v>
+        <v>dbo</v>
       </c>
       <c r="C25" t="str">
         <f>"Trigger_"&amp;C2&amp;"_AuditData"</f>
-        <v>Trigger_InvoiceSettings_AuditData</v>
+        <v>Trigger_CompassionLevels_AuditData</v>
       </c>
       <c r="J25" s="3" t="str">
         <f>A25&amp;" ["&amp;B25&amp;"].["&amp;C25&amp;"] ON ["&amp;B2&amp;"].["&amp;C2&amp;"]"</f>
-        <v>CREATE TRIGGER [Client].[Trigger_InvoiceSettings_AuditData] ON [Client].[InvoiceSettings]</v>
+        <v>CREATE TRIGGER [dbo].[Trigger_CompassionLevels_AuditData] ON [dbo].[CompassionLevels]</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N25" s="18" t="str">
         <f>"    "&amp;B2&amp;"."&amp;C2</f>
-        <v xml:space="preserve">    Client.InvoiceSettings</v>
+        <v xml:space="preserve">    dbo.CompassionLevels</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="4"/>
@@ -4407,7 +4199,7 @@
         <v/>
       </c>
       <c r="X25" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
@@ -4420,10 +4212,10 @@
       </c>
       <c r="L26" s="4" t="str">
         <f>IF(NOT(ISBLANK(B4)),"["&amp;B4&amp;"] = ISNULL(@"&amp;B4&amp;", 0)","")</f>
-        <v>[InvoiceSettingsId] = ISNULL(@InvoiceSettingsId, 0)</v>
+        <v>[CompassionLevelId] = ISNULL(@CompassionLevelId, 0)</v>
       </c>
       <c r="N26" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="4"/>
@@ -4442,7 +4234,7 @@
         <v/>
       </c>
       <c r="X26" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
@@ -4454,11 +4246,11 @@
         <v>BEGIN</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N27" s="18" t="str">
         <f>"    "&amp;B4&amp;" = @"&amp;B4</f>
-        <v xml:space="preserve">    InvoiceSettingsId = @InvoiceSettingsId</v>
+        <v xml:space="preserve">    CompassionLevelId = @CompassionLevelId</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="4"/>
@@ -4478,7 +4270,7 @@
       </c>
       <c r="X27" s="13" t="str">
         <f>"                    .AddWithValue(""@"&amp;C2&amp;"Id"", "&amp;LOWER(C2)&amp;"Id, DbType.Int32);"</f>
-        <v>                    .AddWithValue("@InvoiceSettingsId", invoicesettingsId, DbType.Int32);</v>
+        <v>                    .AddWithValue("@CompassionLevelsId", compassionlevelsId, DbType.Int32);</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
@@ -4493,7 +4285,7 @@
         <v>11</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T28" s="16" t="str">
         <f t="shared" si="7"/>
@@ -4510,21 +4302,21 @@
       </c>
       <c r="L29" s="4" t="str">
         <f>"INSERT INTO "&amp;B2&amp;"."&amp;C2&amp;" ("</f>
-        <v>INSERT INTO Client.InvoiceSettings (</v>
+        <v>INSERT INTO dbo.CompassionLevels (</v>
       </c>
       <c r="P29" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R29" s="6" t="str">
         <f>"        public "&amp;C2&amp;"("</f>
-        <v>        public InvoiceSettings(</v>
+        <v>        public CompassionLevels(</v>
       </c>
       <c r="T29" s="16" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="X29" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
@@ -4537,14 +4329,14 @@
       </c>
       <c r="L30" s="4" t="str">
         <f>IF(NOT(ISBLANK(B5)),"["&amp;B5&amp;"]"&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>[Description]</v>
+        <v>[Name]</v>
       </c>
       <c r="R30" s="6" t="str">
         <f>IF(NOT(ISBLANK(B4)),"            int"&amp;" "&amp;LOWER(LEFT(B4,1))&amp;MID(B4,2,LEN(B4)-1)&amp;IF(LEN(R31)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            int invoiceSettingsId,</v>
+        <v xml:space="preserve">            int compassionLevelId,</v>
       </c>
       <c r="X30" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
@@ -4561,13 +4353,13 @@
       </c>
       <c r="R31" s="6" t="str">
         <f t="shared" ref="R31:R46" si="11">IF(NOT(ISBLANK(B5)),"            "&amp;Q12&amp;" "&amp;LOWER(LEFT(B5,1))&amp;MID(B5,2,LEN(B5)-1)&amp;IF(LEN(R32)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">             description</v>
+        <v xml:space="preserve">             name</v>
       </c>
       <c r="T31" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="X31" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
@@ -4587,7 +4379,7 @@
         <v/>
       </c>
       <c r="T32" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
@@ -4611,7 +4403,7 @@
       </c>
       <c r="X33" s="13" t="str">
         <f>"        public DataResult&lt;I"&amp;C2&amp;"&gt; Save(I"&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;IInvoiceSettings&gt; Save(IInvoiceSettings value)</v>
+        <v xml:space="preserve">        public DataResult&lt;ICompassionLevels&gt; Save(ICompassionLevels value)</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
@@ -4632,10 +4424,10 @@
       </c>
       <c r="T34" s="16" t="str">
         <f>"        public static IEnumerable&lt;I"&amp;C2&amp;"&gt; ParseMultipleReader(IDataReader reader)"</f>
-        <v>        public static IEnumerable&lt;IInvoiceSettings&gt; ParseMultipleReader(IDataReader reader)</v>
+        <v>        public static IEnumerable&lt;ICompassionLevels&gt; ParseMultipleReader(IDataReader reader)</v>
       </c>
       <c r="X34" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
@@ -4655,21 +4447,21 @@
         <v/>
       </c>
       <c r="T35" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X35" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Save""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("Client.USP_InvoiceSettings_Save"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_CompassionLevels_Save"))</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>"        INSERT ["&amp;B$2&amp;"].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)"</f>
-        <v xml:space="preserve">        INSERT [Client].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
+        <v xml:space="preserve">        INSERT [dbo].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
       </c>
       <c r="J36" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">        INSERT [Client].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
+        <v xml:space="preserve">        INSERT [dbo].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
       </c>
       <c r="L36" s="4" t="str">
         <f t="shared" si="10"/>
@@ -4681,20 +4473,20 @@
       </c>
       <c r="T36" s="16" t="str">
         <f>"            var "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;"s = new List&lt;I"&amp;C2&amp;"&gt;();"</f>
-        <v>            var invoiceSettingss = new List&lt;IInvoiceSettings&gt;();</v>
+        <v>            var compassionLevelss = new List&lt;ICompassionLevels&gt;();</v>
       </c>
       <c r="X36" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>"        SELECT 'INSERT', @Token, '["&amp;B$2&amp;"]', '["&amp;C$2&amp;"]', P."&amp;B$4&amp;", DATA = ("</f>
-        <v xml:space="preserve">        SELECT 'INSERT', @Token, '[Client]', '[InvoiceSettings]', P.InvoiceSettingsId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'INSERT', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
       </c>
       <c r="J37" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">        SELECT 'INSERT', @Token, '[Client]', '[InvoiceSettings]', P.InvoiceSettingsId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'INSERT', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
       </c>
       <c r="L37" s="4" t="str">
         <f t="shared" si="10"/>
@@ -4709,7 +4501,7 @@
       </c>
       <c r="X37" s="13" t="str">
         <f>"                var idParameter = command.AddOutput(""@"&amp;C2&amp;"Id"", DbType.Int32);"</f>
-        <v>                var idParameter = command.AddOutput("@InvoiceSettingsId", DbType.Int32);</v>
+        <v>                var idParameter = command.AddOutput("@CompassionLevelsId", DbType.Int32);</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
@@ -4729,10 +4521,10 @@
         <v/>
       </c>
       <c r="T38" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X38" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
@@ -4752,21 +4544,21 @@
         <v/>
       </c>
       <c r="T39" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="X39" s="13" t="str">
         <f>IF(NOT(ISBLANK(B4)),"                    .AddWithValue(""@"&amp;B4&amp;""", value.Id, DbType.Int32"&amp;")"&amp;IF(LEN(X40)&gt;0,"",";"),"")</f>
-        <v>                    .AddWithValue("@InvoiceSettingsId", value.Id, DbType.Int32)</v>
+        <v>                    .AddWithValue("@CompassionLevelId", value.Id, DbType.Int32)</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>"                WHERE Record."&amp;B$4&amp;" = P."&amp;B$4</f>
-        <v xml:space="preserve">                WHERE Record.InvoiceSettingsId = P.InvoiceSettingsId</v>
+        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
       </c>
       <c r="J40" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">                WHERE Record.InvoiceSettingsId = P.InvoiceSettingsId</v>
+        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
       </c>
       <c r="L40" s="4" t="str">
         <f t="shared" si="10"/>
@@ -4778,11 +4570,11 @@
       </c>
       <c r="T40" s="16" t="str">
         <f>"                "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;"s.Add(ParseReader(reader));"</f>
-        <v>                invoiceSettingss.Add(ParseReader(reader));</v>
+        <v>                compassionLevelss.Add(ParseReader(reader));</v>
       </c>
       <c r="X40" s="13" t="str">
         <f t="shared" ref="X40:X55" si="12">IF(NOT(ISBLANK(B5)),"                    .AddWithValue(""@"&amp;B5&amp;""", value."&amp;B5&amp;", DbType."&amp;IF(NOT(OR(ISBLANK(Q12),Q12="int")),UPPER(LEFT(Q12,1))&amp;MID(Q12,2,LEN(Q12)-1),"Int32")&amp;")"&amp;IF(LEFT(X41,24)="                    .Add","",";"),"")</f>
-        <v>                    .AddWithValue("@Description", value.Description, DbType.Int32);</v>
+        <v>                    .AddWithValue("@Name", value.Name, DbType.Int32);</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
@@ -4802,7 +4594,7 @@
         <v/>
       </c>
       <c r="T41" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="X41" s="13" t="str">
         <f t="shared" si="12"/>
@@ -4851,7 +4643,7 @@
       </c>
       <c r="T43" s="16" t="str">
         <f>"            return "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;"s;"</f>
-        <v>            return invoiceSettingss;</v>
+        <v>            return compassionLevelss;</v>
       </c>
       <c r="X43" s="13" t="str">
         <f t="shared" si="12"/>
@@ -4875,7 +4667,7 @@
         <v/>
       </c>
       <c r="T44" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X44" s="13" t="str">
         <f t="shared" si="12"/>
@@ -4915,7 +4707,7 @@
         <v>    </v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R46" s="6" t="str">
         <f t="shared" si="11"/>
@@ -4923,7 +4715,7 @@
       </c>
       <c r="T46" s="16" t="str">
         <f>"        private enum "&amp;C2&amp;"Col"</f>
-        <v>        private enum InvoiceSettingsCol</v>
+        <v>        private enum CompassionLevelsCol</v>
       </c>
       <c r="X46" s="13" t="str">
         <f t="shared" si="12"/>
@@ -4939,13 +4731,13 @@
         <v xml:space="preserve">        -- Detect deletes</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R47" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T47" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X47" s="13" t="str">
         <f t="shared" si="12"/>
@@ -4962,13 +4754,13 @@
       </c>
       <c r="L48" s="4" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@Description</v>
+        <v>@Name</v>
       </c>
       <c r="R48" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T48" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X48" s="13" t="str">
         <f t="shared" si="12"/>
@@ -4989,11 +4781,11 @@
       </c>
       <c r="R49" s="6" t="str">
         <f>IF(NOT(ISBLANK(B4)),"            Id = "&amp;LOWER(LEFT(B4,1))&amp;MID(B4,2,LEN(B4)-1)&amp;";","")</f>
-        <v xml:space="preserve">            Id = invoiceSettingsId;</v>
+        <v xml:space="preserve">            Id = compassionLevelId;</v>
       </c>
       <c r="T49" s="16" t="str">
         <f t="shared" ref="T49:T64" si="14">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;IF(LEN(T15)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            Description</v>
+        <v xml:space="preserve">            Name</v>
       </c>
       <c r="X49" s="13" t="str">
         <f t="shared" si="12"/>
@@ -5003,11 +4795,11 @@
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>"        INSERT ["&amp;B$2&amp;"].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)"</f>
-        <v xml:space="preserve">        INSERT [Client].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
+        <v xml:space="preserve">        INSERT [dbo].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
       </c>
       <c r="J50" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">        INSERT [Client].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
+        <v xml:space="preserve">        INSERT [dbo].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
       </c>
       <c r="L50" s="4" t="str">
         <f t="shared" si="13"/>
@@ -5015,7 +4807,7 @@
       </c>
       <c r="R50" s="6" t="str">
         <f t="shared" ref="R50:R65" si="15">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;" = "&amp;LOWER(LEFT(B5,1))&amp;MID(B5,2,LEN(B5)-1)&amp;";","")</f>
-        <v xml:space="preserve">            Description = description;</v>
+        <v xml:space="preserve">            Name = name;</v>
       </c>
       <c r="T50" s="16" t="str">
         <f t="shared" si="14"/>
@@ -5029,11 +4821,11 @@
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>"        SELECT 'DELETE', @Token, '["&amp;B$2&amp;"]', '["&amp;C$2&amp;"]', P."&amp;B$4&amp;", DATA = ("</f>
-        <v xml:space="preserve">        SELECT 'DELETE', @Token, '[Client]', '[InvoiceSettings]', P.InvoiceSettingsId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'DELETE', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
       </c>
       <c r="J51" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">        SELECT 'DELETE', @Token, '[Client]', '[InvoiceSettings]', P.InvoiceSettingsId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'DELETE', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
       </c>
       <c r="L51" s="4" t="str">
         <f>IF(NOT(ISBLANK(B8)),"@"&amp;B8&amp;IF(NOT(ISBLANK(B9)),",",""),"")</f>
@@ -5105,11 +4897,11 @@
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>"                WHERE Record."&amp;B$4&amp;" = P."&amp;B$4</f>
-        <v xml:space="preserve">                WHERE Record.InvoiceSettingsId = P.InvoiceSettingsId</v>
+        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
       </c>
       <c r="J54" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">                WHERE Record.InvoiceSettingsId = P.InvoiceSettingsId</v>
+        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
       </c>
       <c r="L54" s="4" t="str">
         <f t="shared" si="13"/>
@@ -5195,7 +4987,7 @@
         <v/>
       </c>
       <c r="X57" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
@@ -5219,7 +5011,7 @@
         <v/>
       </c>
       <c r="X58" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
@@ -5243,7 +5035,7 @@
         <v/>
       </c>
       <c r="X59" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
@@ -5267,7 +5059,7 @@
         <v/>
       </c>
       <c r="X60" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
@@ -5291,7 +5083,7 @@
         <v/>
       </c>
       <c r="X61" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
@@ -5336,20 +5128,20 @@
         <v/>
       </c>
       <c r="X63" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>"        INSERT ["&amp;B$2&amp;"].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)"</f>
-        <v xml:space="preserve">        INSERT [Client].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
+        <v xml:space="preserve">        INSERT [dbo].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
       </c>
       <c r="J64" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">        INSERT [Client].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
+        <v xml:space="preserve">        INSERT [dbo].[AuditData] (ChangeType, ChangeToken, SchemaName, ObjectName, RecordId, Record)</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R64" s="6" t="str">
         <f t="shared" si="15"/>
@@ -5360,27 +5152,27 @@
         <v/>
       </c>
       <c r="X64" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>"        SELECT 'UPDATE', @Token, '["&amp;B$2&amp;"]', '["&amp;C$2&amp;"]', P."&amp;B$4&amp;", DATA = ("</f>
-        <v xml:space="preserve">        SELECT 'UPDATE', @Token, '[Client]', '[InvoiceSettings]', P.InvoiceSettingsId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'UPDATE', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
       </c>
       <c r="J65" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">        SELECT 'UPDATE', @Token, '[Client]', '[InvoiceSettings]', P.InvoiceSettingsId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'UPDATE', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
       </c>
       <c r="R65" s="6" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="T65" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X65" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
@@ -5393,13 +5185,13 @@
       </c>
       <c r="L66" s="4" t="str">
         <f>"SELECT @"&amp;B4&amp;" = SCOPE_IDENTITY()"</f>
-        <v>SELECT @InvoiceSettingsId = SCOPE_IDENTITY()</v>
+        <v>SELECT @CompassionLevelId = SCOPE_IDENTITY()</v>
       </c>
       <c r="T66" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="X66" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
@@ -5411,29 +5203,29 @@
         <v xml:space="preserve">                FROM inserted Record</v>
       </c>
       <c r="R67" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="T67" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="T67" s="16" t="s">
-        <v>57</v>
-      </c>
       <c r="X67" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>"                WHERE Record."&amp;B$4&amp;" = P."&amp;B$4</f>
-        <v xml:space="preserve">                WHERE Record.InvoiceSettingsId = P.InvoiceSettingsId</v>
+        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
       </c>
       <c r="J68" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">                WHERE Record.InvoiceSettingsId = P.InvoiceSettingsId</v>
+        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="R68" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
@@ -5448,7 +5240,7 @@
         <v>14</v>
       </c>
       <c r="R69" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
@@ -5460,7 +5252,7 @@
         <v xml:space="preserve">                )</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
@@ -5485,7 +5277,7 @@
       </c>
       <c r="L72" s="4" t="str">
         <f>"UPDATE "&amp;B2&amp;"."&amp;C2</f>
-        <v>UPDATE Client.InvoiceSettings</v>
+        <v>UPDATE dbo.CompassionLevels</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
@@ -5497,7 +5289,7 @@
         <v xml:space="preserve">        END</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.25">
@@ -5510,7 +5302,7 @@
       </c>
       <c r="L74" s="4" t="str">
         <f t="shared" ref="L74:L89" si="16">IF(AND(NOT(ISBLANK(B5)),ISERROR(FIND("Id",B5))),"["&amp;B5&amp;"] = @"&amp;B5&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>[Description] = @Description</v>
+        <v>[Name] = @Name</v>
       </c>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.25">
@@ -5605,18 +5397,18 @@
     </row>
     <row r="90" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L90" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="91" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L91" s="4" t="str">
         <f>"["&amp;B4&amp;"] = @"&amp;B4</f>
-        <v>[InvoiceSettingsId] = @InvoiceSettingsId</v>
+        <v>[CompassionLevelId] = @CompassionLevelId</v>
       </c>
     </row>
     <row r="93" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L93" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="12:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added map areas and shops.
</commit_message>
<xml_diff>
--- a/Table Creator.xlsx
+++ b/Table Creator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew\Dropbox\Programming Projects\C#\DungeonsAndDragons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\PersonalProjects\DungeonsAndDragons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="117">
   <si>
     <t>Fields</t>
   </si>
@@ -315,12 +315,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>CurrencyType</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
     <t xml:space="preserve">            return !value.Id.HasValue ? Create(value) : Update(value);</t>
   </si>
   <si>
@@ -336,15 +330,6 @@
     <t>                var result = ExecuteNonQuery(command);</t>
   </si>
   <si>
-    <t>InvoiceLayoutType</t>
-  </si>
-  <si>
-    <t>TimeFrequency</t>
-  </si>
-  <si>
-    <t>CommunicationType</t>
-  </si>
-  <si>
     <t>dbo</t>
   </si>
   <si>
@@ -354,25 +339,43 @@
     <t>varchar(50)</t>
   </si>
   <si>
-    <t>DeityId</t>
-  </si>
-  <si>
-    <t>CompassionLevels</t>
-  </si>
-  <si>
-    <t>Deities</t>
-  </si>
-  <si>
-    <t>AuthorityLevelId</t>
-  </si>
-  <si>
-    <t>CompassionLevelId</t>
-  </si>
-  <si>
     <t>FlavourText</t>
   </si>
   <si>
     <t>varchar(MAX)</t>
+  </si>
+  <si>
+    <t>MapAreaTypes</t>
+  </si>
+  <si>
+    <t>ParentMapAreaId</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>ParentMapAreaLocationN</t>
+  </si>
+  <si>
+    <t>ParentMapAreaLocationW</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>ShopId</t>
+  </si>
+  <si>
+    <t>MapImage</t>
+  </si>
+  <si>
+    <t>Shops</t>
+  </si>
+  <si>
+    <t>OwnerActorId</t>
+  </si>
+  <si>
+    <t>CostModifier</t>
   </si>
 </sst>
 </file>
@@ -816,7 +819,7 @@
   <dimension ref="A1:AR102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,26 +916,26 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="J2" s="3" t="str">
         <f>A2&amp;" ["&amp;B2&amp;"].["&amp;C2&amp;"]"</f>
-        <v>CREATE TABLE [dbo].[Deities]</v>
+        <v>CREATE TABLE [dbo].[Shops]</v>
       </c>
       <c r="L2" s="22" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Create]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_Deities_Create]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_Shops_Create]</v>
       </c>
       <c r="N2" s="23" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Update]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_Deities_Update]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_Shops_Update]</v>
       </c>
       <c r="P2" s="18" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Get]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_Deities_Get]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_Shops_Get]</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>46</v>
@@ -954,9 +957,6 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>109</v>
-      </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
@@ -981,15 +981,15 @@
       </c>
       <c r="L3" s="22" t="str">
         <f>IF(NOT(ISBLANK(B4)),"@"&amp;B4&amp;" "&amp;UPPER(C4)&amp;" = NULL OUTPUT,","")</f>
-        <v>@DeityId INT = NULL OUTPUT,</v>
+        <v>@ShopId INT = NULL OUTPUT,</v>
       </c>
       <c r="N3" s="23" t="str">
         <f>IF(NOT(ISBLANK(B4)),"@"&amp;B4&amp;" "&amp;UPPER(C4)&amp;",","")</f>
-        <v>@DeityId INT,</v>
+        <v>@ShopId INT,</v>
       </c>
       <c r="P3" s="18" t="str">
         <f>"@"&amp;C2&amp;"Id"&amp;" INT"</f>
-        <v>@DeitiesId INT</v>
+        <v>@ShopsId INT</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>47</v>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B4" s="14" t="str">
         <f>IF(NOT(ISBLANK(B3)),B3,LEFT(C2,LEN(C2)-1)&amp;"Id")</f>
-        <v>DeityId</v>
+        <v>ShopId</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>6</v>
@@ -1025,15 +1025,15 @@
       <c r="H4" s="14"/>
       <c r="J4" s="3" t="str">
         <f>"    "&amp;B4&amp;" "&amp;UPPER(C4)&amp;IF(E4," NOT NULL","")&amp;IF(D4," IDENTITY(1,1)","")&amp;IF(NOT(ISBLANK(F4))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_PK PRIMARY KEY","")&amp;IF(LEN(G4)&gt;0," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_FK FOREIGN KEY REFERENCES "&amp;G4,"")&amp;IF(NOT(ISBLANK(H4))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_DF DEFAULT("&amp;H4&amp;")","")&amp;IF(NOT(ISBLANK(B5)),",","")</f>
-        <v xml:space="preserve">    DeityId INT IDENTITY(1,1) CONSTRAINT Deities_DeityId_PK PRIMARY KEY,</v>
+        <v xml:space="preserve">    ShopId INT IDENTITY(1,1) CONSTRAINT Shops_ShopId_PK PRIMARY KEY,</v>
       </c>
       <c r="L4" s="22" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@AuthorityLevelId INT,</v>
+        <v>@OwnerActorId INT,</v>
       </c>
       <c r="N4" s="23" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@AuthorityLevelId INT,</v>
+        <v>@OwnerActorId INT,</v>
       </c>
       <c r="P4" s="18" t="s">
         <v>38</v>
@@ -1057,30 +1057,32 @@
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" t="str">
-        <f>IF(UPPER(RIGHT(B5,2))="ID",B$2&amp;"."&amp;LEFT(B5,LEN(B5)-2)&amp;"("&amp;B5&amp;")","")</f>
-        <v>dbo.AuthorityLevel(AuthorityLevelId)</v>
+        <f>IF(UPPER(RIGHT(B5,2))="ID",B$2&amp;"."&amp;LEFT(B5,LEN(B5)-2)&amp;"s("&amp;B5&amp;")","")</f>
+        <v>dbo.OwnerActors(OwnerActorId)</v>
       </c>
       <c r="H5" s="19"/>
       <c r="J5" s="3" t="str">
         <f t="shared" ref="J5:J32" si="0">"    "&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(E5," NOT NULL","")&amp;IF(D5," IDENTITY(1,1)","")&amp;IF(NOT(ISBLANK(F5))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_PK PRIMARY KEY","")&amp;IF(LEN(G5)&gt;0," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_FK FOREIGN KEY REFERENCES "&amp;G5,"")&amp;IF(NOT(ISBLANK(H5))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_DF DEFAULT("&amp;H5&amp;")","")&amp;IF(NOT(ISBLANK(B6)),",","")</f>
-        <v xml:space="preserve">    AuthorityLevelId INT CONSTRAINT Deities_AuthorityLevelId_FK FOREIGN KEY REFERENCES dbo.AuthorityLevel(AuthorityLevelId),</v>
+        <v xml:space="preserve">    OwnerActorId INT NOT NULL CONSTRAINT Shops_OwnerActorId_FK FOREIGN KEY REFERENCES dbo.OwnerActors(OwnerActorId),</v>
       </c>
       <c r="L5" s="22" t="str">
         <f t="shared" ref="L5:L19" si="1">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;" "&amp;UPPER(C6)&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>@CompassionLevelId INT,</v>
+        <v>@CostModifier DECIMAL,</v>
       </c>
       <c r="N5" s="23" t="str">
         <f t="shared" ref="N5:N19" si="2">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;" "&amp;UPPER(C6)&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>@CompassionLevelId INT,</v>
+        <v>@CostModifier DECIMAL,</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>49</v>
@@ -1100,30 +1102,34 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" t="str">
-        <f t="shared" ref="G6" si="3">IF(UPPER(RIGHT(B6,2))="ID",B$2&amp;"."&amp;LEFT(B6,LEN(B6)-2)&amp;"("&amp;B6&amp;")","")</f>
-        <v>dbo.CompassionLevel(CompassionLevelId)</v>
-      </c>
-      <c r="H6" s="19"/>
+        <f t="shared" ref="G6:G32" si="3">IF(UPPER(RIGHT(B6,2))="ID",B$2&amp;"."&amp;LEFT(B6,LEN(B6)-2)&amp;"s("&amp;B6&amp;")","")</f>
+        <v/>
+      </c>
+      <c r="H6" s="19">
+        <v>1</v>
+      </c>
       <c r="J6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    CompassionLevelId INT CONSTRAINT Deities_CompassionLevelId_FK FOREIGN KEY REFERENCES dbo.CompassionLevel(CompassionLevelId),</v>
+        <v xml:space="preserve">    CostModifier DECIMAL NOT NULL CONSTRAINT Shops_CostModifier_DF DEFAULT(1),</v>
       </c>
       <c r="L6" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>@FlavourText VARCHAR(MAX)</v>
+        <v>@FlavourText VARCHAR(MAX),</v>
       </c>
       <c r="N6" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>@FlavourText VARCHAR(MAX)</v>
+        <v>@FlavourText VARCHAR(MAX),</v>
       </c>
       <c r="P6" s="18" t="s">
         <v>89</v>
@@ -1140,7 +1146,7 @@
       </c>
       <c r="X6" s="12" t="str">
         <f>"    public interface I"&amp;C2&amp;"Repository"</f>
-        <v>    public interface IDeitiesRepository</v>
+        <v>    public interface IShopsRepository</v>
       </c>
       <c r="Z6" s="13" t="s">
         <v>67</v>
@@ -1148,34 +1154,34 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" t="str">
-        <f t="shared" ref="G7:G20" si="4">IF(UPPER(RIGHT(B7,2))="ID",B$2&amp;"."&amp;LEFT(B7,LEN(B7)-2)&amp;"("&amp;B7&amp;")","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H7" s="2"/>
       <c r="J7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    FlavourText VARCHAR(MAX)</v>
+        <v xml:space="preserve">    FlavourText VARCHAR(MAX),</v>
       </c>
       <c r="L7" s="22" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>@ShopId INT,</v>
       </c>
       <c r="N7" s="23" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>@ShopId INT,</v>
       </c>
       <c r="P7" s="18" t="str">
         <f>IF(NOT(ISBLANK(B4)),"    ["&amp;B4&amp;"]"&amp;IF(LEN(P8)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">    [DeityId],</v>
+        <v xml:space="preserve">    [ShopId],</v>
       </c>
       <c r="R7" s="5" t="str">
         <f>"namespace Dots.Domain."&amp;B2</f>
@@ -1196,31 +1202,35 @@
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>dbo.Shops(ShopId)</v>
       </c>
       <c r="H8" s="2"/>
       <c r="J8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     </v>
+        <v xml:space="preserve">    ShopId INT CONSTRAINT Shops_ShopId_FK FOREIGN KEY REFERENCES dbo.Shops(ShopId),</v>
       </c>
       <c r="L8" s="22" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>@MapImage BINARY,</v>
       </c>
       <c r="N8" s="23" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>@MapImage BINARY,</v>
       </c>
       <c r="P8" s="18" t="str">
-        <f t="shared" ref="P8:P22" si="5">IF(NOT(ISBLANK(B5)),"    ["&amp;B5&amp;"]"&amp;IF(LEN(P9)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">    [AuthorityLevelId],</v>
+        <f t="shared" ref="P8:P22" si="4">IF(NOT(ISBLANK(B5)),"    ["&amp;B5&amp;"]"&amp;IF(LEN(P9)&gt;0,",",""),"")</f>
+        <v xml:space="preserve">    [OwnerActorId],</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>50</v>
@@ -1230,11 +1240,11 @@
       </c>
       <c r="V8" s="16" t="str">
         <f>"    public static class "&amp;C2&amp;"Helper"</f>
-        <v>    public static class DeitiesHelper</v>
+        <v>    public static class ShopsHelper</v>
       </c>
       <c r="X8" s="12" t="str">
         <f>"        "&amp;C2&amp;" Get(int "&amp;LOWER(C2)&amp;"Id);"</f>
-        <v>        Deities Get(int deitiesId);</v>
+        <v>        Shops Get(int shopsId);</v>
       </c>
       <c r="Z8" s="13" t="str">
         <f>"namespace Dots.Domain.Repositories."&amp;B2&amp;"s"</f>
@@ -1242,39 +1252,43 @@
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H9" s="2"/>
       <c r="J9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     </v>
+        <v xml:space="preserve">    MapImage BINARY,</v>
       </c>
       <c r="L9" s="22" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>@ParentMapAreaId INT,</v>
       </c>
       <c r="N9" s="23" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>@ParentMapAreaId INT,</v>
       </c>
       <c r="P9" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    [CompassionLevelId],</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">    [CostModifier],</v>
       </c>
       <c r="R9" s="5" t="str">
         <f>"    public interface I"&amp;C2&amp;" : IEntity"</f>
-        <v>    public interface IDeities : IEntity</v>
+        <v>    public interface IShops : IEntity</v>
       </c>
       <c r="T9" s="6" t="str">
         <f>"    public class "&amp;C2&amp;" : IEntity"</f>
-        <v>    public class Deities : IEntity</v>
+        <v>    public class Shops : IEntity</v>
       </c>
       <c r="V9" s="16" t="s">
         <v>51</v>
@@ -1287,31 +1301,35 @@
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>dbo.ParentMapAreas(ParentMapAreaId)</v>
       </c>
       <c r="H10" s="19"/>
       <c r="J10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     </v>
+        <v xml:space="preserve">    ParentMapAreaId INT CONSTRAINT Shops_ParentMapAreaId_FK FOREIGN KEY REFERENCES dbo.ParentMapAreas(ParentMapAreaId),</v>
       </c>
       <c r="L10" s="22" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>@ParentMapAreaLocationN DECIMAL,</v>
       </c>
       <c r="N10" s="23" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>@ParentMapAreaLocationN DECIMAL,</v>
       </c>
       <c r="P10" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">    [FlavourText]</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">    [FlavourText],</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>51</v>
@@ -1321,43 +1339,47 @@
       </c>
       <c r="V10" s="16" t="str">
         <f>"        public static "&amp;C2&amp;" ParseReader(IDataReader reader)"</f>
-        <v>        public static Deities ParseReader(IDataReader reader)</v>
+        <v>        public static Shops ParseReader(IDataReader reader)</v>
       </c>
       <c r="X10" s="12" t="str">
         <f>"        DataResult&lt;"&amp;C2&amp;"&gt; Save("&amp;C2&amp;" "&amp;LOWER(C2)&amp;");"</f>
-        <v>        DataResult&lt;Deities&gt; Save(Deities deities);</v>
+        <v>        DataResult&lt;Shops&gt; Save(Shops shops);</v>
       </c>
       <c r="Z10" s="13" t="str">
         <f>"    public class Sql"&amp;C2&amp;"Repository : Repository&lt;"&amp;C2&amp;"&gt;, I"&amp;C2&amp;"Repository"</f>
-        <v>    public class SqlDeitiesRepository : Repository&lt;Deities&gt;, IDeitiesRepository</v>
+        <v>    public class SqlShopsRepository : Repository&lt;Shops&gt;, IShopsRepository</v>
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H11" s="19"/>
       <c r="J11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     </v>
+        <v xml:space="preserve">    ParentMapAreaLocationN DECIMAL,</v>
       </c>
       <c r="L11" s="22" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>@ParentMapAreaLocationW DECIMAL</v>
       </c>
       <c r="N11" s="23" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>@ParentMapAreaLocationW DECIMAL</v>
       </c>
       <c r="P11" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">    [ShopId],</v>
       </c>
       <c r="T11" s="6" t="s">
         <v>57</v>
@@ -1373,19 +1395,23 @@
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H12" s="19"/>
       <c r="J12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     </v>
+        <v xml:space="preserve">    ParentMapAreaLocationW DECIMAL</v>
       </c>
       <c r="L12" s="22" t="str">
         <f t="shared" si="1"/>
@@ -1396,34 +1422,34 @@
         <v/>
       </c>
       <c r="P12" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">    [MapImage],</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" ref="Q12:Q27" si="6">IF(NOT(ISBLANK(C5)),C5,"")</f>
+        <f t="shared" ref="Q12:Q27" si="5">IF(NOT(ISBLANK(C5)),C5,"")</f>
         <v>int</v>
       </c>
       <c r="R12" s="5" t="str">
-        <f t="shared" ref="R12:R27" si="7">IF(NOT(ISBLANK(C5)),"        "&amp;IF(ISBLANK(S12),C5,S12)&amp;" "&amp;B5&amp;" { get; set; }","")</f>
-        <v xml:space="preserve">        string AuthorityLevelId { get; set; }</v>
+        <f t="shared" ref="R12:R27" si="6">IF(NOT(ISBLANK(C5)),"        "&amp;IF(ISBLANK(S12),C5,S12)&amp;" "&amp;B5&amp;" { get; set; }","")</f>
+        <v xml:space="preserve">        string OwnerActorId { get; set; }</v>
       </c>
       <c r="S12" t="s">
         <v>95</v>
       </c>
       <c r="T12" s="6" t="str">
-        <f t="shared" ref="T12:T27" si="8">IF(LEN(R12)&gt;0,"        public "&amp;TRIM(R12),"")</f>
-        <v xml:space="preserve">        public string AuthorityLevelId { get; set; }</v>
+        <f t="shared" ref="T12:T27" si="7">IF(LEN(R12)&gt;0,"        public "&amp;TRIM(R12),"")</f>
+        <v xml:space="preserve">        public string OwnerActorId { get; set; }</v>
       </c>
       <c r="V12" s="16" t="str">
         <f>"            return new "&amp;C2&amp;"("</f>
-        <v>            return new Deities(</v>
+        <v>            return new Shops(</v>
       </c>
       <c r="X12" s="12" t="s">
         <v>55</v>
       </c>
       <c r="Z12" s="13" t="str">
         <f>"        public Sql"&amp;C2&amp;"Repository(IUnitOfWork unitOfWork)"</f>
-        <v>        public SqlDeitiesRepository(IUnitOfWork unitOfWork)</v>
+        <v>        public SqlShopsRepository(IUnitOfWork unitOfWork)</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
@@ -1433,7 +1459,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H13" s="2"/>
@@ -1450,27 +1476,27 @@
         <v/>
       </c>
       <c r="P13" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">    [ParentMapAreaId],</v>
+      </c>
+      <c r="Q13" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q13" t="str">
+        <v>decimal</v>
+      </c>
+      <c r="R13" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>int</v>
-      </c>
-      <c r="R13" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">        string CompassionLevelId { get; set; }</v>
+        <v xml:space="preserve">        string CostModifier { get; set; }</v>
       </c>
       <c r="S13" t="s">
         <v>95</v>
       </c>
       <c r="T13" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">        public string CompassionLevelId { get; set; }</v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">        public string CostModifier { get; set; }</v>
       </c>
       <c r="V13" s="16" t="str">
         <f>"                reader.Get&lt;int&gt;("&amp;C2&amp;"Col.Id),"</f>
-        <v xml:space="preserve">                reader.Get&lt;int&gt;(DeitiesCol.Id),</v>
+        <v xml:space="preserve">                reader.Get&lt;int&gt;(ShopsCol.Id),</v>
       </c>
       <c r="Z13" s="13" t="s">
         <v>68</v>
@@ -1483,7 +1509,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H14" s="2"/>
@@ -1500,27 +1526,27 @@
         <v/>
       </c>
       <c r="P14" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">    [ParentMapAreaLocationN],</v>
+      </c>
+      <c r="Q14" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q14" t="str">
+        <v>varchar(MAX)</v>
+      </c>
+      <c r="R14" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>varchar(MAX)</v>
-      </c>
-      <c r="R14" s="5" t="str">
-        <f t="shared" si="7"/>
         <v xml:space="preserve">        int FlavourText { get; set; }</v>
       </c>
       <c r="S14" t="s">
         <v>6</v>
       </c>
       <c r="T14" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">        public int FlavourText { get; set; }</v>
       </c>
       <c r="V14" s="16" t="str">
-        <f t="shared" ref="V14:V29" si="9">IF(LEN(S12)&gt;0,"                reader.Get&lt;"&amp;S12&amp;"&gt;("&amp;C$2&amp;"Col."&amp;B5&amp;")"&amp;IF(LEN(V15)&gt;0,",",""),"")</f>
-        <v>                reader.Get&lt;string&gt;(DeitiesCol.AuthorityLevelId),</v>
+        <f t="shared" ref="V14:V29" si="8">IF(LEN(S12)&gt;0,"                reader.Get&lt;"&amp;S12&amp;"&gt;("&amp;C$2&amp;"Col."&amp;B5&amp;")"&amp;IF(LEN(V15)&gt;0,",",""),"")</f>
+        <v>                reader.Get&lt;string&gt;(ShopsCol.OwnerActorId),</v>
       </c>
       <c r="Z14" s="13" t="s">
         <v>52</v>
@@ -1533,7 +1559,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H15" s="2"/>
@@ -1550,27 +1576,24 @@
         <v/>
       </c>
       <c r="P15" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">    [ParentMapAreaLocationW]</v>
+      </c>
+      <c r="Q15" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q15" t="str">
+        <v>int</v>
+      </c>
+      <c r="R15" s="5" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R15" s="5" t="str">
+        <v xml:space="preserve">        int ShopId { get; set; }</v>
+      </c>
+      <c r="T15" s="6" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="S15" t="s">
-        <v>96</v>
-      </c>
-      <c r="T15" s="6" t="str">
+        <v xml:space="preserve">        public int ShopId { get; set; }</v>
+      </c>
+      <c r="V15" s="16" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="V15" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;string&gt;(DeitiesCol.CompassionLevelId),</v>
+        <v>                reader.Get&lt;string&gt;(ShopsCol.CostModifier),</v>
       </c>
       <c r="Z15" s="13" t="s">
         <v>53</v>
@@ -1583,7 +1606,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H16" s="2"/>
@@ -1600,27 +1623,24 @@
         <v/>
       </c>
       <c r="P16" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q16" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q16" t="str">
+        <v>binary</v>
+      </c>
+      <c r="R16" s="5" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R16" s="5" t="str">
+        <v xml:space="preserve">        binary MapImage { get; set; }</v>
+      </c>
+      <c r="T16" s="6" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="S16" t="s">
-        <v>97</v>
-      </c>
-      <c r="T16" s="6" t="str">
+        <v xml:space="preserve">        public binary MapImage { get; set; }</v>
+      </c>
+      <c r="V16" s="16" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="V16" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;int&gt;(DeitiesCol.FlavourText),</v>
+        <v>                reader.Get&lt;int&gt;(ShopsCol.FlavourText)</v>
       </c>
     </row>
     <row r="17" spans="2:26" x14ac:dyDescent="0.25">
@@ -1630,7 +1650,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H17" s="2"/>
@@ -1647,31 +1667,28 @@
         <v/>
       </c>
       <c r="P17" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q17" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q17" t="str">
+        <v>int</v>
+      </c>
+      <c r="R17" s="5" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R17" s="5" t="str">
+        <v xml:space="preserve">        int ParentMapAreaId { get; set; }</v>
+      </c>
+      <c r="T17" s="6" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="S17" t="s">
-        <v>95</v>
-      </c>
-      <c r="T17" s="6" t="str">
+        <v xml:space="preserve">        public int ParentMapAreaId { get; set; }</v>
+      </c>
+      <c r="V17" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V17" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;CurrencyType&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z17" s="13" t="str">
         <f>"        protected override "&amp;C2&amp;" Map(IDataReader reader)"</f>
-        <v xml:space="preserve">        protected override Deities Map(IDataReader reader)</v>
+        <v xml:space="preserve">        protected override Shops Map(IDataReader reader)</v>
       </c>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
@@ -1681,7 +1698,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H18" s="2"/>
@@ -1698,27 +1715,24 @@
         <v/>
       </c>
       <c r="P18" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q18" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q18" t="str">
+        <v>decimal</v>
+      </c>
+      <c r="R18" s="5" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R18" s="5" t="str">
+        <v xml:space="preserve">        decimal ParentMapAreaLocationN { get; set; }</v>
+      </c>
+      <c r="T18" s="6" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="S18" t="s">
-        <v>95</v>
-      </c>
-      <c r="T18" s="6" t="str">
+        <v xml:space="preserve">        public decimal ParentMapAreaLocationN { get; set; }</v>
+      </c>
+      <c r="V18" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V18" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;bool&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z18" s="13" t="s">
         <v>79</v>
@@ -1731,7 +1745,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H19" s="2"/>
@@ -1748,31 +1762,28 @@
         <v/>
       </c>
       <c r="P19" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q19" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q19" t="str">
+        <v>decimal</v>
+      </c>
+      <c r="R19" s="5" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R19" s="5" t="str">
+        <v xml:space="preserve">        decimal ParentMapAreaLocationW { get; set; }</v>
+      </c>
+      <c r="T19" s="6" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="S19" t="s">
-        <v>95</v>
-      </c>
-      <c r="T19" s="6" t="str">
+        <v xml:space="preserve">        public decimal ParentMapAreaLocationW { get; set; }</v>
+      </c>
+      <c r="V19" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V19" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;string&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z19" s="13" t="str">
         <f>"           return "&amp;C2&amp;"Helper.ParseReader(reader);"</f>
-        <v>           return DeitiesHelper.ParseReader(reader);</v>
+        <v>           return ShopsHelper.ParseReader(reader);</v>
       </c>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.25">
@@ -1782,7 +1793,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H20" s="2"/>
@@ -1797,27 +1808,24 @@
         <v>38</v>
       </c>
       <c r="P20" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q20" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="Q20" t="str">
+      <c r="R20" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R20" s="5" t="str">
+      <c r="T20" s="6" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="S20" t="s">
-        <v>103</v>
-      </c>
-      <c r="T20" s="6" t="str">
+      <c r="V20" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V20" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;string&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z20" s="13" t="s">
         <v>80</v>
@@ -1830,7 +1838,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" t="str">
-        <f t="shared" ref="G21:G24" si="10">IF(UPPER(RIGHT(B21,2))="ID",B$2&amp;"."&amp;LEFT(B21,LEN(B21)-2)&amp;"("&amp;B21&amp;")","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H21" s="2"/>
@@ -1842,27 +1850,24 @@
         <v>11</v>
       </c>
       <c r="P21" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q21" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="Q21" t="str">
+      <c r="R21" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R21" s="5" t="str">
+      <c r="T21" s="6" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="S21" t="s">
-        <v>6</v>
-      </c>
-      <c r="T21" s="6" t="str">
+      <c r="V21" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V21" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;string&gt;(DeitiesCol.),</v>
       </c>
     </row>
     <row r="22" spans="2:26" x14ac:dyDescent="0.25">
@@ -1872,7 +1877,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H22" s="2"/>
@@ -1884,31 +1889,28 @@
         <v>39</v>
       </c>
       <c r="P22" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q22" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="Q22" t="str">
+      <c r="R22" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R22" s="5" t="str">
+      <c r="T22" s="6" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="S22" t="s">
-        <v>104</v>
-      </c>
-      <c r="T22" s="6" t="str">
+      <c r="V22" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V22" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;InvoiceLayoutType&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z22" s="13" t="str">
         <f>"        public "&amp;C2&amp;" Get(int "&amp;LOWER(C2)&amp;"Id)"</f>
-        <v>        public Deities Get(int deitiesId)</v>
+        <v>        public Shops Get(int shopsId)</v>
       </c>
     </row>
     <row r="23" spans="2:26" x14ac:dyDescent="0.25">
@@ -1918,7 +1920,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H23" s="2"/>
@@ -1931,26 +1933,23 @@
       </c>
       <c r="N23" s="23" t="str">
         <f>"UPDATE "&amp;B2&amp;"."&amp;C2</f>
-        <v>UPDATE dbo.Deities</v>
+        <v>UPDATE dbo.Shops</v>
       </c>
       <c r="Q23" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R23" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R23" s="5" t="str">
+      <c r="T23" s="6" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="S23" t="s">
-        <v>104</v>
-      </c>
-      <c r="T23" s="6" t="str">
+      <c r="V23" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V23" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;int&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z23" s="13" t="s">
         <v>52</v>
@@ -1963,7 +1962,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H24" s="2"/>
@@ -1973,7 +1972,7 @@
       </c>
       <c r="L24" s="22" t="str">
         <f>"FROM "&amp;B2&amp;"."&amp;C2</f>
-        <v>FROM dbo.Deities</v>
+        <v>FROM dbo.Shops</v>
       </c>
       <c r="N24" s="23" t="s">
         <v>45</v>
@@ -1982,27 +1981,24 @@
         <v>90</v>
       </c>
       <c r="Q24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R24" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R24" s="5" t="str">
+      <c r="T24" s="6" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="S24" t="s">
-        <v>97</v>
-      </c>
-      <c r="T24" s="6" t="str">
+      <c r="V24" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V24" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;TimeFrequency&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z24" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Get""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Deities_Get"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Shops_Get"))</v>
       </c>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.25">
@@ -2012,7 +2008,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" t="str">
-        <f t="shared" ref="G25:G29" si="11">IF(UPPER(RIGHT(B25,2))="ID",B$2&amp;"."&amp;LEFT(B25,LEN(B25)-2)&amp;"("&amp;B25&amp;")","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H25" s="2"/>
@@ -2024,31 +2020,28 @@
         <v>40</v>
       </c>
       <c r="N25" s="23" t="str">
-        <f t="shared" ref="N25:N40" si="12">IF(NOT(ISBLANK(B5)),"["&amp;B5&amp;"] = @"&amp;B5&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>[AuthorityLevelId] = @AuthorityLevelId,</v>
+        <f t="shared" ref="N25:N40" si="9">IF(NOT(ISBLANK(B5)),"["&amp;B5&amp;"] = @"&amp;B5&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
+        <v>[OwnerActorId] = @OwnerActorId,</v>
       </c>
       <c r="P25" s="18" t="str">
         <f>"    "&amp;B2&amp;"."&amp;C2</f>
-        <v xml:space="preserve">    dbo.Deities</v>
+        <v xml:space="preserve">    dbo.Shops</v>
       </c>
       <c r="Q25" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R25" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R25" s="5" t="str">
+      <c r="T25" s="6" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="S25" t="s">
-        <v>105</v>
-      </c>
-      <c r="T25" s="6" t="str">
+      <c r="V25" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V25" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;TimeFrequency&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z25" s="13" t="s">
         <v>69</v>
@@ -2061,7 +2054,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H26" s="2"/>
@@ -2071,30 +2064,30 @@
       </c>
       <c r="L26" s="22" t="str">
         <f>IF(NOT(ISBLANK(B4)),"["&amp;B4&amp;"] = ISNULL(@"&amp;B4&amp;", 0)","")</f>
-        <v>[DeityId] = ISNULL(@DeityId, 0)</v>
+        <v>[ShopId] = ISNULL(@ShopId, 0)</v>
       </c>
       <c r="N26" s="23" t="str">
-        <f t="shared" si="12"/>
-        <v>[CompassionLevelId] = @CompassionLevelId,</v>
+        <f t="shared" si="9"/>
+        <v>[CostModifier] = @CostModifier,</v>
       </c>
       <c r="P26" s="18" t="s">
         <v>40</v>
       </c>
       <c r="Q26" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R26" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R26" s="5" t="str">
+      <c r="T26" s="6" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="T26" s="6" t="str">
+      <c r="V26" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V26" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;bool&gt;(DeitiesCol.),</v>
       </c>
       <c r="Z26" s="13" t="s">
         <v>70</v>
@@ -2107,7 +2100,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H27" s="2"/>
@@ -2119,32 +2112,32 @@
         <v>41</v>
       </c>
       <c r="N27" s="23" t="str">
-        <f t="shared" si="12"/>
-        <v>[FlavourText] = @FlavourText</v>
+        <f t="shared" si="9"/>
+        <v>[FlavourText] = @FlavourText,</v>
       </c>
       <c r="P27" s="18" t="str">
         <f>"    "&amp;B4&amp;" = @"&amp;B4</f>
-        <v xml:space="preserve">    DeityId = @DeityId</v>
+        <v xml:space="preserve">    ShopId = @ShopId</v>
       </c>
       <c r="Q27" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R27" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R27" s="5" t="str">
+      <c r="T27" s="6" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="T27" s="6" t="str">
+      <c r="V27" s="16" t="str">
         <f t="shared" si="8"/>
         <v/>
-      </c>
-      <c r="V27" s="16" t="str">
-        <f t="shared" si="9"/>
-        <v>                reader.Get&lt;CommunicationType&gt;(DeitiesCol.)</v>
       </c>
       <c r="Z27" s="13" t="str">
         <f>"                    .AddWithValue(""@"&amp;C2&amp;"Id"", "&amp;LOWER(C2)&amp;"Id, SqlDbType.Int);"</f>
-        <v>                    .AddWithValue("@DeitiesId", deitiesId, SqlDbType.Int);</v>
+        <v>                    .AddWithValue("@ShopsId", shopsId, SqlDbType.Int);</v>
       </c>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.25">
@@ -2154,7 +2147,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H28" s="2"/>
@@ -2166,14 +2159,14 @@
         <v>11</v>
       </c>
       <c r="N28" s="23" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="9"/>
+        <v>[ShopId] = @ShopId,</v>
       </c>
       <c r="R28" s="5" t="s">
         <v>56</v>
       </c>
       <c r="V28" s="16" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -2184,7 +2177,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H29" s="2"/>
@@ -2194,21 +2187,21 @@
       </c>
       <c r="L29" s="22" t="str">
         <f>"INSERT INTO "&amp;B2&amp;"."&amp;C2&amp;" ("</f>
-        <v>INSERT INTO dbo.Deities (</v>
+        <v>INSERT INTO dbo.Shops (</v>
       </c>
       <c r="N29" s="23" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="9"/>
+        <v>[MapImage] = @MapImage,</v>
       </c>
       <c r="R29" s="5" t="s">
         <v>55</v>
       </c>
       <c r="T29" s="6" t="str">
         <f>"        public "&amp;C2&amp;"("</f>
-        <v>        public Deities(</v>
+        <v>        public Shops(</v>
       </c>
       <c r="V29" s="16" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="Z29" s="13" t="s">
@@ -2222,7 +2215,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" t="str">
-        <f t="shared" ref="G30:G32" si="13">IF(UPPER(RIGHT(B30,2))="ID",B$2&amp;"."&amp;LEFT(B30,LEN(B30)-2)&amp;"("&amp;B30&amp;")","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H30" s="2"/>
@@ -2232,15 +2225,15 @@
       </c>
       <c r="L30" s="22" t="str">
         <f>IF(NOT(ISBLANK(B5)),"["&amp;B5&amp;"]"&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>[AuthorityLevelId],</v>
+        <v>[OwnerActorId],</v>
       </c>
       <c r="N30" s="23" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="9"/>
+        <v>[ParentMapAreaId] = @ParentMapAreaId,</v>
       </c>
       <c r="T30" s="6" t="str">
         <f>IF(NOT(ISBLANK(B4)),"            int"&amp;" "&amp;LOWER(LEFT(B4,1))&amp;MID(B4,2,LEN(B4)-1)&amp;IF(LEN(T31)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            int deityId,</v>
+        <v xml:space="preserve">            int shopId,</v>
       </c>
       <c r="Z30" s="13" t="s">
         <v>72</v>
@@ -2253,7 +2246,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H31" s="2"/>
@@ -2262,16 +2255,16 @@
         <v xml:space="preserve">     </v>
       </c>
       <c r="L31" s="22" t="str">
-        <f t="shared" ref="L31:L45" si="14">IF(NOT(ISBLANK(B6)),"["&amp;B6&amp;"]"&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>[CompassionLevelId],</v>
+        <f t="shared" ref="L31:L45" si="10">IF(NOT(ISBLANK(B6)),"["&amp;B6&amp;"]"&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
+        <v>[CostModifier],</v>
       </c>
       <c r="N31" s="23" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="9"/>
+        <v>[ParentMapAreaLocationN] = @ParentMapAreaLocationN,</v>
       </c>
       <c r="T31" s="6" t="str">
-        <f t="shared" ref="T31:T46" si="15">IF(NOT(ISBLANK(B5)),"            "&amp;S12&amp;" "&amp;LOWER(LEFT(B5,1))&amp;MID(B5,2,LEN(B5)-1)&amp;IF(LEN(T32)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            string authorityLevelId,</v>
+        <f t="shared" ref="T31:T46" si="11">IF(NOT(ISBLANK(B5)),"            "&amp;S12&amp;" "&amp;LOWER(LEFT(B5,1))&amp;MID(B5,2,LEN(B5)-1)&amp;IF(LEN(T32)&gt;0,",",""),"")</f>
+        <v xml:space="preserve">            string ownerActorId,</v>
       </c>
       <c r="V31" s="16" t="s">
         <v>83</v>
@@ -2287,7 +2280,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H32" s="2"/>
@@ -2296,16 +2289,16 @@
         <v xml:space="preserve">     </v>
       </c>
       <c r="L32" s="22" t="str">
-        <f t="shared" si="14"/>
-        <v>[FlavourText]</v>
+        <f t="shared" si="10"/>
+        <v>[FlavourText],</v>
       </c>
       <c r="N32" s="23" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="9"/>
+        <v>[ParentMapAreaLocationW] = @ParentMapAreaLocationW</v>
       </c>
       <c r="T32" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">            string compassionLevelId,</v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">            string costModifier,</v>
       </c>
       <c r="V32" s="16" t="s">
         <v>53</v>
@@ -2320,82 +2313,82 @@
         <v>);</v>
       </c>
       <c r="L33" s="22" t="str">
-        <f t="shared" si="14"/>
-        <v/>
+        <f t="shared" si="10"/>
+        <v>[ShopId],</v>
       </c>
       <c r="N33" s="23" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T33" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">            int flavourText</v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">            int flavourText,</v>
       </c>
       <c r="V33" s="16" t="s">
         <v>12</v>
       </c>
       <c r="Z33" s="13" t="str">
         <f>"        public DataResult&lt;"&amp;C2&amp;"&gt; Save("&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;Deities&gt; Save(Deities value)</v>
+        <v xml:space="preserve">        public DataResult&lt;Shops&gt; Save(Shops value)</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L34" s="22" t="str">
-        <f t="shared" si="14"/>
-        <v/>
+        <f t="shared" si="10"/>
+        <v>[MapImage],</v>
       </c>
       <c r="N34" s="23" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T34" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v/>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">             shopId,</v>
       </c>
       <c r="V34" s="16" t="str">
         <f>"        public static IEnumerable&lt;"&amp;C2&amp;"&gt; ParseMultipleReader(IDataReader reader)"</f>
-        <v>        public static IEnumerable&lt;Deities&gt; ParseMultipleReader(IDataReader reader)</v>
+        <v>        public static IEnumerable&lt;Shops&gt; ParseMultipleReader(IDataReader reader)</v>
       </c>
       <c r="Z34" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L35" s="22" t="str">
-        <f t="shared" si="14"/>
-        <v/>
+        <f t="shared" si="10"/>
+        <v>[ParentMapAreaId],</v>
       </c>
       <c r="N35" s="23" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T35" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v/>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">             mapImage,</v>
       </c>
       <c r="V35" s="16" t="s">
         <v>52</v>
       </c>
       <c r="Z35" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L36" s="22" t="str">
-        <f t="shared" si="14"/>
-        <v/>
+        <f t="shared" si="10"/>
+        <v>[ParentMapAreaLocationN],</v>
       </c>
       <c r="N36" s="23" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T36" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v/>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">             parentMapAreaId,</v>
       </c>
       <c r="V36" s="16" t="str">
         <f>"            var "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;"s = new List&lt;"&amp;C2&amp;"&gt;();"</f>
-        <v>            var deitiess = new List&lt;Deities&gt;();</v>
+        <v>            var shopss = new List&lt;Shops&gt;();</v>
       </c>
       <c r="Z36" s="13" t="s">
         <v>53</v>
@@ -2403,16 +2396,16 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L37" s="22" t="str">
-        <f t="shared" si="14"/>
-        <v/>
+        <f t="shared" si="10"/>
+        <v>[ParentMapAreaLocationW]</v>
       </c>
       <c r="N37" s="23" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T37" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v/>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">             parentMapAreaLocationN,</v>
       </c>
       <c r="V37" s="16" t="s">
         <v>12</v>
@@ -2420,36 +2413,36 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L38" s="22" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N38" s="23" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T38" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v/>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">             parentMapAreaLocationW</v>
       </c>
       <c r="V38" s="16" t="s">
         <v>84</v>
       </c>
       <c r="Z38" s="13" t="str">
         <f>"        public DataResult&lt;"&amp;C2&amp;"&gt; Create("&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;Deities&gt; Create(Deities value)</v>
+        <v xml:space="preserve">        public DataResult&lt;Shops&gt; Create(Shops value)</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L39" s="22" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N39" s="23" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T39" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="V39" s="16" t="s">
@@ -2461,37 +2454,37 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L40" s="22" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N40" s="23" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T40" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="V40" s="16" t="str">
         <f>"                "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;".Add(ParseReader(reader));"</f>
-        <v>                deities.Add(ParseReader(reader));</v>
+        <v>                shops.Add(ParseReader(reader));</v>
       </c>
       <c r="Z40" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Create""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Deities_Create"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Shops_Create"))</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L41" s="22" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N41" s="23" t="str">
         <f>IF(NOT(ISBLANK(B4)),"WHERE ["&amp;B4&amp;"] = ISNULL(@"&amp;B4&amp;", 0)","")</f>
-        <v>WHERE [DeityId] = ISNULL(@DeityId, 0)</v>
+        <v>WHERE [ShopId] = ISNULL(@ShopId, 0)</v>
       </c>
       <c r="T41" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="V41" s="16" t="s">
@@ -2503,7 +2496,7 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L42" s="22" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N42" s="23" t="str">
@@ -2511,7 +2504,7 @@
         <v/>
       </c>
       <c r="T42" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="V42" s="16" t="s">
@@ -2519,29 +2512,29 @@
       </c>
       <c r="Z42" s="13" t="str">
         <f>"                var idParameter = command.AddOutput(""@"&amp;C2&amp;"Id"", SqlDbType.Int);"</f>
-        <v>                var idParameter = command.AddOutput("@DeitiesId", SqlDbType.Int);</v>
+        <v>                var idParameter = command.AddOutput("@ShopsId", SqlDbType.Int);</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L43" s="22" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N43" s="23" t="s">
         <v>93</v>
       </c>
       <c r="T43" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="V43" s="16" t="str">
         <f>"            return "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;";"</f>
-        <v>            return deities;</v>
+        <v>            return shops;</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L44" s="22" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N44" s="23" t="str">
@@ -2549,7 +2542,7 @@
         <v/>
       </c>
       <c r="T44" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="V44" s="16" t="s">
@@ -2561,22 +2554,22 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L45" s="22" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N45" s="23" t="s">
         <v>14</v>
       </c>
       <c r="T45" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="V45" s="16" t="s">
         <v>12</v>
       </c>
       <c r="Z45" s="13" t="str">
-        <f t="shared" ref="Z45" si="16">IF(NOT(ISBLANK(B4)),"                    .AddWithValue(""@"&amp;B4&amp;""", value.Id,  SqlDbType.Int"&amp;")"&amp;IF(LEN(Z46)&gt;0,"",";"),"")</f>
-        <v>                    .AddWithValue("@DeityId", value.Id,  SqlDbType.Int)</v>
+        <f t="shared" ref="Z45" si="12">IF(NOT(ISBLANK(B4)),"                    .AddWithValue(""@"&amp;B4&amp;""", value.Id,  SqlDbType.Int"&amp;")"&amp;IF(LEN(Z46)&gt;0,"",";"),"")</f>
+        <v>                    .AddWithValue("@ShopId", value.Id,  SqlDbType.Int)</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
@@ -2584,16 +2577,16 @@
         <v>41</v>
       </c>
       <c r="T46" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="V46" s="16" t="str">
         <f>"        private enum "&amp;C2&amp;"Col"</f>
-        <v>        private enum DeitiesCol</v>
+        <v>        private enum ShopsCol</v>
       </c>
       <c r="Z46" s="13" t="str">
         <f>IF(NOT(ISBLANK(B5)),"                    .AddWithValue(""@"&amp;B5&amp;""", value."&amp;B5&amp;", SqlDbType."&amp;IF(NOT(OR(ISBLANK(Q12),Q12="int")),UPPER(LEFT(Q12,1))&amp;MID(Q12,2,LEN(Q12)-1),"Int")&amp;")"&amp;IF(LEFT(Z47,24)="                    .Add","",";"),"")</f>
-        <v>                    .AddWithValue("@AuthorityLevelId", value.AuthorityLevelId, SqlDbType.Int)</v>
+        <v>                    .AddWithValue("@OwnerActorId", value.OwnerActorId, SqlDbType.Int)</v>
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
@@ -2607,14 +2600,14 @@
         <v>52</v>
       </c>
       <c r="Z47" s="13" t="str">
-        <f t="shared" ref="Z47:Z62" si="17">IF(NOT(ISBLANK(B6)),"                    .AddWithValue(""@"&amp;B6&amp;""", value."&amp;B6&amp;", SqlDbType."&amp;IF(NOT(OR(ISBLANK(Q13),Q13="int")),UPPER(LEFT(Q13,1))&amp;MID(Q13,2,LEN(Q13)-1),"Int")&amp;")"&amp;IF(LEFT(Z48,24)="                    .Add","",";"),"")</f>
-        <v>                    .AddWithValue("@CompassionLevelId", value.CompassionLevelId, SqlDbType.Int)</v>
+        <f t="shared" ref="Z47:Z62" si="13">IF(NOT(ISBLANK(B6)),"                    .AddWithValue(""@"&amp;B6&amp;""", value."&amp;B6&amp;", SqlDbType."&amp;IF(NOT(OR(ISBLANK(Q13),Q13="int")),UPPER(LEFT(Q13,1))&amp;MID(Q13,2,LEN(Q13)-1),"Int")&amp;")"&amp;IF(LEFT(Z48,24)="                    .Add","",";"),"")</f>
+        <v>                    .AddWithValue("@CostModifier", value.CostModifier, SqlDbType.Decimal)</v>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L48" s="22" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@AuthorityLevelId,</v>
+        <v>@OwnerActorId,</v>
       </c>
       <c r="T48" s="6" t="s">
         <v>52</v>
@@ -2623,277 +2616,277 @@
         <v>86</v>
       </c>
       <c r="Z48" s="13" t="str">
-        <f t="shared" si="17"/>
-        <v>                    .AddWithValue("@FlavourText", value.FlavourText, SqlDbType.Varchar(MAX));</v>
+        <f t="shared" si="13"/>
+        <v>                    .AddWithValue("@FlavourText", value.FlavourText, SqlDbType.Varchar(MAX))</v>
       </c>
     </row>
     <row r="49" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L49" s="22" t="str">
-        <f t="shared" ref="L49:L63" si="18">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>@CompassionLevelId,</v>
+        <f t="shared" ref="L49:L63" si="14">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
+        <v>@CostModifier,</v>
       </c>
       <c r="T49" s="6" t="str">
         <f>IF(NOT(ISBLANK(B4)),"            Id = "&amp;LOWER(LEFT(B4,1))&amp;MID(B4,2,LEN(B4)-1)&amp;";","")</f>
-        <v xml:space="preserve">            Id = deityId;</v>
+        <v xml:space="preserve">            Id = shopId;</v>
       </c>
       <c r="V49" s="16" t="str">
-        <f t="shared" ref="V49:V64" si="19">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;IF(LEN(V15)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            AuthorityLevelId,</v>
+        <f t="shared" ref="V49:V64" si="15">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;IF(LEN(V15)&gt;0,",",""),"")</f>
+        <v xml:space="preserve">            OwnerActorId,</v>
       </c>
       <c r="Z49" s="13" t="str">
-        <f t="shared" si="17"/>
-        <v/>
+        <f t="shared" si="13"/>
+        <v>                    .AddWithValue("@ShopId", value.ShopId, SqlDbType.Int)</v>
       </c>
     </row>
     <row r="50" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L50" s="22" t="str">
-        <f t="shared" si="18"/>
-        <v>@FlavourText</v>
+        <f t="shared" si="14"/>
+        <v>@FlavourText,</v>
       </c>
       <c r="T50" s="6" t="str">
-        <f t="shared" ref="T50:T65" si="20">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;" = "&amp;LOWER(LEFT(B5,1))&amp;MID(B5,2,LEN(B5)-1)&amp;";","")</f>
-        <v xml:space="preserve">            AuthorityLevelId = authorityLevelId;</v>
+        <f t="shared" ref="T50:T65" si="16">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;" = "&amp;LOWER(LEFT(B5,1))&amp;MID(B5,2,LEN(B5)-1)&amp;";","")</f>
+        <v xml:space="preserve">            OwnerActorId = ownerActorId;</v>
       </c>
       <c r="V50" s="16" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">            CompassionLevelId,</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">            CostModifier,</v>
       </c>
       <c r="Z50" s="13" t="str">
-        <f t="shared" si="17"/>
-        <v/>
+        <f t="shared" si="13"/>
+        <v>                    .AddWithValue("@MapImage", value.MapImage, SqlDbType.Binary)</v>
       </c>
     </row>
     <row r="51" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L51" s="22" t="str">
         <f>IF(NOT(ISBLANK(B8)),"@"&amp;B8&amp;IF(NOT(ISBLANK(B9)),",",""),"")</f>
-        <v/>
+        <v>@ShopId,</v>
       </c>
       <c r="T51" s="6" t="str">
-        <f t="shared" si="20"/>
-        <v xml:space="preserve">            CompassionLevelId = compassionLevelId;</v>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">            CostModifier = costModifier;</v>
       </c>
       <c r="V51" s="16" t="str">
-        <f t="shared" si="19"/>
-        <v xml:space="preserve">            FlavourText,</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">            FlavourText</v>
       </c>
       <c r="Z51" s="13" t="str">
-        <f t="shared" si="17"/>
-        <v/>
+        <f t="shared" si="13"/>
+        <v>                    .AddWithValue("@ParentMapAreaId", value.ParentMapAreaId, SqlDbType.Int)</v>
       </c>
     </row>
     <row r="52" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L52" s="22" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+        <f t="shared" si="14"/>
+        <v>@MapImage,</v>
       </c>
       <c r="T52" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">            FlavourText = flavourText;</v>
       </c>
       <c r="V52" s="16" t="str">
-        <f t="shared" si="19"/>
-        <v/>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">            ShopId</v>
       </c>
       <c r="Z52" s="13" t="str">
-        <f t="shared" si="17"/>
-        <v/>
+        <f t="shared" si="13"/>
+        <v>                    .AddWithValue("@ParentMapAreaLocationN", value.ParentMapAreaLocationN, SqlDbType.Decimal)</v>
       </c>
     </row>
     <row r="53" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L53" s="22" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+        <f t="shared" si="14"/>
+        <v>@ParentMapAreaId,</v>
       </c>
       <c r="T53" s="6" t="str">
-        <f t="shared" si="20"/>
-        <v/>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">            ShopId = shopId;</v>
       </c>
       <c r="V53" s="16" t="str">
-        <f t="shared" si="19"/>
-        <v/>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">            MapImage</v>
       </c>
       <c r="Z53" s="13" t="str">
-        <f t="shared" si="17"/>
-        <v/>
+        <f t="shared" si="13"/>
+        <v>                    .AddWithValue("@ParentMapAreaLocationW", value.ParentMapAreaLocationW, SqlDbType.Decimal);</v>
       </c>
     </row>
     <row r="54" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L54" s="22" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+        <f t="shared" si="14"/>
+        <v>@ParentMapAreaLocationN,</v>
       </c>
       <c r="T54" s="6" t="str">
-        <f t="shared" si="20"/>
-        <v/>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">            MapImage = mapImage;</v>
       </c>
       <c r="V54" s="16" t="str">
-        <f t="shared" si="19"/>
-        <v/>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">            ParentMapAreaId</v>
       </c>
       <c r="Z54" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L55" s="22" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+        <f t="shared" si="14"/>
+        <v>@ParentMapAreaLocationW</v>
       </c>
       <c r="T55" s="6" t="str">
-        <f t="shared" si="20"/>
-        <v/>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">            ParentMapAreaId = parentMapAreaId;</v>
       </c>
       <c r="V55" s="16" t="str">
-        <f t="shared" si="19"/>
-        <v/>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">            ParentMapAreaLocationN</v>
       </c>
       <c r="Z55" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L56" s="22" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="T56" s="6" t="str">
-        <f t="shared" si="20"/>
-        <v/>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">            ParentMapAreaLocationN = parentMapAreaLocationN;</v>
       </c>
       <c r="V56" s="16" t="str">
-        <f t="shared" si="19"/>
-        <v/>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">            ParentMapAreaLocationW</v>
       </c>
       <c r="Z56" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L57" s="22" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="T57" s="6" t="str">
-        <f t="shared" si="20"/>
-        <v/>
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">            ParentMapAreaLocationW = parentMapAreaLocationW;</v>
       </c>
       <c r="V57" s="16" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Z57" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L58" s="22" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="T58" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="V58" s="16" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Z58" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L59" s="22" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="T59" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="V59" s="16" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Z59" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L60" s="22" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="T60" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="V60" s="16" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Z60" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L61" s="22" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="T61" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="V61" s="16" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Z61" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L62" s="22" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="T62" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="V62" s="16" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Z62" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L63" s="22" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="T63" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="V63" s="16" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Z63" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="12:26" x14ac:dyDescent="0.25">
@@ -2901,30 +2894,30 @@
         <v>41</v>
       </c>
       <c r="T64" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="V64" s="16" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="12:26" x14ac:dyDescent="0.25">
       <c r="T65" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="V65" s="16" t="s">
         <v>53</v>
       </c>
       <c r="Z65" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L66" s="22" t="str">
         <f>"SELECT @"&amp;B4&amp;" = SCOPE_IDENTITY()"</f>
-        <v>SELECT @DeityId = SCOPE_IDENTITY()</v>
+        <v>SELECT @ShopId = SCOPE_IDENTITY()</v>
       </c>
       <c r="V66" s="16" t="s">
         <v>54</v>
@@ -2939,7 +2932,7 @@
       </c>
       <c r="Z67" s="13" t="str">
         <f>"                return new DataResult&lt;"&amp;C2&amp;"&gt;(value, result);"</f>
-        <v>                return new DataResult&lt;Deities&gt;(value, result);</v>
+        <v>                return new DataResult&lt;Shops&gt;(value, result);</v>
       </c>
     </row>
     <row r="68" spans="12:26" x14ac:dyDescent="0.25">
@@ -2967,7 +2960,7 @@
     <row r="71" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z71" s="13" t="str">
         <f>"        public DataResult&lt;"&amp;C2&amp;"&gt; Update("&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;Deities&gt; Update(Deities value)</v>
+        <v xml:space="preserve">        public DataResult&lt;Shops&gt; Update(Shops value)</v>
       </c>
     </row>
     <row r="72" spans="12:26" x14ac:dyDescent="0.25">
@@ -2978,7 +2971,7 @@
     <row r="73" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z73" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Update""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Deities_Update"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Shops_Update"))</v>
       </c>
     </row>
     <row r="74" spans="12:26" x14ac:dyDescent="0.25">
@@ -2993,133 +2986,133 @@
     </row>
     <row r="76" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z76" s="13" t="str">
-        <f t="shared" ref="Z76" si="21">IF(NOT(ISBLANK(B4)),"                    .AddWithValue(""@"&amp;B4&amp;""", value.Id,  SqlDbType.Int"&amp;")"&amp;IF(LEN(Z77)&gt;0,"",";"),"")</f>
-        <v>                    .AddWithValue("@DeityId", value.Id,  SqlDbType.Int)</v>
+        <f t="shared" ref="Z76" si="17">IF(NOT(ISBLANK(B4)),"                    .AddWithValue(""@"&amp;B4&amp;""", value.Id,  SqlDbType.Int"&amp;")"&amp;IF(LEN(Z77)&gt;0,"",";"),"")</f>
+        <v>                    .AddWithValue("@ShopId", value.Id,  SqlDbType.Int)</v>
       </c>
     </row>
     <row r="77" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z77" s="13" t="str">
         <f>IF(NOT(ISBLANK(B5)),"                    .AddWithValue(""@"&amp;B5&amp;""", value."&amp;B5&amp;", SqlDbType."&amp;IF(NOT(OR(ISBLANK(Q12),Q12="int")),UPPER(LEFT(Q12,1))&amp;MID(Q12,2,LEN(Q12)-1),"Int")&amp;")"&amp;IF(LEFT(Z47,24)="                    .Add","",";"),"")</f>
-        <v>                    .AddWithValue("@AuthorityLevelId", value.AuthorityLevelId, SqlDbType.Int)</v>
+        <v>                    .AddWithValue("@OwnerActorId", value.OwnerActorId, SqlDbType.Int)</v>
       </c>
     </row>
     <row r="78" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z78" s="13" t="str">
-        <f t="shared" ref="Z78:Z90" si="22">IF(NOT(ISBLANK(B6)),"                    .AddWithValue(""@"&amp;B6&amp;""", value."&amp;B6&amp;", SqlDbType."&amp;IF(NOT(OR(ISBLANK(Q13),Q13="int")),UPPER(LEFT(Q13,1))&amp;MID(Q13,2,LEN(Q13)-1),"Int")&amp;")"&amp;IF(LEFT(Z48,24)="                    .Add","",";"),"")</f>
-        <v>                    .AddWithValue("@CompassionLevelId", value.CompassionLevelId, SqlDbType.Int)</v>
+        <f t="shared" ref="Z78:Z90" si="18">IF(NOT(ISBLANK(B6)),"                    .AddWithValue(""@"&amp;B6&amp;""", value."&amp;B6&amp;", SqlDbType."&amp;IF(NOT(OR(ISBLANK(Q13),Q13="int")),UPPER(LEFT(Q13,1))&amp;MID(Q13,2,LEN(Q13)-1),"Int")&amp;")"&amp;IF(LEFT(Z48,24)="                    .Add","",";"),"")</f>
+        <v>                    .AddWithValue("@CostModifier", value.CostModifier, SqlDbType.Decimal)</v>
       </c>
     </row>
     <row r="79" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z79" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v>                    .AddWithValue("@FlavourText", value.FlavourText, SqlDbType.Varchar(MAX));</v>
+        <f t="shared" si="18"/>
+        <v>                    .AddWithValue("@FlavourText", value.FlavourText, SqlDbType.Varchar(MAX))</v>
       </c>
     </row>
     <row r="80" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z80" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>                    .AddWithValue("@ShopId", value.ShopId, SqlDbType.Int)</v>
       </c>
     </row>
     <row r="81" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z81" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>                    .AddWithValue("@MapImage", value.MapImage, SqlDbType.Binary)</v>
       </c>
     </row>
     <row r="82" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z82" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>                    .AddWithValue("@ParentMapAreaId", value.ParentMapAreaId, SqlDbType.Int)</v>
       </c>
     </row>
     <row r="83" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z83" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>                    .AddWithValue("@ParentMapAreaLocationN", value.ParentMapAreaLocationN, SqlDbType.Decimal)</v>
       </c>
     </row>
     <row r="84" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z84" s="13" t="str">
-        <f t="shared" si="22"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>                    .AddWithValue("@ParentMapAreaLocationW", value.ParentMapAreaLocationW, SqlDbType.Decimal);</v>
       </c>
     </row>
     <row r="85" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z85" s="13" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z86" s="13" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z87" s="13" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z88" s="13" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z89" s="13" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z90" s="13" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z91" s="13" t="str">
-        <f t="shared" ref="Z91:Z95" si="23">IF(NOT(ISBLANK(B19)),"                    .AddWithValue(""@"&amp;B19&amp;""", value.Id,  SqlDbType.Int"&amp;")"&amp;IF(LEN(Z92)&gt;0,"",";"),"")</f>
+        <f t="shared" ref="Z91:Z95" si="19">IF(NOT(ISBLANK(B19)),"                    .AddWithValue(""@"&amp;B19&amp;""", value.Id,  SqlDbType.Int"&amp;")"&amp;IF(LEN(Z92)&gt;0,"",";"),"")</f>
         <v/>
       </c>
     </row>
     <row r="92" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z92" s="13" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z93" s="13" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z94" s="13" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z95" s="13" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z96" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z98" s="13" t="str">
         <f>"                return new DataResult&lt;"&amp;C2&amp;"&gt;(value, result);"</f>
-        <v>                return new DataResult&lt;Deities&gt;(value, result);</v>
+        <v>                return new DataResult&lt;Shops&gt;(value, result);</v>
       </c>
     </row>
     <row r="99" spans="26:26" x14ac:dyDescent="0.25">
@@ -3242,22 +3235,22 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="J2" s="3" t="str">
         <f>A2&amp;" ["&amp;B2&amp;"].["&amp;C2&amp;"]"</f>
-        <v>CREATE TABLE [dbo].[CompassionLevels]</v>
+        <v>CREATE TABLE [dbo].[MapAreaTypes]</v>
       </c>
       <c r="L2" s="4" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_CreateUpdate]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_CompassionLevels_CreateUpdate]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_MapAreaTypes_CreateUpdate]</v>
       </c>
       <c r="N2" s="18" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Get]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_CompassionLevels_Get]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_MapAreaTypes_Get]</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>46</v>
@@ -3303,11 +3296,11 @@
       </c>
       <c r="L3" s="4" t="str">
         <f>IF(NOT(ISBLANK(B4)),"@"&amp;B4&amp;" "&amp;UPPER(C4)&amp;" = NULL OUTPUT,","")</f>
-        <v>@CompassionLevelId INT = NULL OUTPUT,</v>
+        <v>@MapAreaTypeId INT = NULL OUTPUT,</v>
       </c>
       <c r="N3" s="18" t="str">
         <f>"@"&amp;C2&amp;"Id"&amp;" INT"</f>
-        <v>@CompassionLevelsId INT</v>
+        <v>@MapAreaTypesId INT</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>47</v>
@@ -3328,7 +3321,7 @@
       </c>
       <c r="B4" s="14" t="str">
         <f>LEFT(C2,LEN(C2)-1)&amp;"Id"</f>
-        <v>CompassionLevelId</v>
+        <v>MapAreaTypeId</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>6</v>
@@ -3343,7 +3336,7 @@
       <c r="H4" s="14"/>
       <c r="J4" s="3" t="str">
         <f>"    "&amp;B4&amp;" "&amp;UPPER(C4)&amp;IF(E4," NOT NULL","")&amp;IF(D4," IDENTITY(1,1)","")&amp;IF(NOT(ISBLANK(F4))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_PK PRIMARY KEY","")&amp;IF(LEN(G4)&gt;0," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_FK FOREIGN KEY REFERENCES "&amp;G4,"")&amp;IF(NOT(ISBLANK(H4))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_DF DEFAULT("&amp;H4&amp;")","")&amp;IF(NOT(ISBLANK(B5)),",","")</f>
-        <v xml:space="preserve">    CompassionLevelId INT IDENTITY(1,1) CONSTRAINT CompassionLevels_CompassionLevelId_PK PRIMARY KEY,</v>
+        <v xml:space="preserve">    MapAreaTypeId INT IDENTITY(1,1) CONSTRAINT MapAreaTypes_MapAreaTypeId_PK PRIMARY KEY,</v>
       </c>
       <c r="L4" s="4" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
@@ -3371,10 +3364,10 @@
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="b">
@@ -3382,7 +3375,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" t="str">
-        <f>IF(UPPER(RIGHT(B5,2))="ID",B$2&amp;"."&amp;LEFT(B5,LEN(B5)-2)&amp;"("&amp;B5&amp;")","")</f>
+        <f>IF(UPPER(RIGHT(B5,2))="ID",B$2&amp;"."&amp;LEFT(B5,LEN(B5)-2)&amp;"s("&amp;B5&amp;")","")</f>
         <v/>
       </c>
       <c r="H5" s="2"/>
@@ -3417,7 +3410,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" t="str">
-        <f t="shared" ref="G6:G20" si="2">IF(UPPER(RIGHT(B6,2))="ID",B$2&amp;"."&amp;LEFT(B6,LEN(B6)-2)&amp;"("&amp;B6&amp;")","")</f>
+        <f t="shared" ref="G6:G20" si="2">IF(UPPER(RIGHT(B6,2))="ID",B$2&amp;"."&amp;LEFT(B6,LEN(B6)-2)&amp;"s("&amp;B6&amp;")","")</f>
         <v/>
       </c>
       <c r="H6" s="2"/>
@@ -3443,7 +3436,7 @@
       </c>
       <c r="V6" s="12" t="str">
         <f>"    public interface I"&amp;C2&amp;"Repository"</f>
-        <v>    public interface ICompassionLevelsRepository</v>
+        <v>    public interface IMapAreaTypesRepository</v>
       </c>
       <c r="X6" s="13" t="s">
         <v>67</v>
@@ -3470,7 +3463,7 @@
       </c>
       <c r="N7" s="18" t="str">
         <f>IF(NOT(ISBLANK(B4)),"    ["&amp;B4&amp;"]"&amp;IF(LEN(N8)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">    [CompassionLevelId],</v>
+        <v xml:space="preserve">    [MapAreaTypeId],</v>
       </c>
       <c r="P7" s="5" t="str">
         <f>"namespace Dots.Domain."&amp;B2</f>
@@ -3521,11 +3514,11 @@
       </c>
       <c r="T8" s="16" t="str">
         <f>"    public static class "&amp;C2&amp;"Helper"</f>
-        <v>    public static class CompassionLevelsHelper</v>
+        <v>    public static class MapAreaTypesHelper</v>
       </c>
       <c r="V8" s="12" t="str">
         <f>"        I"&amp;C2&amp;" Get(int "&amp;LOWER(C2)&amp;"Id);"</f>
-        <v>        ICompassionLevels Get(int compassionlevelsId);</v>
+        <v>        IMapAreaTypes Get(int mapareatypesId);</v>
       </c>
       <c r="X8" s="13" t="str">
         <f>"namespace Dots.Domain.Repositories."&amp;B2</f>
@@ -3557,11 +3550,11 @@
       </c>
       <c r="P9" s="5" t="str">
         <f>"    public interface I"&amp;C2&amp;" : IEntity"</f>
-        <v>    public interface ICompassionLevels : IEntity</v>
+        <v>    public interface IMapAreaTypes : IEntity</v>
       </c>
       <c r="R9" s="6" t="str">
         <f>"    public class "&amp;C2&amp;" : I"&amp;C2</f>
-        <v>    public class CompassionLevels : ICompassionLevels</v>
+        <v>    public class MapAreaTypes : IMapAreaTypes</v>
       </c>
       <c r="T9" s="16" t="s">
         <v>51</v>
@@ -3604,15 +3597,15 @@
       </c>
       <c r="T10" s="16" t="str">
         <f>"        public static I"&amp;C2&amp;" ParseReader(IDataReader reader)"</f>
-        <v>        public static ICompassionLevels ParseReader(IDataReader reader)</v>
+        <v>        public static IMapAreaTypes ParseReader(IDataReader reader)</v>
       </c>
       <c r="V10" s="12" t="str">
         <f>"        DataResult&lt;I"&amp;C2&amp;"&gt; Save(I"&amp;C2&amp;" "&amp;LOWER(C2)&amp;");"</f>
-        <v>        DataResult&lt;ICompassionLevels&gt; Save(ICompassionLevels compassionlevels);</v>
+        <v>        DataResult&lt;IMapAreaTypes&gt; Save(IMapAreaTypes mapareatypes);</v>
       </c>
       <c r="X10" s="13" t="str">
         <f>"    public class Sql"&amp;C2&amp;"Repository : Repository&lt;I"&amp;C2&amp;"&gt;, I"&amp;C2&amp;"Repository"</f>
-        <v>    public class SqlCompassionLevelsRepository : Repository&lt;ICompassionLevels&gt;, ICompassionLevelsRepository</v>
+        <v>    public class SqlMapAreaTypesRepository : Repository&lt;IMapAreaTypes&gt;, IMapAreaTypesRepository</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
@@ -3688,14 +3681,14 @@
       </c>
       <c r="T12" s="16" t="str">
         <f>"            return new "&amp;C2&amp;"("</f>
-        <v>            return new CompassionLevels(</v>
+        <v>            return new MapAreaTypes(</v>
       </c>
       <c r="V12" s="12" t="s">
         <v>55</v>
       </c>
       <c r="X12" s="13" t="str">
         <f>"        public Sql"&amp;C2&amp;"Repository(IUnitOfWork unitOfWork)"</f>
-        <v>        public SqlCompassionLevelsRepository(IUnitOfWork unitOfWork)</v>
+        <v>        public SqlMapAreaTypesRepository(IUnitOfWork unitOfWork)</v>
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
@@ -3735,7 +3728,7 @@
       </c>
       <c r="T13" s="16" t="str">
         <f>"                reader.Get&lt;int&gt;("&amp;C2&amp;"Col.Id),"</f>
-        <v xml:space="preserve">                reader.Get&lt;int&gt;(CompassionLevelsCol.Id),</v>
+        <v xml:space="preserve">                reader.Get&lt;int&gt;(MapAreaTypesCol.Id),</v>
       </c>
       <c r="X13" s="13" t="s">
         <v>68</v>
@@ -3908,7 +3901,7 @@
       </c>
       <c r="X17" s="13" t="str">
         <f>"        protected override I"&amp;C2&amp;" Map(IDataReader reader)"</f>
-        <v xml:space="preserve">        protected override ICompassionLevels Map(IDataReader reader)</v>
+        <v xml:space="preserve">        protected override IMapAreaTypes Map(IDataReader reader)</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
@@ -3995,7 +3988,7 @@
       </c>
       <c r="X19" s="13" t="str">
         <f>"           return "&amp;C2&amp;"Helper.ParseReader(reader);"</f>
-        <v>           return CompassionLevelsHelper.ParseReader(reader);</v>
+        <v>           return MapAreaTypesHelper.ParseReader(reader);</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
@@ -4095,7 +4088,7 @@
       </c>
       <c r="X22" s="13" t="str">
         <f>"        public I"&amp;C2&amp;" Get(int "&amp;LOWER(C2)&amp;"Id)"</f>
-        <v>        public ICompassionLevels Get(int compassionlevelsId)</v>
+        <v>        public IMapAreaTypes Get(int mapareatypesId)</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
@@ -4108,7 +4101,7 @@
       </c>
       <c r="L23" s="4" t="str">
         <f>"SELECT "&amp;B4</f>
-        <v>SELECT CompassionLevelId</v>
+        <v>SELECT MapAreaTypeId</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="4"/>
@@ -4133,7 +4126,7 @@
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L24" s="4" t="str">
         <f>"FROM "&amp;B2&amp;"."&amp;C2</f>
-        <v>FROM dbo.CompassionLevels</v>
+        <v>FROM dbo.MapAreaTypes</v>
       </c>
       <c r="N24" s="18" t="s">
         <v>90</v>
@@ -4156,7 +4149,7 @@
       </c>
       <c r="X24" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Get""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_CompassionLevels_Get"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_MapAreaTypes_Get"))</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
@@ -4169,18 +4162,18 @@
       </c>
       <c r="C25" t="str">
         <f>"Trigger_"&amp;C2&amp;"_AuditData"</f>
-        <v>Trigger_CompassionLevels_AuditData</v>
+        <v>Trigger_MapAreaTypes_AuditData</v>
       </c>
       <c r="J25" s="3" t="str">
         <f>A25&amp;" ["&amp;B25&amp;"].["&amp;C25&amp;"] ON ["&amp;B2&amp;"].["&amp;C2&amp;"]"</f>
-        <v>CREATE TRIGGER [dbo].[Trigger_CompassionLevels_AuditData] ON [dbo].[CompassionLevels]</v>
+        <v>CREATE TRIGGER [dbo].[Trigger_MapAreaTypes_AuditData] ON [dbo].[MapAreaTypes]</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>40</v>
       </c>
       <c r="N25" s="18" t="str">
         <f>"    "&amp;B2&amp;"."&amp;C2</f>
-        <v xml:space="preserve">    dbo.CompassionLevels</v>
+        <v xml:space="preserve">    dbo.MapAreaTypes</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="4"/>
@@ -4212,7 +4205,7 @@
       </c>
       <c r="L26" s="4" t="str">
         <f>IF(NOT(ISBLANK(B4)),"["&amp;B4&amp;"] = ISNULL(@"&amp;B4&amp;", 0)","")</f>
-        <v>[CompassionLevelId] = ISNULL(@CompassionLevelId, 0)</v>
+        <v>[MapAreaTypeId] = ISNULL(@MapAreaTypeId, 0)</v>
       </c>
       <c r="N26" s="18" t="s">
         <v>40</v>
@@ -4250,7 +4243,7 @@
       </c>
       <c r="N27" s="18" t="str">
         <f>"    "&amp;B4&amp;" = @"&amp;B4</f>
-        <v xml:space="preserve">    CompassionLevelId = @CompassionLevelId</v>
+        <v xml:space="preserve">    MapAreaTypeId = @MapAreaTypeId</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="4"/>
@@ -4270,7 +4263,7 @@
       </c>
       <c r="X27" s="13" t="str">
         <f>"                    .AddWithValue(""@"&amp;C2&amp;"Id"", "&amp;LOWER(C2)&amp;"Id, DbType.Int32);"</f>
-        <v>                    .AddWithValue("@CompassionLevelsId", compassionlevelsId, DbType.Int32);</v>
+        <v>                    .AddWithValue("@MapAreaTypesId", mapareatypesId, DbType.Int32);</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
@@ -4302,14 +4295,14 @@
       </c>
       <c r="L29" s="4" t="str">
         <f>"INSERT INTO "&amp;B2&amp;"."&amp;C2&amp;" ("</f>
-        <v>INSERT INTO dbo.CompassionLevels (</v>
+        <v>INSERT INTO dbo.MapAreaTypes (</v>
       </c>
       <c r="P29" s="5" t="s">
         <v>55</v>
       </c>
       <c r="R29" s="6" t="str">
         <f>"        public "&amp;C2&amp;"("</f>
-        <v>        public CompassionLevels(</v>
+        <v>        public MapAreaTypes(</v>
       </c>
       <c r="T29" s="16" t="str">
         <f t="shared" si="7"/>
@@ -4333,7 +4326,7 @@
       </c>
       <c r="R30" s="6" t="str">
         <f>IF(NOT(ISBLANK(B4)),"            int"&amp;" "&amp;LOWER(LEFT(B4,1))&amp;MID(B4,2,LEN(B4)-1)&amp;IF(LEN(R31)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            int compassionLevelId,</v>
+        <v xml:space="preserve">            int mapAreaTypeId,</v>
       </c>
       <c r="X30" s="13" t="s">
         <v>72</v>
@@ -4403,7 +4396,7 @@
       </c>
       <c r="X33" s="13" t="str">
         <f>"        public DataResult&lt;I"&amp;C2&amp;"&gt; Save(I"&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;ICompassionLevels&gt; Save(ICompassionLevels value)</v>
+        <v xml:space="preserve">        public DataResult&lt;IMapAreaTypes&gt; Save(IMapAreaTypes value)</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
@@ -4424,7 +4417,7 @@
       </c>
       <c r="T34" s="16" t="str">
         <f>"        public static IEnumerable&lt;I"&amp;C2&amp;"&gt; ParseMultipleReader(IDataReader reader)"</f>
-        <v>        public static IEnumerable&lt;ICompassionLevels&gt; ParseMultipleReader(IDataReader reader)</v>
+        <v>        public static IEnumerable&lt;IMapAreaTypes&gt; ParseMultipleReader(IDataReader reader)</v>
       </c>
       <c r="X34" s="13" t="s">
         <v>52</v>
@@ -4451,7 +4444,7 @@
       </c>
       <c r="X35" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Save""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_CompassionLevels_Save"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_MapAreaTypes_Save"))</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
@@ -4473,7 +4466,7 @@
       </c>
       <c r="T36" s="16" t="str">
         <f>"            var "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;"s = new List&lt;I"&amp;C2&amp;"&gt;();"</f>
-        <v>            var compassionLevelss = new List&lt;ICompassionLevels&gt;();</v>
+        <v>            var mapAreaTypess = new List&lt;IMapAreaTypes&gt;();</v>
       </c>
       <c r="X36" s="13" t="s">
         <v>69</v>
@@ -4482,11 +4475,11 @@
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>"        SELECT 'INSERT', @Token, '["&amp;B$2&amp;"]', '["&amp;C$2&amp;"]', P."&amp;B$4&amp;", DATA = ("</f>
-        <v xml:space="preserve">        SELECT 'INSERT', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'INSERT', @Token, '[dbo]', '[MapAreaTypes]', P.MapAreaTypeId, DATA = (</v>
       </c>
       <c r="J37" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">        SELECT 'INSERT', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'INSERT', @Token, '[dbo]', '[MapAreaTypes]', P.MapAreaTypeId, DATA = (</v>
       </c>
       <c r="L37" s="4" t="str">
         <f t="shared" si="10"/>
@@ -4501,7 +4494,7 @@
       </c>
       <c r="X37" s="13" t="str">
         <f>"                var idParameter = command.AddOutput(""@"&amp;C2&amp;"Id"", DbType.Int32);"</f>
-        <v>                var idParameter = command.AddOutput("@CompassionLevelsId", DbType.Int32);</v>
+        <v>                var idParameter = command.AddOutput("@MapAreaTypesId", DbType.Int32);</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
@@ -4548,17 +4541,17 @@
       </c>
       <c r="X39" s="13" t="str">
         <f>IF(NOT(ISBLANK(B4)),"                    .AddWithValue(""@"&amp;B4&amp;""", value.Id, DbType.Int32"&amp;")"&amp;IF(LEN(X40)&gt;0,"",";"),"")</f>
-        <v>                    .AddWithValue("@CompassionLevelId", value.Id, DbType.Int32)</v>
+        <v>                    .AddWithValue("@MapAreaTypeId", value.Id, DbType.Int32)</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>"                WHERE Record."&amp;B$4&amp;" = P."&amp;B$4</f>
-        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
+        <v xml:space="preserve">                WHERE Record.MapAreaTypeId = P.MapAreaTypeId</v>
       </c>
       <c r="J40" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
+        <v xml:space="preserve">                WHERE Record.MapAreaTypeId = P.MapAreaTypeId</v>
       </c>
       <c r="L40" s="4" t="str">
         <f t="shared" si="10"/>
@@ -4570,7 +4563,7 @@
       </c>
       <c r="T40" s="16" t="str">
         <f>"                "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;"s.Add(ParseReader(reader));"</f>
-        <v>                compassionLevelss.Add(ParseReader(reader));</v>
+        <v>                mapAreaTypess.Add(ParseReader(reader));</v>
       </c>
       <c r="X40" s="13" t="str">
         <f t="shared" ref="X40:X55" si="12">IF(NOT(ISBLANK(B5)),"                    .AddWithValue(""@"&amp;B5&amp;""", value."&amp;B5&amp;", DbType."&amp;IF(NOT(OR(ISBLANK(Q12),Q12="int")),UPPER(LEFT(Q12,1))&amp;MID(Q12,2,LEN(Q12)-1),"Int32")&amp;")"&amp;IF(LEFT(X41,24)="                    .Add","",";"),"")</f>
@@ -4643,7 +4636,7 @@
       </c>
       <c r="T43" s="16" t="str">
         <f>"            return "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;"s;"</f>
-        <v>            return compassionLevelss;</v>
+        <v>            return mapAreaTypess;</v>
       </c>
       <c r="X43" s="13" t="str">
         <f t="shared" si="12"/>
@@ -4715,7 +4708,7 @@
       </c>
       <c r="T46" s="16" t="str">
         <f>"        private enum "&amp;C2&amp;"Col"</f>
-        <v>        private enum CompassionLevelsCol</v>
+        <v>        private enum MapAreaTypesCol</v>
       </c>
       <c r="X46" s="13" t="str">
         <f t="shared" si="12"/>
@@ -4781,7 +4774,7 @@
       </c>
       <c r="R49" s="6" t="str">
         <f>IF(NOT(ISBLANK(B4)),"            Id = "&amp;LOWER(LEFT(B4,1))&amp;MID(B4,2,LEN(B4)-1)&amp;";","")</f>
-        <v xml:space="preserve">            Id = compassionLevelId;</v>
+        <v xml:space="preserve">            Id = mapAreaTypeId;</v>
       </c>
       <c r="T49" s="16" t="str">
         <f t="shared" ref="T49:T64" si="14">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;IF(LEN(T15)&gt;0,",",""),"")</f>
@@ -4821,11 +4814,11 @@
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>"        SELECT 'DELETE', @Token, '["&amp;B$2&amp;"]', '["&amp;C$2&amp;"]', P."&amp;B$4&amp;", DATA = ("</f>
-        <v xml:space="preserve">        SELECT 'DELETE', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'DELETE', @Token, '[dbo]', '[MapAreaTypes]', P.MapAreaTypeId, DATA = (</v>
       </c>
       <c r="J51" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">        SELECT 'DELETE', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'DELETE', @Token, '[dbo]', '[MapAreaTypes]', P.MapAreaTypeId, DATA = (</v>
       </c>
       <c r="L51" s="4" t="str">
         <f>IF(NOT(ISBLANK(B8)),"@"&amp;B8&amp;IF(NOT(ISBLANK(B9)),",",""),"")</f>
@@ -4897,11 +4890,11 @@
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>"                WHERE Record."&amp;B$4&amp;" = P."&amp;B$4</f>
-        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
+        <v xml:space="preserve">                WHERE Record.MapAreaTypeId = P.MapAreaTypeId</v>
       </c>
       <c r="J54" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
+        <v xml:space="preserve">                WHERE Record.MapAreaTypeId = P.MapAreaTypeId</v>
       </c>
       <c r="L54" s="4" t="str">
         <f t="shared" si="13"/>
@@ -5158,11 +5151,11 @@
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>"        SELECT 'UPDATE', @Token, '["&amp;B$2&amp;"]', '["&amp;C$2&amp;"]', P."&amp;B$4&amp;", DATA = ("</f>
-        <v xml:space="preserve">        SELECT 'UPDATE', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'UPDATE', @Token, '[dbo]', '[MapAreaTypes]', P.MapAreaTypeId, DATA = (</v>
       </c>
       <c r="J65" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">        SELECT 'UPDATE', @Token, '[dbo]', '[CompassionLevels]', P.CompassionLevelId, DATA = (</v>
+        <v xml:space="preserve">        SELECT 'UPDATE', @Token, '[dbo]', '[MapAreaTypes]', P.MapAreaTypeId, DATA = (</v>
       </c>
       <c r="R65" s="6" t="str">
         <f t="shared" si="15"/>
@@ -5185,7 +5178,7 @@
       </c>
       <c r="L66" s="4" t="str">
         <f>"SELECT @"&amp;B4&amp;" = SCOPE_IDENTITY()"</f>
-        <v>SELECT @CompassionLevelId = SCOPE_IDENTITY()</v>
+        <v>SELECT @MapAreaTypeId = SCOPE_IDENTITY()</v>
       </c>
       <c r="T66" s="16" t="s">
         <v>54</v>
@@ -5215,11 +5208,11 @@
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>"                WHERE Record."&amp;B$4&amp;" = P."&amp;B$4</f>
-        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
+        <v xml:space="preserve">                WHERE Record.MapAreaTypeId = P.MapAreaTypeId</v>
       </c>
       <c r="J68" s="3" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">                WHERE Record.CompassionLevelId = P.CompassionLevelId</v>
+        <v xml:space="preserve">                WHERE Record.MapAreaTypeId = P.MapAreaTypeId</v>
       </c>
       <c r="L68" s="4" t="s">
         <v>43</v>
@@ -5277,7 +5270,7 @@
       </c>
       <c r="L72" s="4" t="str">
         <f>"UPDATE "&amp;B2&amp;"."&amp;C2</f>
-        <v>UPDATE dbo.CompassionLevels</v>
+        <v>UPDATE dbo.MapAreaTypes</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
@@ -5403,7 +5396,7 @@
     <row r="91" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L91" s="4" t="str">
         <f>"["&amp;B4&amp;"] = @"&amp;B4</f>
-        <v>[CompassionLevelId] = @CompassionLevelId</v>
+        <v>[MapAreaTypeId] = @MapAreaTypeId</v>
       </c>
     </row>
     <row r="93" spans="12:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added first set of repositories and models. Made a start on the interface.
</commit_message>
<xml_diff>
--- a/Table Creator.xlsx
+++ b/Table Creator.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\PersonalProjects\DungeonsAndDragons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DungeonsAndDragons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Games" sheetId="8" r:id="rId1"/>
     <sheet name="Enum Tables" sheetId="12" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="105">
   <si>
     <t>Fields</t>
   </si>
@@ -339,19 +339,13 @@
     <t>CompassionLevels</t>
   </si>
   <si>
-    <t>Games</t>
-  </si>
-  <si>
-    <t>StartDate</t>
-  </si>
-  <si>
-    <t>datetime2(3)</t>
+    <t>Ts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,6 +593,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -634,6 +645,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -788,12 +816,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -891,19 +921,19 @@
       </c>
       <c r="J2" s="3" t="str">
         <f>A2&amp;" ["&amp;B2&amp;"].["&amp;C2&amp;"]"</f>
-        <v>CREATE TABLE [dbo].[Games]</v>
+        <v>CREATE TABLE [dbo].[Ts]</v>
       </c>
       <c r="L2" s="22" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Create]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_Games_Create]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_Ts_Create]</v>
       </c>
       <c r="N2" s="23" t="str">
         <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Update]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_Games_Update]</v>
+        <v>CREATE PROCEDURE [dbo].[USP_Ts_Update]</v>
       </c>
       <c r="P2" s="18" t="str">
-        <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_Get]"</f>
-        <v>CREATE PROCEDURE [dbo].[USP_Games_Get]</v>
+        <f>"CREATE PROCEDURE"&amp;" ["&amp;B2&amp;"].[USP_"&amp;C2&amp;"_GetById]"</f>
+        <v>CREATE PROCEDURE [dbo].[USP_Ts_GetById]</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>46</v>
@@ -949,15 +979,15 @@
       </c>
       <c r="L3" s="22" t="str">
         <f>IF(NOT(ISBLANK(B4)),"@"&amp;B4&amp;" "&amp;UPPER(C4)&amp;" = NULL OUTPUT,","")</f>
-        <v>@GameId INT = NULL OUTPUT,</v>
+        <v>@TId INT = NULL OUTPUT,</v>
       </c>
       <c r="N3" s="23" t="str">
         <f>IF(NOT(ISBLANK(B4)),"@"&amp;B4&amp;" "&amp;UPPER(C4)&amp;",","")</f>
-        <v>@GameId INT,</v>
+        <v>@TId INT,</v>
       </c>
       <c r="P3" s="18" t="str">
-        <f>"@"&amp;C2&amp;"Id"&amp;" INT"</f>
-        <v>@GamesId INT</v>
+        <f>IF(NOT(ISBLANK(B4)),"@"&amp;B4)</f>
+        <v>@TId</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>47</v>
@@ -978,7 +1008,7 @@
       </c>
       <c r="B4" s="14" t="str">
         <f>IF(NOT(ISBLANK(B3)),B3,LEFT(C2,LEN(C2)-1)&amp;"Id")</f>
-        <v>GameId</v>
+        <v>TId</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>6</v>
@@ -993,15 +1023,15 @@
       <c r="H4" s="14"/>
       <c r="J4" s="3" t="str">
         <f>"    "&amp;B4&amp;" "&amp;UPPER(C4)&amp;IF(E4," NOT NULL","")&amp;IF(D4," IDENTITY(1,1)","")&amp;IF(NOT(ISBLANK(F4))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_PK PRIMARY KEY","")&amp;IF(LEN(G4)&gt;0," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_FK FOREIGN KEY REFERENCES "&amp;G4,"")&amp;IF(NOT(ISBLANK(H4))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B4&amp;"_DF DEFAULT("&amp;H4&amp;")","")&amp;IF(NOT(ISBLANK(B5)),",","")</f>
-        <v xml:space="preserve">    GameId INT IDENTITY(1,1) CONSTRAINT Games_GameId_PK PRIMARY KEY,</v>
+        <v xml:space="preserve">    TId INT IDENTITY(1,1) CONSTRAINT Ts_TId_PK PRIMARY KEY</v>
       </c>
       <c r="L4" s="22" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@Name VARCHAR(50),</v>
+        <v/>
       </c>
       <c r="N4" s="23" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@Name VARCHAR(50),</v>
+        <v/>
       </c>
       <c r="P4" s="18" t="s">
         <v>38</v>
@@ -1024,12 +1054,8 @@
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1040,15 +1066,15 @@
       <c r="H5" s="19"/>
       <c r="J5" s="3" t="str">
         <f t="shared" ref="J5:J32" si="0">"    "&amp;B5&amp;" "&amp;UPPER(C5)&amp;IF(E5," NOT NULL","")&amp;IF(D5," IDENTITY(1,1)","")&amp;IF(NOT(ISBLANK(F5))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_PK PRIMARY KEY","")&amp;IF(LEN(G5)&gt;0," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_FK FOREIGN KEY REFERENCES "&amp;G5,"")&amp;IF(NOT(ISBLANK(H5))," CONSTRAINT "&amp;C$2&amp;"_"&amp;B5&amp;"_DF DEFAULT("&amp;H5&amp;")","")&amp;IF(NOT(ISBLANK(B6)),",","")</f>
-        <v xml:space="preserve">    Name VARCHAR(50),</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L5" s="22" t="str">
         <f t="shared" ref="L5:L19" si="1">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;" "&amp;UPPER(C6)&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>@StartDate DATETIME2(3)</v>
+        <v/>
       </c>
       <c r="N5" s="23" t="str">
         <f t="shared" ref="N5:N19" si="2">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;" "&amp;UPPER(C6)&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>@StartDate DATETIME2(3)</v>
+        <v/>
       </c>
       <c r="R5" s="5" t="s">
         <v>49</v>
@@ -1067,12 +1093,8 @@
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1083,7 +1105,7 @@
       <c r="H6" s="19"/>
       <c r="J6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    StartDate DATETIME2(3)</v>
+        <v xml:space="preserve">     </v>
       </c>
       <c r="L6" s="22" t="str">
         <f t="shared" si="1"/>
@@ -1108,7 +1130,7 @@
       </c>
       <c r="X6" s="12" t="str">
         <f>"    public interface I"&amp;C2&amp;"Repository"</f>
-        <v>    public interface IGamesRepository</v>
+        <v>    public interface ITsRepository</v>
       </c>
       <c r="Z6" s="13" t="s">
         <v>67</v>
@@ -1139,7 +1161,7 @@
       </c>
       <c r="P7" s="18" t="str">
         <f>IF(NOT(ISBLANK(B4)),"    ["&amp;B4&amp;"]"&amp;IF(LEN(P8)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">    [GameId],</v>
+        <v xml:space="preserve">    [TId]</v>
       </c>
       <c r="R7" s="5" t="str">
         <f>"namespace Dots.Domain."&amp;B2</f>
@@ -1184,7 +1206,7 @@
       </c>
       <c r="P8" s="18" t="str">
         <f t="shared" ref="P8:P22" si="4">IF(NOT(ISBLANK(B5)),"    ["&amp;B5&amp;"]"&amp;IF(LEN(P9)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">    [Name],</v>
+        <v/>
       </c>
       <c r="R8" s="5" t="s">
         <v>50</v>
@@ -1194,11 +1216,11 @@
       </c>
       <c r="V8" s="16" t="str">
         <f>"    public static class "&amp;C2&amp;"Helper"</f>
-        <v>    public static class GamesHelper</v>
+        <v>    public static class TsHelper</v>
       </c>
       <c r="X8" s="12" t="str">
         <f>"        "&amp;C2&amp;" Get(int "&amp;LOWER(C2)&amp;"Id);"</f>
-        <v>        Games Get(int gamesId);</v>
+        <v>        Ts Get(int tsId);</v>
       </c>
       <c r="Z8" s="13" t="str">
         <f>"namespace Dots.Domain.Repositories."&amp;B2&amp;"s"</f>
@@ -1230,15 +1252,15 @@
       </c>
       <c r="P9" s="18" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    [StartDate]</v>
+        <v/>
       </c>
       <c r="R9" s="5" t="str">
         <f>"    public interface I"&amp;C2&amp;" : IEntity"</f>
-        <v>    public interface IGames : IEntity</v>
+        <v>    public interface ITs : IEntity</v>
       </c>
       <c r="T9" s="6" t="str">
         <f>"    public class "&amp;C2&amp;" : IEntity"</f>
-        <v>    public class Games : IEntity</v>
+        <v>    public class Ts : IEntity</v>
       </c>
       <c r="V9" s="16" t="s">
         <v>51</v>
@@ -1285,15 +1307,15 @@
       </c>
       <c r="V10" s="16" t="str">
         <f>"        public static "&amp;C2&amp;" ParseReader(IDataReader reader)"</f>
-        <v>        public static Games ParseReader(IDataReader reader)</v>
+        <v>        public static Ts ParseReader(IDataReader reader)</v>
       </c>
       <c r="X10" s="12" t="str">
         <f>"        DataResult&lt;"&amp;C2&amp;"&gt; Save("&amp;C2&amp;" "&amp;LOWER(C2)&amp;");"</f>
-        <v>        DataResult&lt;Games&gt; Save(Games games);</v>
+        <v>        DataResult&lt;Ts&gt; Save(Ts ts);</v>
       </c>
       <c r="Z10" s="13" t="str">
         <f>"    public class Sql"&amp;C2&amp;"Repository : Repository&lt;"&amp;C2&amp;"&gt;, I"&amp;C2&amp;"Repository"</f>
-        <v>    public class SqlGamesRepository : Repository&lt;Games&gt;, IGamesRepository</v>
+        <v>    public class SqlTsRepository : Repository&lt;Ts&gt;, ITsRepository</v>
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
@@ -1365,26 +1387,26 @@
       </c>
       <c r="Q12" t="str">
         <f t="shared" ref="Q12:Q27" si="5">IF(NOT(ISBLANK(C5)),C5,"")</f>
-        <v>varchar(50)</v>
+        <v/>
       </c>
       <c r="R12" s="5" t="str">
         <f t="shared" ref="R12:R27" si="6">IF(NOT(ISBLANK(C5)),"        "&amp;IF(ISBLANK(S12),C5,S12)&amp;" "&amp;B5&amp;" { get; set; }","")</f>
-        <v xml:space="preserve">        varchar(50) Name { get; set; }</v>
+        <v/>
       </c>
       <c r="T12" s="6" t="str">
         <f t="shared" ref="T12:T27" si="7">IF(LEN(R12)&gt;0,"        public "&amp;TRIM(R12),"")</f>
-        <v xml:space="preserve">        public varchar(50) Name { get; set; }</v>
+        <v/>
       </c>
       <c r="V12" s="16" t="str">
         <f>"            return new "&amp;C2&amp;"("</f>
-        <v>            return new Games(</v>
+        <v>            return new Ts(</v>
       </c>
       <c r="X12" s="12" t="s">
         <v>55</v>
       </c>
       <c r="Z12" s="13" t="str">
         <f>"        public Sql"&amp;C2&amp;"Repository(IUnitOfWork unitOfWork)"</f>
-        <v>        public SqlGamesRepository(IUnitOfWork unitOfWork)</v>
+        <v>        public SqlTsRepository(IUnitOfWork unitOfWork)</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
@@ -1416,19 +1438,19 @@
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="5"/>
-        <v>datetime2(3)</v>
+        <v/>
       </c>
       <c r="R13" s="5" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">        datetime2(3) StartDate { get; set; }</v>
+        <v/>
       </c>
       <c r="T13" s="6" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">        public datetime2(3) StartDate { get; set; }</v>
+        <v/>
       </c>
       <c r="V13" s="16" t="str">
         <f>"                reader.Get&lt;int&gt;("&amp;C2&amp;"Col.Id),"</f>
-        <v xml:space="preserve">                reader.Get&lt;int&gt;(GamesCol.Id),</v>
+        <v xml:space="preserve">                reader.Get&lt;int&gt;(TsCol.Id),</v>
       </c>
       <c r="Z13" s="13" t="s">
         <v>68</v>
@@ -1617,7 +1639,7 @@
       </c>
       <c r="Z17" s="13" t="str">
         <f>"        protected override "&amp;C2&amp;" Map(IDataReader reader)"</f>
-        <v xml:space="preserve">        protected override Games Map(IDataReader reader)</v>
+        <v xml:space="preserve">        protected override Ts Map(IDataReader reader)</v>
       </c>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
@@ -1712,7 +1734,7 @@
       </c>
       <c r="Z19" s="13" t="str">
         <f>"           return "&amp;C2&amp;"Helper.ParseReader(reader);"</f>
-        <v>           return GamesHelper.ParseReader(reader);</v>
+        <v>           return TsHelper.ParseReader(reader);</v>
       </c>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.25">
@@ -1839,7 +1861,7 @@
       </c>
       <c r="Z22" s="13" t="str">
         <f>"        public "&amp;C2&amp;" Get(int "&amp;LOWER(C2)&amp;"Id)"</f>
-        <v>        public Games Get(int gamesId)</v>
+        <v>        public Ts Get(int tsId)</v>
       </c>
     </row>
     <row r="23" spans="2:26" x14ac:dyDescent="0.25">
@@ -1862,7 +1884,7 @@
       </c>
       <c r="N23" s="23" t="str">
         <f>"UPDATE "&amp;B2&amp;"."&amp;C2</f>
-        <v>UPDATE dbo.Games</v>
+        <v>UPDATE dbo.Ts</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="5"/>
@@ -1901,7 +1923,7 @@
       </c>
       <c r="L24" s="22" t="str">
         <f>"FROM "&amp;B2&amp;"."&amp;C2</f>
-        <v>FROM dbo.Games</v>
+        <v>FROM dbo.Ts</v>
       </c>
       <c r="N24" s="23" t="s">
         <v>45</v>
@@ -1927,7 +1949,7 @@
       </c>
       <c r="Z24" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Get""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Games_Get"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Ts_Get"))</v>
       </c>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.25">
@@ -1950,11 +1972,11 @@
       </c>
       <c r="N25" s="23" t="str">
         <f t="shared" ref="N25:N40" si="9">IF(NOT(ISBLANK(B5)),"["&amp;B5&amp;"] = @"&amp;B5&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>[Name] = @Name,</v>
+        <v/>
       </c>
       <c r="P25" s="18" t="str">
         <f>"    "&amp;B2&amp;"."&amp;C2</f>
-        <v xml:space="preserve">    dbo.Games</v>
+        <v xml:space="preserve">    dbo.Ts</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="5"/>
@@ -1993,11 +2015,11 @@
       </c>
       <c r="L26" s="22" t="str">
         <f>IF(NOT(ISBLANK(B4)),"["&amp;B4&amp;"] = ISNULL(@"&amp;B4&amp;", 0)","")</f>
-        <v>[GameId] = ISNULL(@GameId, 0)</v>
+        <v>[TId] = ISNULL(@TId, 0)</v>
       </c>
       <c r="N26" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>[StartDate] = @StartDate</v>
+        <v/>
       </c>
       <c r="P26" s="18" t="s">
         <v>40</v>
@@ -2046,7 +2068,7 @@
       </c>
       <c r="P27" s="18" t="str">
         <f>"    "&amp;B4&amp;" = @"&amp;B4</f>
-        <v xml:space="preserve">    GameId = @GameId</v>
+        <v xml:space="preserve">    TId = @TId</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="5"/>
@@ -2066,7 +2088,7 @@
       </c>
       <c r="Z27" s="13" t="str">
         <f>"                    .AddWithValue(""@"&amp;C2&amp;"Id"", "&amp;LOWER(C2)&amp;"Id, DbType.Int32);"</f>
-        <v>                    .AddWithValue("@GamesId", gamesId, DbType.Int32);</v>
+        <v>                    .AddWithValue("@TsId", tsId, DbType.Int32);</v>
       </c>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.25">
@@ -2116,7 +2138,7 @@
       </c>
       <c r="L29" s="22" t="str">
         <f>"INSERT INTO "&amp;B2&amp;"."&amp;C2&amp;" ("</f>
-        <v>INSERT INTO dbo.Games (</v>
+        <v>INSERT INTO dbo.Ts (</v>
       </c>
       <c r="N29" s="23" t="str">
         <f t="shared" si="9"/>
@@ -2127,7 +2149,7 @@
       </c>
       <c r="T29" s="6" t="str">
         <f>"        public "&amp;C2&amp;"("</f>
-        <v>        public Games(</v>
+        <v>        public Ts(</v>
       </c>
       <c r="V29" s="16" t="str">
         <f t="shared" si="8"/>
@@ -2154,7 +2176,7 @@
       </c>
       <c r="L30" s="22" t="str">
         <f>IF(NOT(ISBLANK(B5)),"["&amp;B5&amp;"]"&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>[Name],</v>
+        <v/>
       </c>
       <c r="N30" s="23" t="str">
         <f t="shared" si="9"/>
@@ -2162,7 +2184,7 @@
       </c>
       <c r="T30" s="6" t="str">
         <f>IF(NOT(ISBLANK(B4)),"            int"&amp;" "&amp;LOWER(LEFT(B4,1))&amp;MID(B4,2,LEN(B4)-1)&amp;IF(LEN(T31)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            int gameId,</v>
+        <v xml:space="preserve">            int tId</v>
       </c>
       <c r="Z30" s="13" t="s">
         <v>72</v>
@@ -2185,7 +2207,7 @@
       </c>
       <c r="L31" s="22" t="str">
         <f t="shared" ref="L31:L45" si="10">IF(NOT(ISBLANK(B6)),"["&amp;B6&amp;"]"&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>[StartDate]</v>
+        <v/>
       </c>
       <c r="N31" s="23" t="str">
         <f t="shared" si="9"/>
@@ -2193,7 +2215,7 @@
       </c>
       <c r="T31" s="6" t="str">
         <f t="shared" ref="T31:T46" si="11">IF(NOT(ISBLANK(B5)),"            "&amp;S12&amp;" "&amp;LOWER(LEFT(B5,1))&amp;MID(B5,2,LEN(B5)-1)&amp;IF(LEN(T32)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">             name,</v>
+        <v/>
       </c>
       <c r="V31" s="16" t="s">
         <v>83</v>
@@ -2227,7 +2249,7 @@
       </c>
       <c r="T32" s="6" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">             startDate</v>
+        <v/>
       </c>
       <c r="V32" s="16" t="s">
         <v>53</v>
@@ -2258,7 +2280,7 @@
       </c>
       <c r="Z33" s="13" t="str">
         <f>"        public DataResult&lt;"&amp;C2&amp;"&gt; Save("&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;Games&gt; Save(Games value)</v>
+        <v xml:space="preserve">        public DataResult&lt;Ts&gt; Save(Ts value)</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
@@ -2276,7 +2298,7 @@
       </c>
       <c r="V34" s="16" t="str">
         <f>"        public static IEnumerable&lt;"&amp;C2&amp;"&gt; ParseMultipleReader(IDataReader reader)"</f>
-        <v>        public static IEnumerable&lt;Games&gt; ParseMultipleReader(IDataReader reader)</v>
+        <v>        public static IEnumerable&lt;Ts&gt; ParseMultipleReader(IDataReader reader)</v>
       </c>
       <c r="Z34" s="13" t="s">
         <v>96</v>
@@ -2317,7 +2339,7 @@
       </c>
       <c r="V36" s="16" t="str">
         <f>"            var "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;"s = new List&lt;"&amp;C2&amp;"&gt;();"</f>
-        <v>            var gamess = new List&lt;Games&gt;();</v>
+        <v>            var tss = new List&lt;Ts&gt;();</v>
       </c>
       <c r="Z36" s="13" t="s">
         <v>53</v>
@@ -2358,7 +2380,7 @@
       </c>
       <c r="Z38" s="13" t="str">
         <f>"        public DataResult&lt;"&amp;C2&amp;"&gt; Create("&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;Games&gt; Create(Games value)</v>
+        <v xml:space="preserve">        public DataResult&lt;Ts&gt; Create(Ts value)</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
@@ -2396,11 +2418,11 @@
       </c>
       <c r="V40" s="16" t="str">
         <f>"                "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;".Add(ParseReader(reader));"</f>
-        <v>                games.Add(ParseReader(reader));</v>
+        <v>                ts.Add(ParseReader(reader));</v>
       </c>
       <c r="Z40" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Create""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Games_Create"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Ts_Create"))</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
@@ -2410,7 +2432,7 @@
       </c>
       <c r="N41" s="23" t="str">
         <f>IF(NOT(ISBLANK(B4)),"WHERE ["&amp;B4&amp;"] = ISNULL(@"&amp;B4&amp;", 0)","")</f>
-        <v>WHERE [GameId] = ISNULL(@GameId, 0)</v>
+        <v>WHERE [TId] = ISNULL(@TId, 0)</v>
       </c>
       <c r="T41" s="6" t="str">
         <f t="shared" si="11"/>
@@ -2441,7 +2463,7 @@
       </c>
       <c r="Z42" s="13" t="str">
         <f>"                var idParameter = command.AddOutput(""@"&amp;C2&amp;"Id"", SqlDbType.Int);"</f>
-        <v>                var idParameter = command.AddOutput("@GamesId", SqlDbType.Int);</v>
+        <v>                var idParameter = command.AddOutput("@TsId", SqlDbType.Int);</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
@@ -2458,7 +2480,7 @@
       </c>
       <c r="V43" s="16" t="str">
         <f>"            return "&amp;LOWER(LEFT(C2,1))&amp;MID(C2,2,LEN(C2)-1)&amp;";"</f>
-        <v>            return games;</v>
+        <v>            return ts;</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
@@ -2498,7 +2520,7 @@
       </c>
       <c r="Z45" s="13" t="str">
         <f>IF(NOT(ISBLANK(B4)),"                    .AddWithValue(""@"&amp;B4&amp;""", value.Id,  DbType.Int32"&amp;")"&amp;IF(LEN(Z46)&gt;0,"",";"),"")</f>
-        <v>                    .AddWithValue("@GameId", value.Id,  DbType.Int32)</v>
+        <v>                    .AddWithValue("@TId", value.Id,  DbType.Int32);</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
@@ -2511,11 +2533,11 @@
       </c>
       <c r="V46" s="16" t="str">
         <f>"        private enum "&amp;C2&amp;"Col"</f>
-        <v>        private enum GamesCol</v>
+        <v>        private enum TsCol</v>
       </c>
       <c r="Z46" s="13" t="str">
         <f>IF(NOT(ISBLANK(B5)),"                    .AddWithValue(""@"&amp;B5&amp;""", value."&amp;B5&amp;", DbType."&amp;IF(NOT(OR(ISBLANK(Q12),Q12="int")),UPPER(LEFT(Q12,1))&amp;MID(Q12,2,LEN(Q12)-1),"Int32")&amp;")"&amp;IF(LEFT(Z47,24)="                    .Add","",";"),"")</f>
-        <v>                    .AddWithValue("@Name", value.Name, DbType.Varchar(50))</v>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
@@ -2530,13 +2552,13 @@
       </c>
       <c r="Z47" s="13" t="str">
         <f>IF(NOT(ISBLANK(B6)),"                    .AddWithValue(""@"&amp;B6&amp;""", value."&amp;B6&amp;", DbType."&amp;IF(NOT(OR(ISBLANK(Q13),Q13="int")),UPPER(LEFT(Q13,1))&amp;MID(Q13,2,LEN(Q13)-1),"Int32")&amp;")"&amp;IF(LEFT(Z48,24)="                    .Add","",";"),"")</f>
-        <v>                    .AddWithValue("@StartDate", value.StartDate, DbType.Datetime2(3));</v>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L48" s="22" t="str">
         <f>IF(NOT(ISBLANK(B5)),"@"&amp;B5&amp;IF(NOT(ISBLANK(B6)),",",""),"")</f>
-        <v>@Name,</v>
+        <v/>
       </c>
       <c r="T48" s="6" t="s">
         <v>52</v>
@@ -2552,15 +2574,15 @@
     <row r="49" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L49" s="22" t="str">
         <f t="shared" ref="L49:L63" si="13">IF(NOT(ISBLANK(B6)),"@"&amp;B6&amp;IF(NOT(ISBLANK(B7)),",",""),"")</f>
-        <v>@StartDate</v>
+        <v/>
       </c>
       <c r="T49" s="6" t="str">
         <f>IF(NOT(ISBLANK(B4)),"            Id = "&amp;LOWER(LEFT(B4,1))&amp;MID(B4,2,LEN(B4)-1)&amp;";","")</f>
-        <v xml:space="preserve">            Id = gameId;</v>
+        <v xml:space="preserve">            Id = tId;</v>
       </c>
       <c r="V49" s="16" t="str">
         <f t="shared" ref="V49:V64" si="14">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;IF(LEN(V15)&gt;0,",",""),"")</f>
-        <v xml:space="preserve">            Name</v>
+        <v/>
       </c>
       <c r="Z49" s="13" t="str">
         <f t="shared" si="12"/>
@@ -2574,11 +2596,11 @@
       </c>
       <c r="T50" s="6" t="str">
         <f t="shared" ref="T50:T65" si="15">IF(NOT(ISBLANK(B5)),"            "&amp;B5&amp;" = "&amp;LOWER(LEFT(B5,1))&amp;MID(B5,2,LEN(B5)-1)&amp;";","")</f>
-        <v xml:space="preserve">            Name = name;</v>
+        <v/>
       </c>
       <c r="V50" s="16" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">            StartDate</v>
+        <v/>
       </c>
       <c r="Z50" s="13" t="str">
         <f t="shared" si="12"/>
@@ -2592,7 +2614,7 @@
       </c>
       <c r="T51" s="6" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">            StartDate = startDate;</v>
+        <v/>
       </c>
       <c r="V51" s="16" t="str">
         <f t="shared" si="14"/>
@@ -2846,7 +2868,7 @@
     <row r="66" spans="12:26" x14ac:dyDescent="0.25">
       <c r="L66" s="22" t="str">
         <f>"SELECT @"&amp;B4&amp;" = SCOPE_IDENTITY()"</f>
-        <v>SELECT @GameId = SCOPE_IDENTITY()</v>
+        <v>SELECT @TId = SCOPE_IDENTITY()</v>
       </c>
       <c r="V66" s="16" t="s">
         <v>54</v>
@@ -2861,7 +2883,7 @@
       </c>
       <c r="Z67" s="13" t="str">
         <f>"                return new DataResult&lt;"&amp;C2&amp;"&gt;(value, result);"</f>
-        <v>                return new DataResult&lt;Games&gt;(value, result);</v>
+        <v>                return new DataResult&lt;Ts&gt;(value, result);</v>
       </c>
     </row>
     <row r="68" spans="12:26" x14ac:dyDescent="0.25">
@@ -2889,7 +2911,7 @@
     <row r="71" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z71" s="13" t="str">
         <f>"        public DataResult&lt;"&amp;C2&amp;"&gt; Update("&amp;C2&amp;" value)"</f>
-        <v xml:space="preserve">        public DataResult&lt;Games&gt; Update(Games value)</v>
+        <v xml:space="preserve">        public DataResult&lt;Ts&gt; Update(Ts value)</v>
       </c>
     </row>
     <row r="72" spans="12:26" x14ac:dyDescent="0.25">
@@ -2900,7 +2922,7 @@
     <row r="73" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z73" s="13" t="str">
         <f>"            using (var command = UnitOfWork.CreateStoredProcedure("""&amp;B2&amp;".USP_"&amp;C2&amp;"_Update""))"</f>
-        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Games_Update"))</v>
+        <v>            using (var command = UnitOfWork.CreateStoredProcedure("dbo.USP_Ts_Update"))</v>
       </c>
     </row>
     <row r="74" spans="12:26" x14ac:dyDescent="0.25">
@@ -2916,19 +2938,19 @@
     <row r="76" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z76" s="13" t="str">
         <f>IF(NOT(ISBLANK(B4)),"                    .AddWithValue(""@"&amp;B4&amp;""", value.Id,  DbType.Int32"&amp;")"&amp;IF(LEN(Z77)&gt;0,"",";"),"")</f>
-        <v>                    .AddWithValue("@GameId", value.Id,  DbType.Int32)</v>
+        <v>                    .AddWithValue("@TId", value.Id,  DbType.Int32);</v>
       </c>
     </row>
     <row r="77" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z77" s="13" t="str">
         <f>IF(NOT(ISBLANK(B5)),"                    .AddWithValue(""@"&amp;B5&amp;""", value."&amp;B5&amp;", DbType."&amp;IF(NOT(OR(ISBLANK(Q12),Q12="int")),UPPER(LEFT(Q12,1))&amp;MID(Q12,2,LEN(Q12)-1),"Int32")&amp;")"&amp;IF(LEFT(Z47,24)="                    .Add","",";"),"")</f>
-        <v>                    .AddWithValue("@Name", value.Name, DbType.Varchar(50))</v>
+        <v/>
       </c>
     </row>
     <row r="78" spans="12:26" x14ac:dyDescent="0.25">
       <c r="Z78" s="13" t="str">
         <f t="shared" ref="Z78:Z95" si="16">IF(NOT(ISBLANK(B6)),"                    .AddWithValue(""@"&amp;B6&amp;""", value."&amp;B6&amp;", DbType."&amp;IF(NOT(OR(ISBLANK(Q13),Q13="int")),UPPER(LEFT(Q13,1))&amp;MID(Q13,2,LEN(Q13)-1),"Int32")&amp;")"&amp;IF(LEFT(Z48,24)="                    .Add","",";"),"")</f>
-        <v>                    .AddWithValue("@StartDate", value.StartDate, DbType.Datetime2(3));</v>
+        <v/>
       </c>
     </row>
     <row r="79" spans="12:26" x14ac:dyDescent="0.25">
@@ -3041,7 +3063,7 @@
     <row r="98" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z98" s="13" t="str">
         <f>"                return new DataResult&lt;"&amp;C2&amp;"&gt;(value, result);"</f>
-        <v>                return new DataResult&lt;Games&gt;(value, result);</v>
+        <v>                return new DataResult&lt;Ts&gt;(value, result);</v>
       </c>
     </row>
     <row r="99" spans="26:26" x14ac:dyDescent="0.25">

</xml_diff>